<commit_message>
updated gantt chart and report
</commit_message>
<xml_diff>
--- a/docs/Gantt chart.xlsx
+++ b/docs/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/mini-project-A/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282D8A22-631F-8141-B633-44775790AD04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B1762B-EB26-F448-8D37-B8D6902E6210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="83">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -266,6 +266,9 @@
   </si>
   <si>
     <t>13/12/2020</t>
+  </si>
+  <si>
+    <t>16/12/2020</t>
   </si>
 </sst>
 </file>
@@ -1576,8 +1579,8 @@
   </sheetPr>
   <dimension ref="A1:BQ46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1908,8 +1911,8 @@
       <c r="M5" s="91"/>
       <c r="N5" s="91"/>
       <c r="O5" s="91"/>
-      <c r="P5" s="112">
-        <v>43171</v>
+      <c r="P5" s="112" t="s">
+        <v>82</v>
       </c>
       <c r="Q5" s="91"/>
       <c r="R5" s="91"/>

</xml_diff>

<commit_message>
updated gantt chart and report, added report pdf
</commit_message>
<xml_diff>
--- a/docs/Gantt chart.xlsx
+++ b/docs/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/mini-project-A/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93CED22-B673-F849-95DD-8F1E16E2D496}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B658DD-559C-B546-9E30-8A58D8239B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1277,6 +1277,41 @@
     <xf numFmtId="0" fontId="29" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1287,14 +1322,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1303,36 +1333,6 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,8 +1655,8 @@
   </sheetPr>
   <dimension ref="A1:BQ46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1744,38 +1744,38 @@
     </row>
     <row r="2" spans="1:69" ht="32" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="141" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="125"/>
-      <c r="D2" s="125"/>
-      <c r="E2" s="125"/>
-      <c r="F2" s="125"/>
-      <c r="G2" s="125"/>
+      <c r="C2" s="140"/>
+      <c r="D2" s="140"/>
+      <c r="E2" s="140"/>
+      <c r="F2" s="140"/>
+      <c r="G2" s="140"/>
       <c r="H2" s="94"/>
-      <c r="I2" s="124"/>
-      <c r="J2" s="125"/>
-      <c r="K2" s="125"/>
-      <c r="L2" s="125"/>
-      <c r="M2" s="125"/>
-      <c r="N2" s="125"/>
-      <c r="O2" s="127"/>
-      <c r="P2" s="125"/>
-      <c r="Q2" s="125"/>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="125"/>
-      <c r="W2" s="125"/>
-      <c r="X2" s="125"/>
-      <c r="Y2" s="125"/>
-      <c r="Z2" s="125"/>
-      <c r="AA2" s="125"/>
-      <c r="AB2" s="125"/>
-      <c r="AC2" s="125"/>
-      <c r="AD2" s="125"/>
-      <c r="AE2" s="125"/>
+      <c r="I2" s="139"/>
+      <c r="J2" s="140"/>
+      <c r="K2" s="140"/>
+      <c r="L2" s="140"/>
+      <c r="M2" s="140"/>
+      <c r="N2" s="140"/>
+      <c r="O2" s="142"/>
+      <c r="P2" s="140"/>
+      <c r="Q2" s="140"/>
+      <c r="R2" s="140"/>
+      <c r="S2" s="140"/>
+      <c r="T2" s="140"/>
+      <c r="U2" s="140"/>
+      <c r="V2" s="140"/>
+      <c r="W2" s="140"/>
+      <c r="X2" s="140"/>
+      <c r="Y2" s="140"/>
+      <c r="Z2" s="140"/>
+      <c r="AA2" s="140"/>
+      <c r="AB2" s="140"/>
+      <c r="AC2" s="140"/>
+      <c r="AD2" s="140"/>
+      <c r="AE2" s="140"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1888,41 +1888,41 @@
     </row>
     <row r="4" spans="1:69" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="128" t="s">
+      <c r="B4" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="129"/>
-      <c r="D4" s="132" t="s">
+      <c r="C4" s="125"/>
+      <c r="D4" s="144" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="129"/>
-      <c r="F4" s="129"/>
-      <c r="G4" s="129"/>
+      <c r="E4" s="125"/>
+      <c r="F4" s="125"/>
+      <c r="G4" s="125"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="128" t="s">
+      <c r="I4" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="129"/>
-      <c r="K4" s="129"/>
-      <c r="L4" s="129"/>
-      <c r="M4" s="129"/>
-      <c r="N4" s="129"/>
-      <c r="O4" s="129"/>
-      <c r="P4" s="133" t="s">
+      <c r="J4" s="125"/>
+      <c r="K4" s="125"/>
+      <c r="L4" s="125"/>
+      <c r="M4" s="125"/>
+      <c r="N4" s="125"/>
+      <c r="O4" s="125"/>
+      <c r="P4" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="129"/>
-      <c r="R4" s="129"/>
-      <c r="S4" s="129"/>
-      <c r="T4" s="129"/>
-      <c r="U4" s="129"/>
-      <c r="V4" s="129"/>
-      <c r="W4" s="129"/>
-      <c r="X4" s="129"/>
-      <c r="Y4" s="129"/>
-      <c r="Z4" s="129"/>
-      <c r="AA4" s="129"/>
-      <c r="AB4" s="129"/>
+      <c r="Q4" s="125"/>
+      <c r="R4" s="125"/>
+      <c r="S4" s="125"/>
+      <c r="T4" s="125"/>
+      <c r="U4" s="125"/>
+      <c r="V4" s="125"/>
+      <c r="W4" s="125"/>
+      <c r="X4" s="125"/>
+      <c r="Y4" s="125"/>
+      <c r="Z4" s="125"/>
+      <c r="AA4" s="125"/>
+      <c r="AB4" s="125"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
@@ -1967,40 +1967,40 @@
     </row>
     <row r="5" spans="1:69" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="128" t="s">
+      <c r="B5" s="124" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="129"/>
-      <c r="D5" s="145" t="s">
+      <c r="C5" s="125"/>
+      <c r="D5" s="126" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="129"/>
-      <c r="F5" s="129"/>
-      <c r="G5" s="129"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
+      <c r="G5" s="125"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="128" t="s">
+      <c r="I5" s="124" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="129"/>
-      <c r="K5" s="129"/>
-      <c r="L5" s="129"/>
-      <c r="M5" s="129"/>
-      <c r="N5" s="129"/>
-      <c r="O5" s="129"/>
-      <c r="P5" s="134" t="s">
+      <c r="J5" s="125"/>
+      <c r="K5" s="125"/>
+      <c r="L5" s="125"/>
+      <c r="M5" s="125"/>
+      <c r="N5" s="125"/>
+      <c r="O5" s="125"/>
+      <c r="P5" s="146" t="s">
         <v>79</v>
       </c>
-      <c r="Q5" s="129"/>
-      <c r="R5" s="129"/>
-      <c r="S5" s="129"/>
-      <c r="T5" s="129"/>
-      <c r="U5" s="129"/>
-      <c r="V5" s="129"/>
-      <c r="W5" s="129"/>
-      <c r="X5" s="129"/>
-      <c r="Y5" s="129"/>
-      <c r="Z5" s="129"/>
-      <c r="AA5" s="129"/>
+      <c r="Q5" s="125"/>
+      <c r="R5" s="125"/>
+      <c r="S5" s="125"/>
+      <c r="T5" s="125"/>
+      <c r="U5" s="125"/>
+      <c r="V5" s="125"/>
+      <c r="W5" s="125"/>
+      <c r="X5" s="125"/>
+      <c r="Y5" s="125"/>
+      <c r="Z5" s="125"/>
+      <c r="AA5" s="125"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -2188,201 +2188,201 @@
     </row>
     <row r="8" spans="1:69" ht="17.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="130" t="s">
+      <c r="B8" s="143" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="130" t="s">
+      <c r="C8" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="130" t="s">
+      <c r="D8" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="130" t="s">
+      <c r="E8" s="143" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="130" t="s">
+      <c r="F8" s="143" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="130" t="s">
+      <c r="G8" s="143" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="130" t="s">
+      <c r="H8" s="143" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="139" t="s">
+      <c r="I8" s="132" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="131"/>
-      <c r="K8" s="131"/>
-      <c r="L8" s="131"/>
-      <c r="M8" s="131"/>
-      <c r="N8" s="131"/>
-      <c r="O8" s="131"/>
-      <c r="P8" s="131"/>
-      <c r="Q8" s="131"/>
-      <c r="R8" s="131"/>
-      <c r="S8" s="131"/>
-      <c r="T8" s="131"/>
-      <c r="U8" s="131"/>
-      <c r="V8" s="131"/>
-      <c r="W8" s="131"/>
-      <c r="X8" s="140" t="s">
+      <c r="J8" s="133"/>
+      <c r="K8" s="133"/>
+      <c r="L8" s="133"/>
+      <c r="M8" s="133"/>
+      <c r="N8" s="133"/>
+      <c r="O8" s="133"/>
+      <c r="P8" s="133"/>
+      <c r="Q8" s="133"/>
+      <c r="R8" s="133"/>
+      <c r="S8" s="133"/>
+      <c r="T8" s="133"/>
+      <c r="U8" s="133"/>
+      <c r="V8" s="133"/>
+      <c r="W8" s="133"/>
+      <c r="X8" s="134" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="131"/>
-      <c r="Z8" s="131"/>
-      <c r="AA8" s="131"/>
-      <c r="AB8" s="131"/>
-      <c r="AC8" s="131"/>
-      <c r="AD8" s="131"/>
-      <c r="AE8" s="131"/>
-      <c r="AF8" s="131"/>
-      <c r="AG8" s="131"/>
-      <c r="AH8" s="131"/>
-      <c r="AI8" s="131"/>
-      <c r="AJ8" s="131"/>
-      <c r="AK8" s="131"/>
-      <c r="AL8" s="131"/>
-      <c r="AM8" s="143" t="s">
+      <c r="Y8" s="133"/>
+      <c r="Z8" s="133"/>
+      <c r="AA8" s="133"/>
+      <c r="AB8" s="133"/>
+      <c r="AC8" s="133"/>
+      <c r="AD8" s="133"/>
+      <c r="AE8" s="133"/>
+      <c r="AF8" s="133"/>
+      <c r="AG8" s="133"/>
+      <c r="AH8" s="133"/>
+      <c r="AI8" s="133"/>
+      <c r="AJ8" s="133"/>
+      <c r="AK8" s="133"/>
+      <c r="AL8" s="133"/>
+      <c r="AM8" s="137" t="s">
         <v>14</v>
       </c>
-      <c r="AN8" s="131"/>
-      <c r="AO8" s="131"/>
-      <c r="AP8" s="131"/>
-      <c r="AQ8" s="131"/>
-      <c r="AR8" s="131"/>
-      <c r="AS8" s="131"/>
-      <c r="AT8" s="131"/>
-      <c r="AU8" s="131"/>
-      <c r="AV8" s="131"/>
-      <c r="AW8" s="131"/>
-      <c r="AX8" s="131"/>
-      <c r="AY8" s="131"/>
-      <c r="AZ8" s="131"/>
-      <c r="BA8" s="131"/>
-      <c r="BB8" s="141" t="s">
+      <c r="AN8" s="133"/>
+      <c r="AO8" s="133"/>
+      <c r="AP8" s="133"/>
+      <c r="AQ8" s="133"/>
+      <c r="AR8" s="133"/>
+      <c r="AS8" s="133"/>
+      <c r="AT8" s="133"/>
+      <c r="AU8" s="133"/>
+      <c r="AV8" s="133"/>
+      <c r="AW8" s="133"/>
+      <c r="AX8" s="133"/>
+      <c r="AY8" s="133"/>
+      <c r="AZ8" s="133"/>
+      <c r="BA8" s="133"/>
+      <c r="BB8" s="135" t="s">
         <v>15</v>
       </c>
-      <c r="BC8" s="131"/>
-      <c r="BD8" s="131"/>
-      <c r="BE8" s="131"/>
-      <c r="BF8" s="131"/>
-      <c r="BG8" s="131"/>
-      <c r="BH8" s="131"/>
-      <c r="BI8" s="131"/>
-      <c r="BJ8" s="131"/>
-      <c r="BK8" s="131"/>
-      <c r="BL8" s="131"/>
-      <c r="BM8" s="131"/>
-      <c r="BN8" s="131"/>
-      <c r="BO8" s="131"/>
-      <c r="BP8" s="142"/>
+      <c r="BC8" s="133"/>
+      <c r="BD8" s="133"/>
+      <c r="BE8" s="133"/>
+      <c r="BF8" s="133"/>
+      <c r="BG8" s="133"/>
+      <c r="BH8" s="133"/>
+      <c r="BI8" s="133"/>
+      <c r="BJ8" s="133"/>
+      <c r="BK8" s="133"/>
+      <c r="BL8" s="133"/>
+      <c r="BM8" s="133"/>
+      <c r="BN8" s="133"/>
+      <c r="BO8" s="133"/>
+      <c r="BP8" s="136"/>
       <c r="BQ8" s="21"/>
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="A9" s="25"/>
-      <c r="B9" s="131"/>
-      <c r="C9" s="131"/>
-      <c r="D9" s="131"/>
-      <c r="E9" s="131"/>
-      <c r="F9" s="131"/>
-      <c r="G9" s="131"/>
-      <c r="H9" s="131"/>
-      <c r="I9" s="146" t="s">
+      <c r="B9" s="133"/>
+      <c r="C9" s="133"/>
+      <c r="D9" s="133"/>
+      <c r="E9" s="133"/>
+      <c r="F9" s="133"/>
+      <c r="G9" s="133"/>
+      <c r="H9" s="133"/>
+      <c r="I9" s="127" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="136"/>
-      <c r="K9" s="136"/>
-      <c r="L9" s="136"/>
-      <c r="M9" s="137"/>
-      <c r="N9" s="146" t="s">
+      <c r="J9" s="128"/>
+      <c r="K9" s="128"/>
+      <c r="L9" s="128"/>
+      <c r="M9" s="129"/>
+      <c r="N9" s="127" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="136"/>
-      <c r="P9" s="136"/>
-      <c r="Q9" s="136"/>
-      <c r="R9" s="137"/>
-      <c r="S9" s="146" t="s">
+      <c r="O9" s="128"/>
+      <c r="P9" s="128"/>
+      <c r="Q9" s="128"/>
+      <c r="R9" s="129"/>
+      <c r="S9" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="T9" s="136"/>
-      <c r="U9" s="136"/>
-      <c r="V9" s="136"/>
-      <c r="W9" s="137"/>
-      <c r="X9" s="138" t="s">
+      <c r="T9" s="128"/>
+      <c r="U9" s="128"/>
+      <c r="V9" s="128"/>
+      <c r="W9" s="129"/>
+      <c r="X9" s="131" t="s">
         <v>19</v>
       </c>
-      <c r="Y9" s="136"/>
-      <c r="Z9" s="136"/>
-      <c r="AA9" s="136"/>
-      <c r="AB9" s="137"/>
-      <c r="AC9" s="138" t="s">
+      <c r="Y9" s="128"/>
+      <c r="Z9" s="128"/>
+      <c r="AA9" s="128"/>
+      <c r="AB9" s="129"/>
+      <c r="AC9" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="AD9" s="136"/>
-      <c r="AE9" s="136"/>
-      <c r="AF9" s="136"/>
-      <c r="AG9" s="137"/>
-      <c r="AH9" s="138" t="s">
+      <c r="AD9" s="128"/>
+      <c r="AE9" s="128"/>
+      <c r="AF9" s="128"/>
+      <c r="AG9" s="129"/>
+      <c r="AH9" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="AI9" s="136"/>
-      <c r="AJ9" s="136"/>
-      <c r="AK9" s="136"/>
-      <c r="AL9" s="137"/>
-      <c r="AM9" s="144" t="s">
+      <c r="AI9" s="128"/>
+      <c r="AJ9" s="128"/>
+      <c r="AK9" s="128"/>
+      <c r="AL9" s="129"/>
+      <c r="AM9" s="138" t="s">
         <v>22</v>
       </c>
-      <c r="AN9" s="136"/>
-      <c r="AO9" s="136"/>
-      <c r="AP9" s="136"/>
-      <c r="AQ9" s="137"/>
-      <c r="AR9" s="144" t="s">
+      <c r="AN9" s="128"/>
+      <c r="AO9" s="128"/>
+      <c r="AP9" s="128"/>
+      <c r="AQ9" s="129"/>
+      <c r="AR9" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="AS9" s="136"/>
-      <c r="AT9" s="136"/>
-      <c r="AU9" s="136"/>
-      <c r="AV9" s="137"/>
-      <c r="AW9" s="144" t="s">
+      <c r="AS9" s="128"/>
+      <c r="AT9" s="128"/>
+      <c r="AU9" s="128"/>
+      <c r="AV9" s="129"/>
+      <c r="AW9" s="138" t="s">
         <v>24</v>
       </c>
-      <c r="AX9" s="136"/>
-      <c r="AY9" s="136"/>
-      <c r="AZ9" s="136"/>
-      <c r="BA9" s="137"/>
-      <c r="BB9" s="135" t="s">
+      <c r="AX9" s="128"/>
+      <c r="AY9" s="128"/>
+      <c r="AZ9" s="128"/>
+      <c r="BA9" s="129"/>
+      <c r="BB9" s="130" t="s">
         <v>25</v>
       </c>
-      <c r="BC9" s="136"/>
-      <c r="BD9" s="136"/>
-      <c r="BE9" s="136"/>
-      <c r="BF9" s="137"/>
-      <c r="BG9" s="135" t="s">
+      <c r="BC9" s="128"/>
+      <c r="BD9" s="128"/>
+      <c r="BE9" s="128"/>
+      <c r="BF9" s="129"/>
+      <c r="BG9" s="130" t="s">
         <v>26</v>
       </c>
-      <c r="BH9" s="136"/>
-      <c r="BI9" s="136"/>
-      <c r="BJ9" s="136"/>
-      <c r="BK9" s="137"/>
-      <c r="BL9" s="135" t="s">
+      <c r="BH9" s="128"/>
+      <c r="BI9" s="128"/>
+      <c r="BJ9" s="128"/>
+      <c r="BK9" s="129"/>
+      <c r="BL9" s="130" t="s">
         <v>27</v>
       </c>
-      <c r="BM9" s="136"/>
-      <c r="BN9" s="136"/>
-      <c r="BO9" s="136"/>
-      <c r="BP9" s="137"/>
+      <c r="BM9" s="128"/>
+      <c r="BN9" s="128"/>
+      <c r="BO9" s="128"/>
+      <c r="BP9" s="129"/>
       <c r="BQ9" s="25"/>
     </row>
     <row r="10" spans="1:69" ht="17.25" customHeight="1">
       <c r="A10" s="26"/>
-      <c r="B10" s="131"/>
-      <c r="C10" s="131"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="131"/>
-      <c r="F10" s="131"/>
-      <c r="G10" s="131"/>
-      <c r="H10" s="131"/>
+      <c r="B10" s="133"/>
+      <c r="C10" s="133"/>
+      <c r="D10" s="133"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
       <c r="I10" s="27" t="s">
         <v>28</v>
       </c>
@@ -4383,7 +4383,7 @@
       </c>
       <c r="G33" s="65"/>
       <c r="H33" s="80">
-        <v>0.4</v>
+        <v>0.45</v>
       </c>
       <c r="I33" s="73"/>
       <c r="J33" s="74"/>
@@ -5420,24 +5420,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="BB8:BP8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="AM9:AQ9"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="O2:AE2"/>
@@ -5454,6 +5436,24 @@
     <mergeCell ref="P4:AB4"/>
     <mergeCell ref="P5:AA5"/>
     <mergeCell ref="I5:O5"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="BB8:BP8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="I9:M9"/>
   </mergeCells>
   <conditionalFormatting sqref="H12:H23 H30:H44 H25:H28">
     <cfRule type="colorScale" priority="3">

</xml_diff>

<commit_message>
updated logbook and report
</commit_message>
<xml_diff>
--- a/docs/Gantt chart.xlsx
+++ b/docs/Gantt chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/mini-project-A/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/connecture/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B658DD-559C-B546-9E30-8A58D8239B5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35166B3-9CEB-C545-9587-0A4F8D450FB0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantchart" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="81">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -916,7 +916,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1277,41 +1277,6 @@
     <xf numFmtId="0" fontId="29" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1322,9 +1287,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1333,6 +1303,39 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1655,8 +1658,8 @@
   </sheetPr>
   <dimension ref="A1:BQ46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A66" zoomScale="75" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -1744,38 +1747,38 @@
     </row>
     <row r="2" spans="1:69" ht="32" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="141" t="s">
+      <c r="B2" s="126" t="s">
         <v>75</v>
       </c>
-      <c r="C2" s="140"/>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
+      <c r="C2" s="125"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
       <c r="H2" s="94"/>
-      <c r="I2" s="139"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="140"/>
-      <c r="O2" s="142"/>
-      <c r="P2" s="140"/>
-      <c r="Q2" s="140"/>
-      <c r="R2" s="140"/>
-      <c r="S2" s="140"/>
-      <c r="T2" s="140"/>
-      <c r="U2" s="140"/>
-      <c r="V2" s="140"/>
-      <c r="W2" s="140"/>
-      <c r="X2" s="140"/>
-      <c r="Y2" s="140"/>
-      <c r="Z2" s="140"/>
-      <c r="AA2" s="140"/>
-      <c r="AB2" s="140"/>
-      <c r="AC2" s="140"/>
-      <c r="AD2" s="140"/>
-      <c r="AE2" s="140"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="125"/>
+      <c r="K2" s="125"/>
+      <c r="L2" s="125"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="125"/>
+      <c r="O2" s="127"/>
+      <c r="P2" s="125"/>
+      <c r="Q2" s="125"/>
+      <c r="R2" s="125"/>
+      <c r="S2" s="125"/>
+      <c r="T2" s="125"/>
+      <c r="U2" s="125"/>
+      <c r="V2" s="125"/>
+      <c r="W2" s="125"/>
+      <c r="X2" s="125"/>
+      <c r="Y2" s="125"/>
+      <c r="Z2" s="125"/>
+      <c r="AA2" s="125"/>
+      <c r="AB2" s="125"/>
+      <c r="AC2" s="125"/>
+      <c r="AD2" s="125"/>
+      <c r="AE2" s="125"/>
       <c r="AF2" s="11"/>
       <c r="AG2" s="11"/>
       <c r="AH2" s="11"/>
@@ -1888,41 +1891,41 @@
     </row>
     <row r="4" spans="1:69" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="124" t="s">
+      <c r="B4" s="128" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="125"/>
-      <c r="D4" s="144" t="s">
+      <c r="C4" s="129"/>
+      <c r="D4" s="132" t="s">
         <v>68</v>
       </c>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
-      <c r="G4" s="125"/>
+      <c r="E4" s="129"/>
+      <c r="F4" s="129"/>
+      <c r="G4" s="129"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="124" t="s">
+      <c r="I4" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="125"/>
-      <c r="K4" s="125"/>
-      <c r="L4" s="125"/>
-      <c r="M4" s="125"/>
-      <c r="N4" s="125"/>
-      <c r="O4" s="125"/>
-      <c r="P4" s="145" t="s">
+      <c r="J4" s="129"/>
+      <c r="K4" s="129"/>
+      <c r="L4" s="129"/>
+      <c r="M4" s="129"/>
+      <c r="N4" s="129"/>
+      <c r="O4" s="129"/>
+      <c r="P4" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="Q4" s="125"/>
-      <c r="R4" s="125"/>
-      <c r="S4" s="125"/>
-      <c r="T4" s="125"/>
-      <c r="U4" s="125"/>
-      <c r="V4" s="125"/>
-      <c r="W4" s="125"/>
-      <c r="X4" s="125"/>
-      <c r="Y4" s="125"/>
-      <c r="Z4" s="125"/>
-      <c r="AA4" s="125"/>
-      <c r="AB4" s="125"/>
+      <c r="Q4" s="129"/>
+      <c r="R4" s="129"/>
+      <c r="S4" s="129"/>
+      <c r="T4" s="129"/>
+      <c r="U4" s="129"/>
+      <c r="V4" s="129"/>
+      <c r="W4" s="129"/>
+      <c r="X4" s="129"/>
+      <c r="Y4" s="129"/>
+      <c r="Z4" s="129"/>
+      <c r="AA4" s="129"/>
+      <c r="AB4" s="129"/>
       <c r="AC4" s="17"/>
       <c r="AD4" s="10"/>
       <c r="AE4" s="10"/>
@@ -1967,40 +1970,40 @@
     </row>
     <row r="5" spans="1:69" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="124" t="s">
+      <c r="B5" s="128" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="125"/>
-      <c r="D5" s="126" t="s">
+      <c r="C5" s="129"/>
+      <c r="D5" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="E5" s="125"/>
-      <c r="F5" s="125"/>
-      <c r="G5" s="125"/>
+      <c r="E5" s="129"/>
+      <c r="F5" s="129"/>
+      <c r="G5" s="129"/>
       <c r="H5" s="18"/>
-      <c r="I5" s="124" t="s">
+      <c r="I5" s="128" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="125"/>
-      <c r="K5" s="125"/>
-      <c r="L5" s="125"/>
-      <c r="M5" s="125"/>
-      <c r="N5" s="125"/>
-      <c r="O5" s="125"/>
-      <c r="P5" s="146" t="s">
+      <c r="J5" s="129"/>
+      <c r="K5" s="129"/>
+      <c r="L5" s="129"/>
+      <c r="M5" s="129"/>
+      <c r="N5" s="129"/>
+      <c r="O5" s="129"/>
+      <c r="P5" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="Q5" s="125"/>
-      <c r="R5" s="125"/>
-      <c r="S5" s="125"/>
-      <c r="T5" s="125"/>
-      <c r="U5" s="125"/>
-      <c r="V5" s="125"/>
-      <c r="W5" s="125"/>
-      <c r="X5" s="125"/>
-      <c r="Y5" s="125"/>
-      <c r="Z5" s="125"/>
-      <c r="AA5" s="125"/>
+      <c r="Q5" s="129"/>
+      <c r="R5" s="129"/>
+      <c r="S5" s="129"/>
+      <c r="T5" s="129"/>
+      <c r="U5" s="129"/>
+      <c r="V5" s="129"/>
+      <c r="W5" s="129"/>
+      <c r="X5" s="129"/>
+      <c r="Y5" s="129"/>
+      <c r="Z5" s="129"/>
+      <c r="AA5" s="129"/>
       <c r="AB5" s="19"/>
       <c r="AC5" s="17"/>
       <c r="AD5" s="1"/>
@@ -2188,201 +2191,201 @@
     </row>
     <row r="8" spans="1:69" ht="17.25" customHeight="1">
       <c r="A8" s="24"/>
-      <c r="B8" s="143" t="s">
+      <c r="B8" s="130" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="143" t="s">
+      <c r="C8" s="130" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="143" t="s">
+      <c r="D8" s="130" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="143" t="s">
+      <c r="E8" s="130" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="143" t="s">
+      <c r="F8" s="130" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="143" t="s">
+      <c r="G8" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="143" t="s">
+      <c r="H8" s="130" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="132" t="s">
+      <c r="I8" s="139" t="s">
         <v>12</v>
       </c>
-      <c r="J8" s="133"/>
-      <c r="K8" s="133"/>
-      <c r="L8" s="133"/>
-      <c r="M8" s="133"/>
-      <c r="N8" s="133"/>
-      <c r="O8" s="133"/>
-      <c r="P8" s="133"/>
-      <c r="Q8" s="133"/>
-      <c r="R8" s="133"/>
-      <c r="S8" s="133"/>
-      <c r="T8" s="133"/>
-      <c r="U8" s="133"/>
-      <c r="V8" s="133"/>
-      <c r="W8" s="133"/>
-      <c r="X8" s="134" t="s">
+      <c r="J8" s="131"/>
+      <c r="K8" s="131"/>
+      <c r="L8" s="131"/>
+      <c r="M8" s="131"/>
+      <c r="N8" s="131"/>
+      <c r="O8" s="131"/>
+      <c r="P8" s="131"/>
+      <c r="Q8" s="131"/>
+      <c r="R8" s="131"/>
+      <c r="S8" s="131"/>
+      <c r="T8" s="131"/>
+      <c r="U8" s="131"/>
+      <c r="V8" s="131"/>
+      <c r="W8" s="131"/>
+      <c r="X8" s="140" t="s">
         <v>13</v>
       </c>
-      <c r="Y8" s="133"/>
-      <c r="Z8" s="133"/>
-      <c r="AA8" s="133"/>
-      <c r="AB8" s="133"/>
-      <c r="AC8" s="133"/>
-      <c r="AD8" s="133"/>
-      <c r="AE8" s="133"/>
-      <c r="AF8" s="133"/>
-      <c r="AG8" s="133"/>
-      <c r="AH8" s="133"/>
-      <c r="AI8" s="133"/>
-      <c r="AJ8" s="133"/>
-      <c r="AK8" s="133"/>
-      <c r="AL8" s="133"/>
-      <c r="AM8" s="137" t="s">
+      <c r="Y8" s="131"/>
+      <c r="Z8" s="131"/>
+      <c r="AA8" s="131"/>
+      <c r="AB8" s="131"/>
+      <c r="AC8" s="131"/>
+      <c r="AD8" s="131"/>
+      <c r="AE8" s="131"/>
+      <c r="AF8" s="131"/>
+      <c r="AG8" s="131"/>
+      <c r="AH8" s="131"/>
+      <c r="AI8" s="131"/>
+      <c r="AJ8" s="131"/>
+      <c r="AK8" s="131"/>
+      <c r="AL8" s="131"/>
+      <c r="AM8" s="143" t="s">
         <v>14</v>
       </c>
-      <c r="AN8" s="133"/>
-      <c r="AO8" s="133"/>
-      <c r="AP8" s="133"/>
-      <c r="AQ8" s="133"/>
-      <c r="AR8" s="133"/>
-      <c r="AS8" s="133"/>
-      <c r="AT8" s="133"/>
-      <c r="AU8" s="133"/>
-      <c r="AV8" s="133"/>
-      <c r="AW8" s="133"/>
-      <c r="AX8" s="133"/>
-      <c r="AY8" s="133"/>
-      <c r="AZ8" s="133"/>
-      <c r="BA8" s="133"/>
-      <c r="BB8" s="135" t="s">
+      <c r="AN8" s="131"/>
+      <c r="AO8" s="131"/>
+      <c r="AP8" s="131"/>
+      <c r="AQ8" s="131"/>
+      <c r="AR8" s="131"/>
+      <c r="AS8" s="131"/>
+      <c r="AT8" s="131"/>
+      <c r="AU8" s="131"/>
+      <c r="AV8" s="131"/>
+      <c r="AW8" s="131"/>
+      <c r="AX8" s="131"/>
+      <c r="AY8" s="131"/>
+      <c r="AZ8" s="131"/>
+      <c r="BA8" s="131"/>
+      <c r="BB8" s="141" t="s">
         <v>15</v>
       </c>
-      <c r="BC8" s="133"/>
-      <c r="BD8" s="133"/>
-      <c r="BE8" s="133"/>
-      <c r="BF8" s="133"/>
-      <c r="BG8" s="133"/>
-      <c r="BH8" s="133"/>
-      <c r="BI8" s="133"/>
-      <c r="BJ8" s="133"/>
-      <c r="BK8" s="133"/>
-      <c r="BL8" s="133"/>
-      <c r="BM8" s="133"/>
-      <c r="BN8" s="133"/>
-      <c r="BO8" s="133"/>
-      <c r="BP8" s="136"/>
+      <c r="BC8" s="131"/>
+      <c r="BD8" s="131"/>
+      <c r="BE8" s="131"/>
+      <c r="BF8" s="131"/>
+      <c r="BG8" s="131"/>
+      <c r="BH8" s="131"/>
+      <c r="BI8" s="131"/>
+      <c r="BJ8" s="131"/>
+      <c r="BK8" s="131"/>
+      <c r="BL8" s="131"/>
+      <c r="BM8" s="131"/>
+      <c r="BN8" s="131"/>
+      <c r="BO8" s="131"/>
+      <c r="BP8" s="142"/>
       <c r="BQ8" s="21"/>
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="A9" s="25"/>
-      <c r="B9" s="133"/>
-      <c r="C9" s="133"/>
-      <c r="D9" s="133"/>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="133"/>
-      <c r="I9" s="127" t="s">
+      <c r="B9" s="131"/>
+      <c r="C9" s="131"/>
+      <c r="D9" s="131"/>
+      <c r="E9" s="131"/>
+      <c r="F9" s="131"/>
+      <c r="G9" s="131"/>
+      <c r="H9" s="131"/>
+      <c r="I9" s="146" t="s">
         <v>16</v>
       </c>
-      <c r="J9" s="128"/>
-      <c r="K9" s="128"/>
-      <c r="L9" s="128"/>
-      <c r="M9" s="129"/>
-      <c r="N9" s="127" t="s">
+      <c r="J9" s="136"/>
+      <c r="K9" s="136"/>
+      <c r="L9" s="136"/>
+      <c r="M9" s="137"/>
+      <c r="N9" s="146" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="128"/>
-      <c r="P9" s="128"/>
-      <c r="Q9" s="128"/>
-      <c r="R9" s="129"/>
-      <c r="S9" s="127" t="s">
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
+      <c r="Q9" s="136"/>
+      <c r="R9" s="137"/>
+      <c r="S9" s="146" t="s">
         <v>18</v>
       </c>
-      <c r="T9" s="128"/>
-      <c r="U9" s="128"/>
-      <c r="V9" s="128"/>
-      <c r="W9" s="129"/>
-      <c r="X9" s="131" t="s">
+      <c r="T9" s="136"/>
+      <c r="U9" s="136"/>
+      <c r="V9" s="136"/>
+      <c r="W9" s="137"/>
+      <c r="X9" s="138" t="s">
         <v>19</v>
       </c>
-      <c r="Y9" s="128"/>
-      <c r="Z9" s="128"/>
-      <c r="AA9" s="128"/>
-      <c r="AB9" s="129"/>
-      <c r="AC9" s="131" t="s">
+      <c r="Y9" s="136"/>
+      <c r="Z9" s="136"/>
+      <c r="AA9" s="136"/>
+      <c r="AB9" s="137"/>
+      <c r="AC9" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="AD9" s="128"/>
-      <c r="AE9" s="128"/>
-      <c r="AF9" s="128"/>
-      <c r="AG9" s="129"/>
-      <c r="AH9" s="131" t="s">
+      <c r="AD9" s="136"/>
+      <c r="AE9" s="136"/>
+      <c r="AF9" s="136"/>
+      <c r="AG9" s="137"/>
+      <c r="AH9" s="138" t="s">
         <v>21</v>
       </c>
-      <c r="AI9" s="128"/>
-      <c r="AJ9" s="128"/>
-      <c r="AK9" s="128"/>
-      <c r="AL9" s="129"/>
-      <c r="AM9" s="138" t="s">
+      <c r="AI9" s="136"/>
+      <c r="AJ9" s="136"/>
+      <c r="AK9" s="136"/>
+      <c r="AL9" s="137"/>
+      <c r="AM9" s="144" t="s">
         <v>22</v>
       </c>
-      <c r="AN9" s="128"/>
-      <c r="AO9" s="128"/>
-      <c r="AP9" s="128"/>
-      <c r="AQ9" s="129"/>
-      <c r="AR9" s="138" t="s">
+      <c r="AN9" s="136"/>
+      <c r="AO9" s="136"/>
+      <c r="AP9" s="136"/>
+      <c r="AQ9" s="137"/>
+      <c r="AR9" s="144" t="s">
         <v>23</v>
       </c>
-      <c r="AS9" s="128"/>
-      <c r="AT9" s="128"/>
-      <c r="AU9" s="128"/>
-      <c r="AV9" s="129"/>
-      <c r="AW9" s="138" t="s">
+      <c r="AS9" s="136"/>
+      <c r="AT9" s="136"/>
+      <c r="AU9" s="136"/>
+      <c r="AV9" s="137"/>
+      <c r="AW9" s="144" t="s">
         <v>24</v>
       </c>
-      <c r="AX9" s="128"/>
-      <c r="AY9" s="128"/>
-      <c r="AZ9" s="128"/>
-      <c r="BA9" s="129"/>
-      <c r="BB9" s="130" t="s">
+      <c r="AX9" s="136"/>
+      <c r="AY9" s="136"/>
+      <c r="AZ9" s="136"/>
+      <c r="BA9" s="137"/>
+      <c r="BB9" s="135" t="s">
         <v>25</v>
       </c>
-      <c r="BC9" s="128"/>
-      <c r="BD9" s="128"/>
-      <c r="BE9" s="128"/>
-      <c r="BF9" s="129"/>
-      <c r="BG9" s="130" t="s">
+      <c r="BC9" s="136"/>
+      <c r="BD9" s="136"/>
+      <c r="BE9" s="136"/>
+      <c r="BF9" s="137"/>
+      <c r="BG9" s="135" t="s">
         <v>26</v>
       </c>
-      <c r="BH9" s="128"/>
-      <c r="BI9" s="128"/>
-      <c r="BJ9" s="128"/>
-      <c r="BK9" s="129"/>
-      <c r="BL9" s="130" t="s">
+      <c r="BH9" s="136"/>
+      <c r="BI9" s="136"/>
+      <c r="BJ9" s="136"/>
+      <c r="BK9" s="137"/>
+      <c r="BL9" s="135" t="s">
         <v>27</v>
       </c>
-      <c r="BM9" s="128"/>
-      <c r="BN9" s="128"/>
-      <c r="BO9" s="128"/>
-      <c r="BP9" s="129"/>
+      <c r="BM9" s="136"/>
+      <c r="BN9" s="136"/>
+      <c r="BO9" s="136"/>
+      <c r="BP9" s="137"/>
       <c r="BQ9" s="25"/>
     </row>
     <row r="10" spans="1:69" ht="17.25" customHeight="1">
       <c r="A10" s="26"/>
-      <c r="B10" s="133"/>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="133"/>
+      <c r="B10" s="131"/>
+      <c r="C10" s="131"/>
+      <c r="D10" s="131"/>
+      <c r="E10" s="131"/>
+      <c r="F10" s="131"/>
+      <c r="G10" s="131"/>
+      <c r="H10" s="131"/>
       <c r="I10" s="27" t="s">
         <v>28</v>
       </c>
@@ -3256,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="66">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="I19" s="73"/>
       <c r="J19" s="74"/>
@@ -3341,7 +3344,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="66">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="I20" s="73"/>
       <c r="J20" s="74"/>
@@ -3596,7 +3599,7 @@
         <v>1</v>
       </c>
       <c r="H23" s="66">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I23" s="73"/>
       <c r="J23" s="74"/>
@@ -3756,7 +3759,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="43">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I25" s="44"/>
       <c r="J25" s="45"/>
@@ -3841,7 +3844,7 @@
         <v>1</v>
       </c>
       <c r="H26" s="43">
-        <v>0.7</v>
+        <v>1</v>
       </c>
       <c r="I26" s="52"/>
       <c r="J26" s="53"/>
@@ -3926,7 +3929,7 @@
         <v>1</v>
       </c>
       <c r="H27" s="43">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I27" s="52"/>
       <c r="J27" s="53"/>
@@ -4383,7 +4386,7 @@
       </c>
       <c r="G33" s="65"/>
       <c r="H33" s="80">
-        <v>0.45</v>
+        <v>0.5</v>
       </c>
       <c r="I33" s="73"/>
       <c r="J33" s="74"/>
@@ -5280,11 +5283,15 @@
       <c r="C45" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="21"/>
+      <c r="D45" s="21" t="s">
+        <v>72</v>
+      </c>
       <c r="E45" s="21"/>
       <c r="F45" s="21"/>
       <c r="G45" s="83"/>
-      <c r="H45" s="83"/>
+      <c r="H45" s="147">
+        <v>1</v>
+      </c>
       <c r="I45" s="21"/>
       <c r="J45" s="21"/>
       <c r="K45" s="21"/>
@@ -5420,6 +5427,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="BB8:BP8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="AM9:AQ9"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="O2:AE2"/>
@@ -5436,24 +5461,6 @@
     <mergeCell ref="P4:AB4"/>
     <mergeCell ref="P5:AA5"/>
     <mergeCell ref="I5:O5"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="BB8:BP8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="I9:M9"/>
   </mergeCells>
   <conditionalFormatting sqref="H12:H23 H30:H44 H25:H28">
     <cfRule type="colorScale" priority="3">

</xml_diff>

<commit_message>
removed unnecessary fields in forms
</commit_message>
<xml_diff>
--- a/docs/Gantt chart.xlsx
+++ b/docs/Gantt chart.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/connecture/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64851991-87A3-5D45-91D7-19EAA53E5471}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0460C7FB-05D7-244E-A830-39F59D5981BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gantchart" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="93">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -160,15 +160,6 @@
     <t>Modules</t>
   </si>
   <si>
-    <t>Module-1</t>
-  </si>
-  <si>
-    <t>Module-2</t>
-  </si>
-  <si>
-    <t>Module-3</t>
-  </si>
-  <si>
     <t>Module-4</t>
   </si>
   <si>
@@ -247,18 +238,12 @@
     <t>Riddhi, Aditya, Shauryan, Devansh</t>
   </si>
   <si>
-    <t xml:space="preserve">Module-1 </t>
-  </si>
-  <si>
     <t>Riddhi, Shauryan, Devansh, Aditya</t>
   </si>
   <si>
     <t>2.4.5</t>
   </si>
   <si>
-    <t>Module-5</t>
-  </si>
-  <si>
     <t>Devansh</t>
   </si>
   <si>
@@ -290,6 +275,30 @@
   </si>
   <si>
     <t>17/4/2021</t>
+  </si>
+  <si>
+    <t>Module-2: User profile</t>
+  </si>
+  <si>
+    <t>Module-3: Dashboard</t>
+  </si>
+  <si>
+    <t>Module-4: Navbar</t>
+  </si>
+  <si>
+    <t>Module-5: Posts</t>
+  </si>
+  <si>
+    <t>Module-1: Landing, Login, and Register</t>
+  </si>
+  <si>
+    <t>Module-1: Routes</t>
+  </si>
+  <si>
+    <t>Module-2: Middleware</t>
+  </si>
+  <si>
+    <t>Module-3: Models</t>
   </si>
 </sst>
 </file>
@@ -299,7 +308,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="50">
+  <fonts count="49">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -344,6 +353,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -382,10 +392,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <b/>
@@ -511,11 +523,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF434343"/>
       <name val="Roboto"/>
       <charset val="1"/>
@@ -572,7 +579,7 @@
       <name val="Roboto"/>
     </font>
   </fonts>
-  <fills count="51">
+  <fills count="50">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -829,12 +836,6 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF99FFDD"/>
-        <bgColor rgb="FF73C79E"/>
       </patternFill>
     </fill>
     <fill>
@@ -1113,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1453,7 +1454,6 @@
     <xf numFmtId="0" fontId="29" fillId="35" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="35" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1494,22 +1494,148 @@
     <xf numFmtId="0" fontId="38" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="39" fillId="44" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="29" fillId="45" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="48" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="46" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="36" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="47" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="48" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="43" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="47" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="46" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="49" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1522,154 +1648,26 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="49" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="47" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="22" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="19" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="36" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="48" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="48" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="49" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="44" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="48" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="47" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="50" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1998,18 +1996,18 @@
   </sheetPr>
   <dimension ref="A1:BQ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="AG69" sqref="AG69"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="174" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="149" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="187" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="174" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="160" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" style="149" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
     <col min="9" max="68" width="3.5" customWidth="1"/>
     <col min="69" max="69" width="3.83203125" customWidth="1"/>
@@ -2017,11 +2015,11 @@
   <sheetData>
     <row r="1" spans="1:69" ht="13" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="191"/>
+      <c r="B1" s="164"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="176"/>
-      <c r="F1" s="167"/>
+      <c r="E1" s="151"/>
+      <c r="F1" s="143"/>
       <c r="G1" s="3"/>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>
@@ -2088,38 +2086,38 @@
     </row>
     <row r="2" spans="1:69" ht="32" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="140" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="139"/>
-      <c r="D2" s="139"/>
-      <c r="E2" s="139"/>
-      <c r="F2" s="139"/>
-      <c r="G2" s="139"/>
+      <c r="B2" s="185" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="184"/>
+      <c r="D2" s="184"/>
+      <c r="E2" s="184"/>
+      <c r="F2" s="184"/>
+      <c r="G2" s="184"/>
       <c r="H2" s="87"/>
-      <c r="I2" s="138"/>
-      <c r="J2" s="139"/>
-      <c r="K2" s="139"/>
-      <c r="L2" s="139"/>
-      <c r="M2" s="139"/>
-      <c r="N2" s="139"/>
-      <c r="O2" s="141"/>
-      <c r="P2" s="139"/>
-      <c r="Q2" s="139"/>
-      <c r="R2" s="139"/>
-      <c r="S2" s="139"/>
-      <c r="T2" s="139"/>
-      <c r="U2" s="139"/>
-      <c r="V2" s="139"/>
-      <c r="W2" s="139"/>
-      <c r="X2" s="139"/>
-      <c r="Y2" s="139"/>
-      <c r="Z2" s="139"/>
-      <c r="AA2" s="139"/>
-      <c r="AB2" s="139"/>
-      <c r="AC2" s="139"/>
-      <c r="AD2" s="139"/>
-      <c r="AE2" s="139"/>
+      <c r="I2" s="183"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
+      <c r="L2" s="184"/>
+      <c r="M2" s="184"/>
+      <c r="N2" s="184"/>
+      <c r="O2" s="186"/>
+      <c r="P2" s="184"/>
+      <c r="Q2" s="184"/>
+      <c r="R2" s="184"/>
+      <c r="S2" s="184"/>
+      <c r="T2" s="184"/>
+      <c r="U2" s="184"/>
+      <c r="V2" s="184"/>
+      <c r="W2" s="184"/>
+      <c r="X2" s="184"/>
+      <c r="Y2" s="184"/>
+      <c r="Z2" s="184"/>
+      <c r="AA2" s="184"/>
+      <c r="AB2" s="184"/>
+      <c r="AC2" s="184"/>
+      <c r="AD2" s="184"/>
+      <c r="AE2" s="184"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
       <c r="AH2" s="10"/>
@@ -2161,11 +2159,11 @@
     </row>
     <row r="3" spans="1:69" ht="21" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="192"/>
+      <c r="B3" s="165"/>
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
-      <c r="E3" s="177"/>
-      <c r="F3" s="168"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="144"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
@@ -2232,41 +2230,41 @@
     </row>
     <row r="4" spans="1:69" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="168" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="146" t="s">
-        <v>63</v>
-      </c>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="143"/>
+      <c r="C4" s="169"/>
+      <c r="D4" s="188" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="169"/>
+      <c r="F4" s="169"/>
+      <c r="G4" s="169"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="142" t="s">
-        <v>81</v>
-      </c>
-      <c r="J4" s="143"/>
-      <c r="K4" s="143"/>
-      <c r="L4" s="143"/>
-      <c r="M4" s="143"/>
-      <c r="N4" s="143"/>
-      <c r="O4" s="143"/>
-      <c r="P4" s="147" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q4" s="143"/>
-      <c r="R4" s="143"/>
-      <c r="S4" s="143"/>
-      <c r="T4" s="143"/>
-      <c r="U4" s="143"/>
-      <c r="V4" s="143"/>
-      <c r="W4" s="143"/>
-      <c r="X4" s="143"/>
-      <c r="Y4" s="143"/>
-      <c r="Z4" s="143"/>
-      <c r="AA4" s="143"/>
-      <c r="AB4" s="143"/>
+      <c r="I4" s="168" t="s">
+        <v>76</v>
+      </c>
+      <c r="J4" s="169"/>
+      <c r="K4" s="169"/>
+      <c r="L4" s="169"/>
+      <c r="M4" s="169"/>
+      <c r="N4" s="169"/>
+      <c r="O4" s="169"/>
+      <c r="P4" s="192" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q4" s="169"/>
+      <c r="R4" s="169"/>
+      <c r="S4" s="169"/>
+      <c r="T4" s="169"/>
+      <c r="U4" s="169"/>
+      <c r="V4" s="169"/>
+      <c r="W4" s="169"/>
+      <c r="X4" s="169"/>
+      <c r="Y4" s="169"/>
+      <c r="Z4" s="169"/>
+      <c r="AA4" s="169"/>
+      <c r="AB4" s="169"/>
       <c r="AC4" s="16"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -2311,40 +2309,40 @@
     </row>
     <row r="5" spans="1:69" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="142" t="s">
+      <c r="B5" s="168" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="143"/>
-      <c r="D5" s="159" t="s">
-        <v>64</v>
-      </c>
-      <c r="E5" s="143"/>
-      <c r="F5" s="143"/>
-      <c r="G5" s="143"/>
+      <c r="C5" s="169"/>
+      <c r="D5" s="170" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="169"/>
+      <c r="F5" s="169"/>
+      <c r="G5" s="169"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="142" t="s">
+      <c r="I5" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="143"/>
-      <c r="K5" s="143"/>
-      <c r="L5" s="143"/>
-      <c r="M5" s="143"/>
-      <c r="N5" s="143"/>
-      <c r="O5" s="143"/>
-      <c r="P5" s="148" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q5" s="143"/>
-      <c r="R5" s="143"/>
-      <c r="S5" s="143"/>
-      <c r="T5" s="143"/>
-      <c r="U5" s="143"/>
-      <c r="V5" s="143"/>
-      <c r="W5" s="143"/>
-      <c r="X5" s="143"/>
-      <c r="Y5" s="143"/>
-      <c r="Z5" s="143"/>
-      <c r="AA5" s="143"/>
+      <c r="J5" s="169"/>
+      <c r="K5" s="169"/>
+      <c r="L5" s="169"/>
+      <c r="M5" s="169"/>
+      <c r="N5" s="169"/>
+      <c r="O5" s="169"/>
+      <c r="P5" s="193" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" s="169"/>
+      <c r="R5" s="169"/>
+      <c r="S5" s="169"/>
+      <c r="T5" s="169"/>
+      <c r="U5" s="169"/>
+      <c r="V5" s="169"/>
+      <c r="W5" s="169"/>
+      <c r="X5" s="169"/>
+      <c r="Y5" s="169"/>
+      <c r="Z5" s="169"/>
+      <c r="AA5" s="169"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="1"/>
@@ -2393,7 +2391,7 @@
       <c r="B6" s="22"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="178"/>
+      <c r="E6" s="153"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -2464,7 +2462,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="178"/>
+      <c r="E7" s="153"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -2532,201 +2530,201 @@
     </row>
     <row r="8" spans="1:69" ht="17.25" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="144" t="s">
+      <c r="B8" s="187" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="144" t="s">
+      <c r="C8" s="187" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="144" t="s">
+      <c r="D8" s="187" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="179" t="s">
+      <c r="E8" s="190" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="187" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="144" t="s">
+      <c r="G8" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="144" t="s">
+      <c r="H8" s="187" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="153" t="s">
+      <c r="I8" s="176" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="145"/>
-      <c r="K8" s="145"/>
-      <c r="L8" s="145"/>
-      <c r="M8" s="145"/>
-      <c r="N8" s="145"/>
-      <c r="O8" s="145"/>
-      <c r="P8" s="145"/>
-      <c r="Q8" s="145"/>
-      <c r="R8" s="145"/>
-      <c r="S8" s="145"/>
-      <c r="T8" s="145"/>
-      <c r="U8" s="145"/>
-      <c r="V8" s="145"/>
-      <c r="W8" s="145"/>
-      <c r="X8" s="154" t="s">
+      <c r="J8" s="177"/>
+      <c r="K8" s="177"/>
+      <c r="L8" s="177"/>
+      <c r="M8" s="177"/>
+      <c r="N8" s="177"/>
+      <c r="O8" s="177"/>
+      <c r="P8" s="177"/>
+      <c r="Q8" s="177"/>
+      <c r="R8" s="177"/>
+      <c r="S8" s="177"/>
+      <c r="T8" s="177"/>
+      <c r="U8" s="177"/>
+      <c r="V8" s="177"/>
+      <c r="W8" s="177"/>
+      <c r="X8" s="178" t="s">
         <v>11</v>
       </c>
-      <c r="Y8" s="145"/>
-      <c r="Z8" s="145"/>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="145"/>
-      <c r="AC8" s="145"/>
-      <c r="AD8" s="145"/>
-      <c r="AE8" s="145"/>
-      <c r="AF8" s="145"/>
-      <c r="AG8" s="145"/>
-      <c r="AH8" s="145"/>
-      <c r="AI8" s="145"/>
-      <c r="AJ8" s="145"/>
-      <c r="AK8" s="145"/>
-      <c r="AL8" s="145"/>
-      <c r="AM8" s="157" t="s">
+      <c r="Y8" s="177"/>
+      <c r="Z8" s="177"/>
+      <c r="AA8" s="177"/>
+      <c r="AB8" s="177"/>
+      <c r="AC8" s="177"/>
+      <c r="AD8" s="177"/>
+      <c r="AE8" s="177"/>
+      <c r="AF8" s="177"/>
+      <c r="AG8" s="177"/>
+      <c r="AH8" s="177"/>
+      <c r="AI8" s="177"/>
+      <c r="AJ8" s="177"/>
+      <c r="AK8" s="177"/>
+      <c r="AL8" s="177"/>
+      <c r="AM8" s="181" t="s">
         <v>12</v>
       </c>
-      <c r="AN8" s="145"/>
-      <c r="AO8" s="145"/>
-      <c r="AP8" s="145"/>
-      <c r="AQ8" s="145"/>
-      <c r="AR8" s="145"/>
-      <c r="AS8" s="145"/>
-      <c r="AT8" s="145"/>
-      <c r="AU8" s="145"/>
-      <c r="AV8" s="145"/>
-      <c r="AW8" s="145"/>
-      <c r="AX8" s="145"/>
-      <c r="AY8" s="145"/>
-      <c r="AZ8" s="145"/>
-      <c r="BA8" s="145"/>
-      <c r="BB8" s="155" t="s">
+      <c r="AN8" s="177"/>
+      <c r="AO8" s="177"/>
+      <c r="AP8" s="177"/>
+      <c r="AQ8" s="177"/>
+      <c r="AR8" s="177"/>
+      <c r="AS8" s="177"/>
+      <c r="AT8" s="177"/>
+      <c r="AU8" s="177"/>
+      <c r="AV8" s="177"/>
+      <c r="AW8" s="177"/>
+      <c r="AX8" s="177"/>
+      <c r="AY8" s="177"/>
+      <c r="AZ8" s="177"/>
+      <c r="BA8" s="177"/>
+      <c r="BB8" s="179" t="s">
         <v>13</v>
       </c>
-      <c r="BC8" s="145"/>
-      <c r="BD8" s="145"/>
-      <c r="BE8" s="145"/>
-      <c r="BF8" s="145"/>
-      <c r="BG8" s="145"/>
-      <c r="BH8" s="145"/>
-      <c r="BI8" s="145"/>
-      <c r="BJ8" s="145"/>
-      <c r="BK8" s="145"/>
-      <c r="BL8" s="145"/>
-      <c r="BM8" s="145"/>
-      <c r="BN8" s="145"/>
-      <c r="BO8" s="145"/>
-      <c r="BP8" s="156"/>
+      <c r="BC8" s="177"/>
+      <c r="BD8" s="177"/>
+      <c r="BE8" s="177"/>
+      <c r="BF8" s="177"/>
+      <c r="BG8" s="177"/>
+      <c r="BH8" s="177"/>
+      <c r="BI8" s="177"/>
+      <c r="BJ8" s="177"/>
+      <c r="BK8" s="177"/>
+      <c r="BL8" s="177"/>
+      <c r="BM8" s="177"/>
+      <c r="BN8" s="177"/>
+      <c r="BO8" s="177"/>
+      <c r="BP8" s="180"/>
       <c r="BQ8" s="20"/>
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="169"/>
-      <c r="C9" s="145"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="180"/>
-      <c r="F9" s="169"/>
-      <c r="G9" s="145"/>
-      <c r="H9" s="145"/>
-      <c r="I9" s="160" t="s">
+      <c r="B9" s="189"/>
+      <c r="C9" s="177"/>
+      <c r="D9" s="177"/>
+      <c r="E9" s="191"/>
+      <c r="F9" s="189"/>
+      <c r="G9" s="177"/>
+      <c r="H9" s="177"/>
+      <c r="I9" s="171" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="150"/>
-      <c r="K9" s="150"/>
-      <c r="L9" s="150"/>
-      <c r="M9" s="151"/>
-      <c r="N9" s="160" t="s">
+      <c r="J9" s="172"/>
+      <c r="K9" s="172"/>
+      <c r="L9" s="172"/>
+      <c r="M9" s="173"/>
+      <c r="N9" s="171" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="150"/>
-      <c r="P9" s="150"/>
-      <c r="Q9" s="150"/>
-      <c r="R9" s="151"/>
-      <c r="S9" s="160" t="s">
+      <c r="O9" s="172"/>
+      <c r="P9" s="172"/>
+      <c r="Q9" s="172"/>
+      <c r="R9" s="173"/>
+      <c r="S9" s="171" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="150"/>
-      <c r="U9" s="150"/>
-      <c r="V9" s="150"/>
-      <c r="W9" s="151"/>
-      <c r="X9" s="152" t="s">
+      <c r="T9" s="172"/>
+      <c r="U9" s="172"/>
+      <c r="V9" s="172"/>
+      <c r="W9" s="173"/>
+      <c r="X9" s="175" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="150"/>
-      <c r="Z9" s="150"/>
-      <c r="AA9" s="150"/>
-      <c r="AB9" s="151"/>
-      <c r="AC9" s="152" t="s">
+      <c r="Y9" s="172"/>
+      <c r="Z9" s="172"/>
+      <c r="AA9" s="172"/>
+      <c r="AB9" s="173"/>
+      <c r="AC9" s="175" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="150"/>
-      <c r="AE9" s="150"/>
-      <c r="AF9" s="150"/>
-      <c r="AG9" s="151"/>
-      <c r="AH9" s="152" t="s">
+      <c r="AD9" s="172"/>
+      <c r="AE9" s="172"/>
+      <c r="AF9" s="172"/>
+      <c r="AG9" s="173"/>
+      <c r="AH9" s="175" t="s">
         <v>19</v>
       </c>
-      <c r="AI9" s="150"/>
-      <c r="AJ9" s="150"/>
-      <c r="AK9" s="150"/>
-      <c r="AL9" s="151"/>
-      <c r="AM9" s="158" t="s">
+      <c r="AI9" s="172"/>
+      <c r="AJ9" s="172"/>
+      <c r="AK9" s="172"/>
+      <c r="AL9" s="173"/>
+      <c r="AM9" s="182" t="s">
         <v>20</v>
       </c>
-      <c r="AN9" s="150"/>
-      <c r="AO9" s="150"/>
-      <c r="AP9" s="150"/>
-      <c r="AQ9" s="151"/>
-      <c r="AR9" s="158" t="s">
+      <c r="AN9" s="172"/>
+      <c r="AO9" s="172"/>
+      <c r="AP9" s="172"/>
+      <c r="AQ9" s="173"/>
+      <c r="AR9" s="182" t="s">
         <v>21</v>
       </c>
-      <c r="AS9" s="150"/>
-      <c r="AT9" s="150"/>
-      <c r="AU9" s="150"/>
-      <c r="AV9" s="151"/>
-      <c r="AW9" s="158" t="s">
+      <c r="AS9" s="172"/>
+      <c r="AT9" s="172"/>
+      <c r="AU9" s="172"/>
+      <c r="AV9" s="173"/>
+      <c r="AW9" s="182" t="s">
         <v>22</v>
       </c>
-      <c r="AX9" s="150"/>
-      <c r="AY9" s="150"/>
-      <c r="AZ9" s="150"/>
-      <c r="BA9" s="151"/>
-      <c r="BB9" s="149" t="s">
+      <c r="AX9" s="172"/>
+      <c r="AY9" s="172"/>
+      <c r="AZ9" s="172"/>
+      <c r="BA9" s="173"/>
+      <c r="BB9" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="BC9" s="150"/>
-      <c r="BD9" s="150"/>
-      <c r="BE9" s="150"/>
-      <c r="BF9" s="151"/>
-      <c r="BG9" s="149" t="s">
+      <c r="BC9" s="172"/>
+      <c r="BD9" s="172"/>
+      <c r="BE9" s="172"/>
+      <c r="BF9" s="173"/>
+      <c r="BG9" s="174" t="s">
         <v>24</v>
       </c>
-      <c r="BH9" s="150"/>
-      <c r="BI9" s="150"/>
-      <c r="BJ9" s="150"/>
-      <c r="BK9" s="151"/>
-      <c r="BL9" s="149" t="s">
+      <c r="BH9" s="172"/>
+      <c r="BI9" s="172"/>
+      <c r="BJ9" s="172"/>
+      <c r="BK9" s="173"/>
+      <c r="BL9" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="BM9" s="150"/>
-      <c r="BN9" s="150"/>
-      <c r="BO9" s="150"/>
-      <c r="BP9" s="151"/>
+      <c r="BM9" s="172"/>
+      <c r="BN9" s="172"/>
+      <c r="BO9" s="172"/>
+      <c r="BP9" s="173"/>
       <c r="BQ9" s="24"/>
     </row>
     <row r="10" spans="1:69" ht="17.25" customHeight="1">
       <c r="A10" s="25"/>
-      <c r="B10" s="169"/>
-      <c r="C10" s="145"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="180"/>
-      <c r="F10" s="169"/>
-      <c r="G10" s="145"/>
-      <c r="H10" s="145"/>
+      <c r="B10" s="189"/>
+      <c r="C10" s="177"/>
+      <c r="D10" s="177"/>
+      <c r="E10" s="191"/>
+      <c r="F10" s="189"/>
+      <c r="G10" s="177"/>
+      <c r="H10" s="177"/>
       <c r="I10" s="26" t="s">
         <v>26</v>
       </c>
@@ -2911,15 +2909,15 @@
     </row>
     <row r="11" spans="1:69" ht="21" customHeight="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="170">
+      <c r="B11" s="145">
         <v>1</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="181"/>
-      <c r="F11" s="170"/>
+      <c r="E11" s="154"/>
+      <c r="F11" s="145"/>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="32"/>
@@ -2990,15 +2988,15 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E12" s="182">
+        <v>63</v>
+      </c>
+      <c r="E12" s="155">
         <v>43961</v>
       </c>
-      <c r="F12" s="171">
+      <c r="F12" s="146">
         <v>44023</v>
       </c>
       <c r="G12" s="38">
@@ -3075,15 +3073,15 @@
         <v>32</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" s="182">
+        <v>63</v>
+      </c>
+      <c r="E13" s="155">
         <v>44023</v>
       </c>
-      <c r="F13" s="171">
+      <c r="F13" s="146">
         <v>44023</v>
       </c>
       <c r="G13" s="38">
@@ -3163,13 +3161,13 @@
         <v>33</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="182" t="s">
-        <v>71</v>
-      </c>
-      <c r="F14" s="171" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="E14" s="155" t="s">
+        <v>68</v>
+      </c>
+      <c r="F14" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="G14" s="38">
         <v>1</v>
@@ -3248,13 +3246,13 @@
         <v>34</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="182" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="171" t="s">
-        <v>72</v>
+        <v>64</v>
+      </c>
+      <c r="E15" s="155" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="G15" s="38">
         <v>2</v>
@@ -3333,13 +3331,13 @@
         <v>36</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E16" s="182">
+        <v>62</v>
+      </c>
+      <c r="E16" s="155">
         <v>44115</v>
       </c>
-      <c r="F16" s="171" t="s">
-        <v>72</v>
+      <c r="F16" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="G16" s="38">
         <v>1</v>
@@ -3418,13 +3416,13 @@
         <v>35</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E17" s="182">
+        <v>62</v>
+      </c>
+      <c r="E17" s="155">
         <v>44115</v>
       </c>
-      <c r="F17" s="171" t="s">
-        <v>72</v>
+      <c r="F17" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="G17" s="38">
         <v>1</v>
@@ -3503,13 +3501,13 @@
         <v>37</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="182">
+        <v>64</v>
+      </c>
+      <c r="E18" s="155">
         <v>44115</v>
       </c>
-      <c r="F18" s="171" t="s">
-        <v>72</v>
+      <c r="F18" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="G18" s="59">
         <v>1</v>
@@ -3585,16 +3583,16 @@
         <v>1.7</v>
       </c>
       <c r="C19" s="58" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="183">
+        <v>64</v>
+      </c>
+      <c r="E19" s="156">
         <v>44115</v>
       </c>
-      <c r="F19" s="171" t="s">
-        <v>72</v>
+      <c r="F19" s="146" t="s">
+        <v>69</v>
       </c>
       <c r="G19" s="59">
         <v>1</v>
@@ -3673,13 +3671,13 @@
         <v>38</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="183">
+        <v>66</v>
+      </c>
+      <c r="E20" s="156">
         <v>44116</v>
       </c>
-      <c r="F20" s="172" t="s">
-        <v>73</v>
+      <c r="F20" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G20" s="59">
         <v>1</v>
@@ -3758,13 +3756,13 @@
         <v>39</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="183">
+        <v>64</v>
+      </c>
+      <c r="E21" s="156">
         <v>44115</v>
       </c>
-      <c r="F21" s="172" t="s">
-        <v>73</v>
+      <c r="F21" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G21" s="59">
         <v>1</v>
@@ -3843,13 +3841,13 @@
         <v>40</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="183">
+        <v>64</v>
+      </c>
+      <c r="E22" s="156">
         <v>44115</v>
       </c>
-      <c r="F22" s="172" t="s">
-        <v>73</v>
+      <c r="F22" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G22" s="59">
         <v>1</v>
@@ -3921,20 +3919,20 @@
     </row>
     <row r="23" spans="1:69" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A23" s="36"/>
-      <c r="B23" s="193">
+      <c r="B23" s="166">
         <v>1.1100000000000001</v>
       </c>
       <c r="C23" s="58" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="E23" s="183">
+        <v>62</v>
+      </c>
+      <c r="E23" s="156">
         <v>44115</v>
       </c>
-      <c r="F23" s="172" t="s">
-        <v>73</v>
+      <c r="F23" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G23" s="59">
         <v>1</v>
@@ -4006,15 +4004,15 @@
     </row>
     <row r="24" spans="1:69" ht="21" customHeight="1">
       <c r="A24" s="20"/>
-      <c r="B24" s="170">
+      <c r="B24" s="145">
         <v>2</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="31"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="170"/>
+      <c r="E24" s="154"/>
+      <c r="F24" s="145"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
       <c r="I24" s="32"/>
@@ -4088,13 +4086,13 @@
         <v>43</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25" s="183">
+        <v>65</v>
+      </c>
+      <c r="E25" s="156">
         <v>44115</v>
       </c>
-      <c r="F25" s="172" t="s">
-        <v>73</v>
+      <c r="F25" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G25" s="38">
         <v>1</v>
@@ -4173,13 +4171,13 @@
         <v>44</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="183">
+        <v>66</v>
+      </c>
+      <c r="E26" s="156">
         <v>44115</v>
       </c>
-      <c r="F26" s="172" t="s">
-        <v>73</v>
+      <c r="F26" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G26" s="38">
         <v>1</v>
@@ -4255,16 +4253,16 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="183">
+        <v>66</v>
+      </c>
+      <c r="E27" s="156">
         <v>44115</v>
       </c>
-      <c r="F27" s="172" t="s">
-        <v>73</v>
+      <c r="F27" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G27" s="38">
         <v>1</v>
@@ -4334,102 +4332,102 @@
       <c r="BP27" s="56"/>
       <c r="BQ27" s="36"/>
     </row>
-    <row r="28" spans="1:69" s="130" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
-      <c r="A28" s="118"/>
-      <c r="B28" s="194">
+    <row r="28" spans="1:69" s="129" customFormat="1" ht="17.25" customHeight="1" outlineLevel="1">
+      <c r="A28" s="117"/>
+      <c r="B28" s="167">
         <v>2.4</v>
       </c>
-      <c r="C28" s="131" t="s">
+      <c r="C28" s="130" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="119"/>
-      <c r="E28" s="184"/>
-      <c r="F28" s="173"/>
-      <c r="G28" s="120"/>
-      <c r="H28" s="121"/>
-      <c r="I28" s="122"/>
-      <c r="J28" s="123"/>
-      <c r="K28" s="124"/>
-      <c r="L28" s="124"/>
-      <c r="M28" s="124"/>
-      <c r="N28" s="125"/>
-      <c r="O28" s="125"/>
-      <c r="P28" s="125"/>
-      <c r="Q28" s="125"/>
-      <c r="R28" s="125"/>
-      <c r="S28" s="124"/>
-      <c r="T28" s="124"/>
-      <c r="U28" s="124"/>
-      <c r="V28" s="124"/>
-      <c r="W28" s="124"/>
-      <c r="X28" s="124"/>
-      <c r="Y28" s="124"/>
-      <c r="Z28" s="124"/>
-      <c r="AA28" s="124"/>
-      <c r="AB28" s="124"/>
-      <c r="AC28" s="126"/>
-      <c r="AD28" s="126"/>
-      <c r="AE28" s="126"/>
-      <c r="AF28" s="126"/>
-      <c r="AG28" s="126"/>
-      <c r="AH28" s="124"/>
-      <c r="AI28" s="124"/>
-      <c r="AJ28" s="124"/>
-      <c r="AK28" s="124"/>
-      <c r="AL28" s="124"/>
-      <c r="AM28" s="124"/>
-      <c r="AN28" s="124"/>
-      <c r="AO28" s="124"/>
-      <c r="AP28" s="124"/>
-      <c r="AQ28" s="124"/>
-      <c r="AR28" s="127"/>
-      <c r="AS28" s="127"/>
-      <c r="AT28" s="127"/>
-      <c r="AU28" s="127"/>
-      <c r="AV28" s="127"/>
-      <c r="AW28" s="124"/>
-      <c r="AX28" s="124"/>
-      <c r="AY28" s="124"/>
-      <c r="AZ28" s="124"/>
-      <c r="BA28" s="124"/>
-      <c r="BB28" s="124"/>
-      <c r="BC28" s="124"/>
-      <c r="BD28" s="124"/>
-      <c r="BE28" s="124"/>
-      <c r="BF28" s="124"/>
-      <c r="BG28" s="128"/>
-      <c r="BH28" s="128"/>
-      <c r="BI28" s="128"/>
-      <c r="BJ28" s="128"/>
-      <c r="BK28" s="128"/>
-      <c r="BL28" s="124"/>
-      <c r="BM28" s="124"/>
-      <c r="BN28" s="124"/>
-      <c r="BO28" s="124"/>
-      <c r="BP28" s="129"/>
-      <c r="BQ28" s="118"/>
+      <c r="D28" s="118"/>
+      <c r="E28" s="157"/>
+      <c r="F28" s="148"/>
+      <c r="G28" s="119"/>
+      <c r="H28" s="120"/>
+      <c r="I28" s="121"/>
+      <c r="J28" s="122"/>
+      <c r="K28" s="123"/>
+      <c r="L28" s="123"/>
+      <c r="M28" s="123"/>
+      <c r="N28" s="124"/>
+      <c r="O28" s="124"/>
+      <c r="P28" s="124"/>
+      <c r="Q28" s="124"/>
+      <c r="R28" s="124"/>
+      <c r="S28" s="123"/>
+      <c r="T28" s="123"/>
+      <c r="U28" s="123"/>
+      <c r="V28" s="123"/>
+      <c r="W28" s="123"/>
+      <c r="X28" s="123"/>
+      <c r="Y28" s="123"/>
+      <c r="Z28" s="123"/>
+      <c r="AA28" s="123"/>
+      <c r="AB28" s="123"/>
+      <c r="AC28" s="125"/>
+      <c r="AD28" s="125"/>
+      <c r="AE28" s="125"/>
+      <c r="AF28" s="125"/>
+      <c r="AG28" s="125"/>
+      <c r="AH28" s="123"/>
+      <c r="AI28" s="123"/>
+      <c r="AJ28" s="123"/>
+      <c r="AK28" s="123"/>
+      <c r="AL28" s="123"/>
+      <c r="AM28" s="123"/>
+      <c r="AN28" s="123"/>
+      <c r="AO28" s="123"/>
+      <c r="AP28" s="123"/>
+      <c r="AQ28" s="123"/>
+      <c r="AR28" s="126"/>
+      <c r="AS28" s="126"/>
+      <c r="AT28" s="126"/>
+      <c r="AU28" s="126"/>
+      <c r="AV28" s="126"/>
+      <c r="AW28" s="123"/>
+      <c r="AX28" s="123"/>
+      <c r="AY28" s="123"/>
+      <c r="AZ28" s="123"/>
+      <c r="BA28" s="123"/>
+      <c r="BB28" s="123"/>
+      <c r="BC28" s="123"/>
+      <c r="BD28" s="123"/>
+      <c r="BE28" s="123"/>
+      <c r="BF28" s="123"/>
+      <c r="BG28" s="127"/>
+      <c r="BH28" s="127"/>
+      <c r="BI28" s="127"/>
+      <c r="BJ28" s="127"/>
+      <c r="BK28" s="127"/>
+      <c r="BL28" s="123"/>
+      <c r="BM28" s="123"/>
+      <c r="BN28" s="123"/>
+      <c r="BO28" s="123"/>
+      <c r="BP28" s="128"/>
+      <c r="BQ28" s="117"/>
     </row>
     <row r="29" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A29" s="36"/>
       <c r="B29" s="59" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E29" s="183" t="s">
-        <v>84</v>
-      </c>
-      <c r="F29" s="172">
+        <v>72</v>
+      </c>
+      <c r="E29" s="156" t="s">
+        <v>79</v>
+      </c>
+      <c r="F29" s="147">
         <v>44319</v>
       </c>
       <c r="G29" s="59">
         <v>3</v>
       </c>
-      <c r="H29" s="133">
+      <c r="H29" s="131">
         <v>1</v>
       </c>
       <c r="I29" s="67"/>
@@ -4462,16 +4460,16 @@
       <c r="AJ29" s="69"/>
       <c r="AK29" s="69"/>
       <c r="AL29" s="69"/>
-      <c r="AM29" s="161"/>
-      <c r="AN29" s="135"/>
-      <c r="AO29" s="135"/>
-      <c r="AP29" s="135"/>
+      <c r="AM29" s="137"/>
+      <c r="AN29" s="133"/>
+      <c r="AO29" s="133"/>
+      <c r="AP29" s="133"/>
       <c r="AQ29" s="106"/>
-      <c r="AR29" s="136"/>
-      <c r="AS29" s="136"/>
-      <c r="AT29" s="136"/>
+      <c r="AR29" s="134"/>
+      <c r="AS29" s="134"/>
+      <c r="AT29" s="134"/>
       <c r="AU29" s="71"/>
-      <c r="AV29" s="136"/>
+      <c r="AV29" s="134"/>
       <c r="AW29" s="106"/>
       <c r="AX29" s="106"/>
       <c r="AY29" s="106"/>
@@ -4497,19 +4495,19 @@
     <row r="30" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A30" s="36"/>
       <c r="B30" s="59" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>47</v>
-      </c>
-      <c r="D30" s="134" t="s">
-        <v>76</v>
-      </c>
-      <c r="E30" s="183">
+        <v>85</v>
+      </c>
+      <c r="D30" s="132" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="156">
         <v>44533</v>
       </c>
-      <c r="F30" s="172" t="s">
-        <v>85</v>
+      <c r="F30" s="147" t="s">
+        <v>80</v>
       </c>
       <c r="G30" s="59">
         <v>5</v>
@@ -4550,23 +4548,23 @@
       <c r="AM30" s="69"/>
       <c r="AN30" s="69"/>
       <c r="AO30" s="106"/>
-      <c r="AP30" s="135"/>
-      <c r="AQ30" s="135"/>
+      <c r="AP30" s="133"/>
+      <c r="AQ30" s="133"/>
       <c r="AR30" s="71"/>
       <c r="AS30" s="71"/>
-      <c r="AT30" s="136"/>
-      <c r="AU30" s="162"/>
-      <c r="AV30" s="136"/>
-      <c r="AW30" s="135"/>
-      <c r="AX30" s="135"/>
+      <c r="AT30" s="134"/>
+      <c r="AU30" s="138"/>
+      <c r="AV30" s="134"/>
+      <c r="AW30" s="133"/>
+      <c r="AX30" s="133"/>
       <c r="AY30" s="106"/>
-      <c r="AZ30" s="135"/>
-      <c r="BA30" s="135"/>
+      <c r="AZ30" s="133"/>
+      <c r="BA30" s="133"/>
       <c r="BB30" s="69"/>
       <c r="BC30" s="69"/>
       <c r="BD30" s="69"/>
       <c r="BE30" s="106" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="BF30" s="106"/>
       <c r="BG30" s="72"/>
@@ -4584,18 +4582,18 @@
     <row r="31" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A31" s="36"/>
       <c r="B31" s="59" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="D31" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="E31" s="183" t="s">
-        <v>87</v>
-      </c>
-      <c r="F31" s="172">
+        <v>72</v>
+      </c>
+      <c r="E31" s="156" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" s="147">
         <v>44474</v>
       </c>
       <c r="G31" s="59">
@@ -4644,8 +4642,8 @@
       <c r="AT31" s="71"/>
       <c r="AU31" s="71"/>
       <c r="AV31" s="71"/>
-      <c r="AW31" s="135"/>
-      <c r="AX31" s="135"/>
+      <c r="AW31" s="133"/>
+      <c r="AX31" s="133"/>
       <c r="AY31" s="69"/>
       <c r="AZ31" s="106"/>
       <c r="BA31" s="69"/>
@@ -4654,10 +4652,10 @@
       <c r="BD31" s="69"/>
       <c r="BE31" s="106"/>
       <c r="BF31" s="106"/>
-      <c r="BG31" s="137"/>
-      <c r="BH31" s="137"/>
-      <c r="BI31" s="137"/>
-      <c r="BJ31" s="137"/>
+      <c r="BG31" s="135"/>
+      <c r="BH31" s="135"/>
+      <c r="BI31" s="135"/>
+      <c r="BJ31" s="135"/>
       <c r="BK31" s="72"/>
       <c r="BL31" s="106"/>
       <c r="BM31" s="69"/>
@@ -4669,18 +4667,18 @@
     <row r="32" spans="1:69" ht="20" customHeight="1" outlineLevel="1">
       <c r="A32" s="36"/>
       <c r="B32" s="59" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="D32" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="E32" s="183" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" s="172">
+        <v>72</v>
+      </c>
+      <c r="E32" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="147">
         <v>44474</v>
       </c>
       <c r="G32" s="59">
@@ -4727,23 +4725,23 @@
       <c r="AR32" s="71"/>
       <c r="AS32" s="71"/>
       <c r="AT32" s="71"/>
-      <c r="AU32" s="162"/>
-      <c r="AV32" s="162"/>
+      <c r="AU32" s="138"/>
+      <c r="AV32" s="138"/>
       <c r="AW32" s="106"/>
       <c r="AX32" s="106"/>
-      <c r="AY32" s="135"/>
-      <c r="AZ32" s="135"/>
-      <c r="BA32" s="106"/>
+      <c r="AY32" s="133"/>
+      <c r="AZ32" s="133"/>
+      <c r="BA32" s="133"/>
       <c r="BB32" s="69"/>
       <c r="BC32" s="69"/>
       <c r="BD32" s="106"/>
       <c r="BE32" s="106"/>
       <c r="BF32" s="106"/>
-      <c r="BG32" s="137"/>
+      <c r="BG32" s="135"/>
       <c r="BH32" s="72"/>
       <c r="BI32" s="72"/>
-      <c r="BJ32" s="137"/>
-      <c r="BK32" s="137"/>
+      <c r="BJ32" s="135"/>
+      <c r="BK32" s="135"/>
       <c r="BL32" s="106"/>
       <c r="BM32" s="106"/>
       <c r="BN32" s="106"/>
@@ -4751,27 +4749,27 @@
       <c r="BP32" s="106"/>
       <c r="BQ32" s="36"/>
     </row>
-    <row r="33" spans="1:69" s="117" customFormat="1" ht="20" customHeight="1" outlineLevel="1">
+    <row r="33" spans="1:69" s="136" customFormat="1" ht="20" customHeight="1" outlineLevel="1">
       <c r="A33" s="36"/>
       <c r="B33" s="59" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>78</v>
+        <v>88</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>79</v>
-      </c>
-      <c r="E33" s="183" t="s">
-        <v>86</v>
-      </c>
-      <c r="F33" s="172" t="s">
-        <v>88</v>
+        <v>74</v>
+      </c>
+      <c r="E33" s="156" t="s">
+        <v>81</v>
+      </c>
+      <c r="F33" s="147" t="s">
+        <v>83</v>
       </c>
       <c r="G33" s="59">
         <v>3</v>
       </c>
-      <c r="H33" s="132">
+      <c r="H33" s="89">
         <v>0.25</v>
       </c>
       <c r="I33" s="67"/>
@@ -4799,59 +4797,59 @@
       <c r="AE33" s="95"/>
       <c r="AF33" s="95"/>
       <c r="AG33" s="95"/>
-      <c r="AH33" s="74"/>
-      <c r="AI33" s="74"/>
-      <c r="AJ33" s="74"/>
-      <c r="AK33" s="74"/>
-      <c r="AL33" s="74"/>
-      <c r="AM33" s="74"/>
-      <c r="AN33" s="74"/>
+      <c r="AH33" s="106"/>
+      <c r="AI33" s="106"/>
+      <c r="AJ33" s="106"/>
+      <c r="AK33" s="106"/>
+      <c r="AL33" s="106"/>
+      <c r="AM33" s="106"/>
+      <c r="AN33" s="106"/>
       <c r="AO33" s="74"/>
       <c r="AP33" s="74"/>
       <c r="AQ33" s="74"/>
       <c r="AR33" s="71"/>
       <c r="AS33" s="71"/>
       <c r="AT33" s="71"/>
-      <c r="AU33" s="71"/>
-      <c r="AV33" s="71"/>
-      <c r="AW33" s="74"/>
-      <c r="AX33" s="74"/>
+      <c r="AU33" s="138"/>
+      <c r="AV33" s="138"/>
+      <c r="AW33" s="106"/>
+      <c r="AX33" s="106"/>
       <c r="AY33" s="106"/>
-      <c r="AZ33" s="106"/>
-      <c r="BA33" s="135"/>
+      <c r="AZ33" s="133"/>
+      <c r="BA33" s="106"/>
       <c r="BB33" s="74"/>
       <c r="BC33" s="74"/>
-      <c r="BD33" s="74"/>
-      <c r="BE33" s="74"/>
-      <c r="BF33" s="74"/>
-      <c r="BG33" s="72"/>
+      <c r="BD33" s="106"/>
+      <c r="BE33" s="106"/>
+      <c r="BF33" s="106"/>
+      <c r="BG33" s="135"/>
       <c r="BH33" s="72"/>
       <c r="BI33" s="72"/>
-      <c r="BJ33" s="72"/>
-      <c r="BK33" s="72"/>
-      <c r="BL33" s="74"/>
-      <c r="BM33" s="74"/>
-      <c r="BN33" s="74"/>
-      <c r="BO33" s="74"/>
-      <c r="BP33" s="74"/>
+      <c r="BJ33" s="135"/>
+      <c r="BK33" s="135"/>
+      <c r="BL33" s="106"/>
+      <c r="BM33" s="106"/>
+      <c r="BN33" s="106"/>
+      <c r="BO33" s="106"/>
+      <c r="BP33" s="106"/>
       <c r="BQ33" s="36"/>
     </row>
     <row r="34" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A34" s="36"/>
       <c r="B34" s="59" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C34" s="58" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D34" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="183">
+        <v>71</v>
+      </c>
+      <c r="E34" s="156">
         <v>44116</v>
       </c>
-      <c r="F34" s="172" t="s">
-        <v>73</v>
+      <c r="F34" s="147" t="s">
+        <v>70</v>
       </c>
       <c r="G34" s="59">
         <v>2</v>
@@ -4923,15 +4921,15 @@
     </row>
     <row r="35" spans="1:69" ht="21" customHeight="1">
       <c r="A35" s="20"/>
-      <c r="B35" s="170">
+      <c r="B35" s="145">
         <v>3</v>
       </c>
       <c r="C35" s="30" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D35" s="31"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="170"/>
+      <c r="E35" s="154"/>
+      <c r="F35" s="145"/>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>
       <c r="I35" s="32"/>
@@ -5002,15 +5000,15 @@
         <v>3.1</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="D36" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E36" s="183" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="172">
+        <v>72</v>
+      </c>
+      <c r="E36" s="156" t="s">
+        <v>79</v>
+      </c>
+      <c r="F36" s="147">
         <v>44319</v>
       </c>
       <c r="G36" s="38">
@@ -5064,11 +5062,11 @@
       <c r="AY36" s="44"/>
       <c r="AZ36" s="44"/>
       <c r="BA36" s="44"/>
-      <c r="BB36" s="163"/>
-      <c r="BC36" s="163"/>
+      <c r="BB36" s="139"/>
+      <c r="BC36" s="139"/>
       <c r="BD36" s="44"/>
-      <c r="BE36" s="163"/>
-      <c r="BF36" s="163"/>
+      <c r="BE36" s="139"/>
+      <c r="BF36" s="139"/>
       <c r="BG36" s="46"/>
       <c r="BH36" s="46"/>
       <c r="BI36" s="46"/>
@@ -5087,15 +5085,15 @@
         <v>3.2</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="D37" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E37" s="183" t="s">
-        <v>87</v>
-      </c>
-      <c r="F37" s="172">
+        <v>72</v>
+      </c>
+      <c r="E37" s="156" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="147">
         <v>44474</v>
       </c>
       <c r="G37" s="38">
@@ -5153,13 +5151,13 @@
       <c r="BC37" s="51"/>
       <c r="BD37" s="51"/>
       <c r="BE37" s="51"/>
-      <c r="BF37" s="189"/>
-      <c r="BG37" s="190"/>
-      <c r="BH37" s="190"/>
+      <c r="BF37" s="162"/>
+      <c r="BG37" s="163"/>
+      <c r="BH37" s="163"/>
       <c r="BI37" s="55"/>
-      <c r="BJ37" s="190"/>
-      <c r="BK37" s="188"/>
-      <c r="BL37" s="189"/>
+      <c r="BJ37" s="163"/>
+      <c r="BK37" s="161"/>
+      <c r="BL37" s="162"/>
       <c r="BM37" s="51"/>
       <c r="BN37" s="51"/>
       <c r="BO37" s="51"/>
@@ -5172,22 +5170,22 @@
         <v>3.3</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="D38" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E38" s="183" t="s">
-        <v>89</v>
-      </c>
-      <c r="F38" s="172">
+        <v>72</v>
+      </c>
+      <c r="E38" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="F38" s="147">
         <v>44474</v>
       </c>
       <c r="G38" s="38">
         <v>3</v>
       </c>
       <c r="H38" s="39">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I38" s="48"/>
       <c r="J38" s="49"/>
@@ -5239,13 +5237,13 @@
       <c r="BD38" s="51"/>
       <c r="BE38" s="51"/>
       <c r="BF38" s="51"/>
-      <c r="BG38" s="190"/>
+      <c r="BG38" s="163"/>
       <c r="BH38" s="55"/>
       <c r="BI38" s="55"/>
-      <c r="BJ38" s="190"/>
+      <c r="BJ38" s="163"/>
       <c r="BK38" s="55"/>
-      <c r="BL38" s="189"/>
-      <c r="BM38" s="189"/>
+      <c r="BL38" s="162"/>
+      <c r="BM38" s="162"/>
       <c r="BN38" s="51"/>
       <c r="BO38" s="51"/>
       <c r="BP38" s="56"/>
@@ -5257,15 +5255,15 @@
         <v>3.4</v>
       </c>
       <c r="C39" s="37" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D39" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="E39" s="183" t="s">
-        <v>89</v>
-      </c>
-      <c r="F39" s="172">
+        <v>72</v>
+      </c>
+      <c r="E39" s="156" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="147">
         <v>44474</v>
       </c>
       <c r="G39" s="38">
@@ -5328,25 +5326,25 @@
       <c r="BH39" s="55"/>
       <c r="BI39" s="55"/>
       <c r="BJ39" s="55"/>
-      <c r="BK39" s="190"/>
+      <c r="BK39" s="163"/>
       <c r="BL39" s="51"/>
-      <c r="BM39" s="189"/>
-      <c r="BN39" s="189"/>
-      <c r="BO39" s="189"/>
+      <c r="BM39" s="162"/>
+      <c r="BN39" s="162"/>
+      <c r="BO39" s="162"/>
       <c r="BP39" s="56"/>
       <c r="BQ39" s="36"/>
     </row>
     <row r="40" spans="1:69" ht="21" customHeight="1">
       <c r="A40" s="20"/>
-      <c r="B40" s="170">
+      <c r="B40" s="145">
         <v>4</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D40" s="31"/>
-      <c r="E40" s="181"/>
-      <c r="F40" s="170"/>
+      <c r="E40" s="154"/>
+      <c r="F40" s="145"/>
       <c r="G40" s="31"/>
       <c r="H40" s="31"/>
       <c r="I40" s="32"/>
@@ -5417,15 +5415,15 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="C41" s="37" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D41" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="E41" s="182">
+        <v>64</v>
+      </c>
+      <c r="E41" s="155">
         <v>44291</v>
       </c>
-      <c r="F41" s="171">
+      <c r="F41" s="146">
         <v>44291</v>
       </c>
       <c r="G41" s="38">
@@ -5491,9 +5489,9 @@
       <c r="BK41" s="46"/>
       <c r="BL41" s="91"/>
       <c r="BM41" s="91"/>
-      <c r="BN41" s="163"/>
+      <c r="BN41" s="139"/>
       <c r="BO41" s="91"/>
-      <c r="BP41" s="164"/>
+      <c r="BP41" s="140"/>
       <c r="BQ41" s="36"/>
     </row>
     <row r="42" spans="1:69" ht="21" customHeight="1">
@@ -5502,21 +5500,21 @@
         <v>4.2</v>
       </c>
       <c r="C42" s="75" t="s">
-        <v>54</v>
-      </c>
-      <c r="D42" s="134" t="s">
-        <v>67</v>
-      </c>
-      <c r="E42" s="185">
+        <v>51</v>
+      </c>
+      <c r="D42" s="132" t="s">
+        <v>64</v>
+      </c>
+      <c r="E42" s="158">
         <v>44260</v>
       </c>
-      <c r="F42" s="175">
+      <c r="F42" s="150">
         <v>44474</v>
       </c>
       <c r="G42" s="76">
         <v>1</v>
       </c>
-      <c r="H42" s="166">
+      <c r="H42" s="142">
         <v>1</v>
       </c>
       <c r="I42" s="20"/>
@@ -5575,10 +5573,10 @@
       <c r="BJ42" s="20"/>
       <c r="BK42" s="20"/>
       <c r="BL42" s="20"/>
-      <c r="BM42" s="165"/>
-      <c r="BN42" s="165"/>
-      <c r="BO42" s="165"/>
-      <c r="BP42" s="165"/>
+      <c r="BM42" s="141"/>
+      <c r="BN42" s="141"/>
+      <c r="BO42" s="141"/>
+      <c r="BP42" s="141"/>
       <c r="BQ42" s="20"/>
     </row>
     <row r="43" spans="1:69" ht="21" customHeight="1">
@@ -5586,7 +5584,7 @@
       <c r="B43" s="76"/>
       <c r="C43" s="20"/>
       <c r="D43" s="20"/>
-      <c r="E43" s="186"/>
+      <c r="E43" s="159"/>
       <c r="F43" s="76"/>
       <c r="G43" s="76"/>
       <c r="H43" s="76"/>
@@ -5654,24 +5652,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="BB8:BP8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="AM9:AQ9"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="O2:AE2"/>
@@ -5688,9 +5668,27 @@
     <mergeCell ref="P4:AB4"/>
     <mergeCell ref="P5:AA5"/>
     <mergeCell ref="I5:O5"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="BB8:BP8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="I9:M9"/>
   </mergeCells>
   <conditionalFormatting sqref="H12:H23 H30:H41 H25:H28">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5700,7 +5698,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12:H23 H30:H41 H25:H28">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>

<commit_message>
added report and ppt
</commit_message>
<xml_diff>
--- a/docs/Gantt chart.xlsx
+++ b/docs/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/connecture/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9270F0-09CF-1449-A991-14E5D0326571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821D427E-2396-0145-8B52-890305ABDA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,13 +302,23 @@
     </r>
   </si>
   <si>
-    <t>Module-1: Redux</t>
-  </si>
-  <si>
     <t>Module-2: Reducers</t>
   </si>
   <si>
-    <t>Module-3: Database Models</t>
+    <r>
+      <t xml:space="preserve">Module-1: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF434343"/>
+        <rFont val="Roboto"/>
+      </rPr>
+      <t>Actions</t>
+    </r>
+  </si>
+  <si>
+    <t>Module-3: Models</t>
   </si>
 </sst>
 </file>
@@ -1589,6 +1599,125 @@
     <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="44" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="45" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="42" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="46" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="46" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="26" fillId="38" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="38" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="40" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="41" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="42" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="43" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="38" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="49" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="54" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="55" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="54" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1599,14 +1728,9 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1624,120 +1748,6 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="42" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="46" fillId="38" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="46" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="26" fillId="38" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="38" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="40" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="41" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="42" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="43" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="38" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="49" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="49" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="54" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="55" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2066,8 +2076,8 @@
   </sheetPr>
   <dimension ref="A1:BQ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
@@ -2156,38 +2166,38 @@
     </row>
     <row r="2" spans="1:69" ht="32" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="148" t="s">
+      <c r="B2" s="193" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="147"/>
-      <c r="D2" s="147"/>
-      <c r="E2" s="147"/>
-      <c r="F2" s="147"/>
-      <c r="G2" s="147"/>
+      <c r="C2" s="192"/>
+      <c r="D2" s="192"/>
+      <c r="E2" s="192"/>
+      <c r="F2" s="192"/>
+      <c r="G2" s="192"/>
       <c r="H2" s="86"/>
-      <c r="I2" s="146"/>
-      <c r="J2" s="147"/>
-      <c r="K2" s="147"/>
-      <c r="L2" s="147"/>
-      <c r="M2" s="147"/>
-      <c r="N2" s="147"/>
-      <c r="O2" s="149"/>
-      <c r="P2" s="147"/>
-      <c r="Q2" s="147"/>
-      <c r="R2" s="147"/>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
-      <c r="V2" s="147"/>
-      <c r="W2" s="147"/>
-      <c r="X2" s="147"/>
-      <c r="Y2" s="147"/>
-      <c r="Z2" s="147"/>
-      <c r="AA2" s="147"/>
-      <c r="AB2" s="147"/>
-      <c r="AC2" s="147"/>
-      <c r="AD2" s="147"/>
-      <c r="AE2" s="147"/>
+      <c r="I2" s="191"/>
+      <c r="J2" s="192"/>
+      <c r="K2" s="192"/>
+      <c r="L2" s="192"/>
+      <c r="M2" s="192"/>
+      <c r="N2" s="192"/>
+      <c r="O2" s="194"/>
+      <c r="P2" s="192"/>
+      <c r="Q2" s="192"/>
+      <c r="R2" s="192"/>
+      <c r="S2" s="192"/>
+      <c r="T2" s="192"/>
+      <c r="U2" s="192"/>
+      <c r="V2" s="192"/>
+      <c r="W2" s="192"/>
+      <c r="X2" s="192"/>
+      <c r="Y2" s="192"/>
+      <c r="Z2" s="192"/>
+      <c r="AA2" s="192"/>
+      <c r="AB2" s="192"/>
+      <c r="AC2" s="192"/>
+      <c r="AD2" s="192"/>
+      <c r="AE2" s="192"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
       <c r="AH2" s="10"/>
@@ -2300,41 +2310,41 @@
     </row>
     <row r="4" spans="1:69" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="150" t="s">
+      <c r="B4" s="176" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="151"/>
-      <c r="D4" s="154" t="s">
+      <c r="C4" s="177"/>
+      <c r="D4" s="196" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="151"/>
-      <c r="F4" s="151"/>
-      <c r="G4" s="151"/>
+      <c r="E4" s="177"/>
+      <c r="F4" s="177"/>
+      <c r="G4" s="177"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="150" t="s">
+      <c r="I4" s="176" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="151"/>
-      <c r="K4" s="151"/>
-      <c r="L4" s="151"/>
-      <c r="M4" s="151"/>
-      <c r="N4" s="151"/>
-      <c r="O4" s="151"/>
-      <c r="P4" s="158" t="s">
+      <c r="J4" s="177"/>
+      <c r="K4" s="177"/>
+      <c r="L4" s="177"/>
+      <c r="M4" s="177"/>
+      <c r="N4" s="177"/>
+      <c r="O4" s="177"/>
+      <c r="P4" s="200" t="s">
         <v>74</v>
       </c>
-      <c r="Q4" s="151"/>
-      <c r="R4" s="151"/>
-      <c r="S4" s="151"/>
-      <c r="T4" s="151"/>
-      <c r="U4" s="151"/>
-      <c r="V4" s="151"/>
-      <c r="W4" s="151"/>
-      <c r="X4" s="151"/>
-      <c r="Y4" s="151"/>
-      <c r="Z4" s="151"/>
-      <c r="AA4" s="151"/>
-      <c r="AB4" s="151"/>
+      <c r="Q4" s="177"/>
+      <c r="R4" s="177"/>
+      <c r="S4" s="177"/>
+      <c r="T4" s="177"/>
+      <c r="U4" s="177"/>
+      <c r="V4" s="177"/>
+      <c r="W4" s="177"/>
+      <c r="X4" s="177"/>
+      <c r="Y4" s="177"/>
+      <c r="Z4" s="177"/>
+      <c r="AA4" s="177"/>
+      <c r="AB4" s="177"/>
       <c r="AC4" s="16"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -2379,40 +2389,40 @@
     </row>
     <row r="5" spans="1:69" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="150" t="s">
+      <c r="B5" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="151"/>
-      <c r="D5" s="170" t="s">
+      <c r="C5" s="177"/>
+      <c r="D5" s="178" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="151"/>
-      <c r="F5" s="151"/>
-      <c r="G5" s="151"/>
+      <c r="E5" s="177"/>
+      <c r="F5" s="177"/>
+      <c r="G5" s="177"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="150" t="s">
+      <c r="I5" s="176" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="151"/>
-      <c r="K5" s="151"/>
-      <c r="L5" s="151"/>
-      <c r="M5" s="151"/>
-      <c r="N5" s="151"/>
-      <c r="O5" s="151"/>
-      <c r="P5" s="159" t="s">
+      <c r="J5" s="177"/>
+      <c r="K5" s="177"/>
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="201" t="s">
         <v>75</v>
       </c>
-      <c r="Q5" s="151"/>
-      <c r="R5" s="151"/>
-      <c r="S5" s="151"/>
-      <c r="T5" s="151"/>
-      <c r="U5" s="151"/>
-      <c r="V5" s="151"/>
-      <c r="W5" s="151"/>
-      <c r="X5" s="151"/>
-      <c r="Y5" s="151"/>
-      <c r="Z5" s="151"/>
-      <c r="AA5" s="151"/>
+      <c r="Q5" s="177"/>
+      <c r="R5" s="177"/>
+      <c r="S5" s="177"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="W5" s="177"/>
+      <c r="X5" s="177"/>
+      <c r="Y5" s="177"/>
+      <c r="Z5" s="177"/>
+      <c r="AA5" s="177"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="1"/>
@@ -2600,201 +2610,201 @@
     </row>
     <row r="8" spans="1:69" ht="17.25" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="195" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="152" t="s">
+      <c r="C8" s="195" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="152" t="s">
+      <c r="D8" s="195" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="156" t="s">
+      <c r="E8" s="198" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="152" t="s">
+      <c r="F8" s="195" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="152" t="s">
+      <c r="G8" s="195" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="152" t="s">
+      <c r="H8" s="195" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="164" t="s">
+      <c r="I8" s="184" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="153"/>
-      <c r="K8" s="153"/>
-      <c r="L8" s="153"/>
-      <c r="M8" s="153"/>
-      <c r="N8" s="153"/>
-      <c r="O8" s="153"/>
-      <c r="P8" s="153"/>
-      <c r="Q8" s="153"/>
-      <c r="R8" s="153"/>
-      <c r="S8" s="153"/>
-      <c r="T8" s="153"/>
-      <c r="U8" s="153"/>
-      <c r="V8" s="153"/>
-      <c r="W8" s="153"/>
-      <c r="X8" s="165" t="s">
+      <c r="J8" s="185"/>
+      <c r="K8" s="185"/>
+      <c r="L8" s="185"/>
+      <c r="M8" s="185"/>
+      <c r="N8" s="185"/>
+      <c r="O8" s="185"/>
+      <c r="P8" s="185"/>
+      <c r="Q8" s="185"/>
+      <c r="R8" s="185"/>
+      <c r="S8" s="185"/>
+      <c r="T8" s="185"/>
+      <c r="U8" s="185"/>
+      <c r="V8" s="185"/>
+      <c r="W8" s="185"/>
+      <c r="X8" s="186" t="s">
         <v>11</v>
       </c>
-      <c r="Y8" s="153"/>
-      <c r="Z8" s="153"/>
-      <c r="AA8" s="153"/>
-      <c r="AB8" s="153"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="153"/>
-      <c r="AE8" s="153"/>
-      <c r="AF8" s="153"/>
-      <c r="AG8" s="153"/>
-      <c r="AH8" s="153"/>
-      <c r="AI8" s="153"/>
-      <c r="AJ8" s="153"/>
-      <c r="AK8" s="153"/>
-      <c r="AL8" s="153"/>
-      <c r="AM8" s="168" t="s">
+      <c r="Y8" s="185"/>
+      <c r="Z8" s="185"/>
+      <c r="AA8" s="185"/>
+      <c r="AB8" s="185"/>
+      <c r="AC8" s="185"/>
+      <c r="AD8" s="185"/>
+      <c r="AE8" s="185"/>
+      <c r="AF8" s="185"/>
+      <c r="AG8" s="185"/>
+      <c r="AH8" s="185"/>
+      <c r="AI8" s="185"/>
+      <c r="AJ8" s="185"/>
+      <c r="AK8" s="185"/>
+      <c r="AL8" s="185"/>
+      <c r="AM8" s="189" t="s">
         <v>12</v>
       </c>
-      <c r="AN8" s="153"/>
-      <c r="AO8" s="153"/>
-      <c r="AP8" s="153"/>
-      <c r="AQ8" s="153"/>
-      <c r="AR8" s="153"/>
-      <c r="AS8" s="153"/>
-      <c r="AT8" s="153"/>
-      <c r="AU8" s="153"/>
-      <c r="AV8" s="153"/>
-      <c r="AW8" s="153"/>
-      <c r="AX8" s="153"/>
-      <c r="AY8" s="153"/>
-      <c r="AZ8" s="153"/>
-      <c r="BA8" s="153"/>
-      <c r="BB8" s="166" t="s">
+      <c r="AN8" s="185"/>
+      <c r="AO8" s="185"/>
+      <c r="AP8" s="185"/>
+      <c r="AQ8" s="185"/>
+      <c r="AR8" s="185"/>
+      <c r="AS8" s="185"/>
+      <c r="AT8" s="185"/>
+      <c r="AU8" s="185"/>
+      <c r="AV8" s="185"/>
+      <c r="AW8" s="185"/>
+      <c r="AX8" s="185"/>
+      <c r="AY8" s="185"/>
+      <c r="AZ8" s="185"/>
+      <c r="BA8" s="185"/>
+      <c r="BB8" s="187" t="s">
         <v>13</v>
       </c>
-      <c r="BC8" s="153"/>
-      <c r="BD8" s="153"/>
-      <c r="BE8" s="153"/>
-      <c r="BF8" s="153"/>
-      <c r="BG8" s="153"/>
-      <c r="BH8" s="153"/>
-      <c r="BI8" s="153"/>
-      <c r="BJ8" s="153"/>
-      <c r="BK8" s="153"/>
-      <c r="BL8" s="153"/>
-      <c r="BM8" s="153"/>
-      <c r="BN8" s="153"/>
-      <c r="BO8" s="153"/>
-      <c r="BP8" s="167"/>
+      <c r="BC8" s="185"/>
+      <c r="BD8" s="185"/>
+      <c r="BE8" s="185"/>
+      <c r="BF8" s="185"/>
+      <c r="BG8" s="185"/>
+      <c r="BH8" s="185"/>
+      <c r="BI8" s="185"/>
+      <c r="BJ8" s="185"/>
+      <c r="BK8" s="185"/>
+      <c r="BL8" s="185"/>
+      <c r="BM8" s="185"/>
+      <c r="BN8" s="185"/>
+      <c r="BO8" s="185"/>
+      <c r="BP8" s="188"/>
       <c r="BQ8" s="20"/>
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="155"/>
-      <c r="C9" s="153"/>
-      <c r="D9" s="153"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="153"/>
-      <c r="H9" s="153"/>
-      <c r="I9" s="171" t="s">
+      <c r="B9" s="197"/>
+      <c r="C9" s="185"/>
+      <c r="D9" s="185"/>
+      <c r="E9" s="199"/>
+      <c r="F9" s="197"/>
+      <c r="G9" s="185"/>
+      <c r="H9" s="185"/>
+      <c r="I9" s="179" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="161"/>
-      <c r="K9" s="161"/>
-      <c r="L9" s="161"/>
-      <c r="M9" s="162"/>
-      <c r="N9" s="171" t="s">
+      <c r="J9" s="180"/>
+      <c r="K9" s="180"/>
+      <c r="L9" s="180"/>
+      <c r="M9" s="181"/>
+      <c r="N9" s="179" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="161"/>
-      <c r="P9" s="161"/>
-      <c r="Q9" s="161"/>
-      <c r="R9" s="162"/>
-      <c r="S9" s="171" t="s">
+      <c r="O9" s="180"/>
+      <c r="P9" s="180"/>
+      <c r="Q9" s="180"/>
+      <c r="R9" s="181"/>
+      <c r="S9" s="179" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="161"/>
-      <c r="U9" s="161"/>
-      <c r="V9" s="161"/>
-      <c r="W9" s="162"/>
-      <c r="X9" s="163" t="s">
+      <c r="T9" s="180"/>
+      <c r="U9" s="180"/>
+      <c r="V9" s="180"/>
+      <c r="W9" s="181"/>
+      <c r="X9" s="183" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="161"/>
-      <c r="Z9" s="161"/>
-      <c r="AA9" s="161"/>
-      <c r="AB9" s="162"/>
-      <c r="AC9" s="163" t="s">
+      <c r="Y9" s="180"/>
+      <c r="Z9" s="180"/>
+      <c r="AA9" s="180"/>
+      <c r="AB9" s="181"/>
+      <c r="AC9" s="183" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="161"/>
-      <c r="AE9" s="161"/>
-      <c r="AF9" s="161"/>
-      <c r="AG9" s="162"/>
-      <c r="AH9" s="163" t="s">
+      <c r="AD9" s="180"/>
+      <c r="AE9" s="180"/>
+      <c r="AF9" s="180"/>
+      <c r="AG9" s="181"/>
+      <c r="AH9" s="183" t="s">
         <v>19</v>
       </c>
-      <c r="AI9" s="161"/>
-      <c r="AJ9" s="161"/>
-      <c r="AK9" s="161"/>
-      <c r="AL9" s="162"/>
-      <c r="AM9" s="169" t="s">
+      <c r="AI9" s="180"/>
+      <c r="AJ9" s="180"/>
+      <c r="AK9" s="180"/>
+      <c r="AL9" s="181"/>
+      <c r="AM9" s="190" t="s">
         <v>20</v>
       </c>
-      <c r="AN9" s="161"/>
-      <c r="AO9" s="161"/>
-      <c r="AP9" s="161"/>
-      <c r="AQ9" s="162"/>
-      <c r="AR9" s="169" t="s">
+      <c r="AN9" s="180"/>
+      <c r="AO9" s="180"/>
+      <c r="AP9" s="180"/>
+      <c r="AQ9" s="181"/>
+      <c r="AR9" s="190" t="s">
         <v>21</v>
       </c>
-      <c r="AS9" s="161"/>
-      <c r="AT9" s="161"/>
-      <c r="AU9" s="161"/>
-      <c r="AV9" s="162"/>
-      <c r="AW9" s="169" t="s">
+      <c r="AS9" s="180"/>
+      <c r="AT9" s="180"/>
+      <c r="AU9" s="180"/>
+      <c r="AV9" s="181"/>
+      <c r="AW9" s="190" t="s">
         <v>22</v>
       </c>
-      <c r="AX9" s="161"/>
-      <c r="AY9" s="161"/>
-      <c r="AZ9" s="161"/>
-      <c r="BA9" s="162"/>
-      <c r="BB9" s="160" t="s">
+      <c r="AX9" s="180"/>
+      <c r="AY9" s="180"/>
+      <c r="AZ9" s="180"/>
+      <c r="BA9" s="181"/>
+      <c r="BB9" s="182" t="s">
         <v>23</v>
       </c>
-      <c r="BC9" s="161"/>
-      <c r="BD9" s="161"/>
-      <c r="BE9" s="161"/>
-      <c r="BF9" s="162"/>
-      <c r="BG9" s="160" t="s">
+      <c r="BC9" s="180"/>
+      <c r="BD9" s="180"/>
+      <c r="BE9" s="180"/>
+      <c r="BF9" s="181"/>
+      <c r="BG9" s="182" t="s">
         <v>24</v>
       </c>
-      <c r="BH9" s="161"/>
-      <c r="BI9" s="161"/>
-      <c r="BJ9" s="161"/>
-      <c r="BK9" s="162"/>
-      <c r="BL9" s="160" t="s">
+      <c r="BH9" s="180"/>
+      <c r="BI9" s="180"/>
+      <c r="BJ9" s="180"/>
+      <c r="BK9" s="181"/>
+      <c r="BL9" s="182" t="s">
         <v>25</v>
       </c>
-      <c r="BM9" s="161"/>
-      <c r="BN9" s="161"/>
-      <c r="BO9" s="161"/>
-      <c r="BP9" s="162"/>
+      <c r="BM9" s="180"/>
+      <c r="BN9" s="180"/>
+      <c r="BO9" s="180"/>
+      <c r="BP9" s="181"/>
       <c r="BQ9" s="24"/>
     </row>
     <row r="10" spans="1:69" ht="17.25" customHeight="1">
       <c r="A10" s="25"/>
-      <c r="B10" s="155"/>
-      <c r="C10" s="153"/>
-      <c r="D10" s="153"/>
-      <c r="E10" s="157"/>
-      <c r="F10" s="155"/>
-      <c r="G10" s="153"/>
-      <c r="H10" s="153"/>
+      <c r="B10" s="197"/>
+      <c r="C10" s="185"/>
+      <c r="D10" s="185"/>
+      <c r="E10" s="199"/>
+      <c r="F10" s="197"/>
+      <c r="G10" s="185"/>
+      <c r="H10" s="185"/>
       <c r="I10" s="26" t="s">
         <v>26</v>
       </c>
@@ -4131,7 +4141,7 @@
       <c r="AZ24" s="35"/>
       <c r="BA24" s="35"/>
       <c r="BB24" s="35"/>
-      <c r="BC24" s="200"/>
+      <c r="BC24" s="174"/>
       <c r="BD24" s="35"/>
       <c r="BE24" s="35"/>
       <c r="BF24" s="35"/>
@@ -4402,80 +4412,80 @@
       <c r="BP27" s="56"/>
       <c r="BQ27" s="36"/>
     </row>
-    <row r="28" spans="1:69" s="189" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
-      <c r="A28" s="172"/>
-      <c r="B28" s="173">
+    <row r="28" spans="1:69" s="163" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+      <c r="A28" s="146"/>
+      <c r="B28" s="147">
         <v>2.4</v>
       </c>
-      <c r="C28" s="174" t="s">
+      <c r="C28" s="148" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="175"/>
-      <c r="E28" s="176"/>
-      <c r="F28" s="177"/>
-      <c r="G28" s="178"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="180"/>
-      <c r="J28" s="181"/>
-      <c r="K28" s="182"/>
-      <c r="L28" s="182"/>
-      <c r="M28" s="182"/>
-      <c r="N28" s="183"/>
-      <c r="O28" s="183"/>
-      <c r="P28" s="183"/>
-      <c r="Q28" s="183"/>
-      <c r="R28" s="183"/>
-      <c r="S28" s="182"/>
-      <c r="T28" s="182"/>
-      <c r="U28" s="182"/>
-      <c r="V28" s="182"/>
-      <c r="W28" s="182"/>
-      <c r="X28" s="182"/>
-      <c r="Y28" s="182"/>
-      <c r="Z28" s="182"/>
-      <c r="AA28" s="182"/>
-      <c r="AB28" s="182"/>
-      <c r="AC28" s="184"/>
-      <c r="AD28" s="184"/>
-      <c r="AE28" s="184"/>
-      <c r="AF28" s="184"/>
-      <c r="AG28" s="184"/>
-      <c r="AH28" s="182"/>
-      <c r="AI28" s="182"/>
-      <c r="AJ28" s="182"/>
-      <c r="AK28" s="182"/>
-      <c r="AL28" s="182"/>
-      <c r="AM28" s="182"/>
-      <c r="AN28" s="182"/>
-      <c r="AO28" s="182"/>
-      <c r="AP28" s="182"/>
-      <c r="AQ28" s="182"/>
-      <c r="AR28" s="185"/>
-      <c r="AS28" s="185"/>
-      <c r="AT28" s="185"/>
-      <c r="AU28" s="185"/>
-      <c r="AV28" s="185"/>
-      <c r="AW28" s="182"/>
-      <c r="AX28" s="182"/>
-      <c r="AY28" s="182"/>
-      <c r="AZ28" s="182"/>
-      <c r="BA28" s="182"/>
-      <c r="BB28" s="182"/>
-      <c r="BC28" s="182"/>
-      <c r="BD28" s="182"/>
-      <c r="BE28" s="182"/>
-      <c r="BF28" s="182"/>
-      <c r="BG28" s="186"/>
-      <c r="BH28" s="186"/>
-      <c r="BI28" s="186"/>
-      <c r="BJ28" s="186"/>
-      <c r="BK28" s="186"/>
-      <c r="BL28" s="182"/>
-      <c r="BM28" s="182"/>
-      <c r="BN28" s="182"/>
-      <c r="BO28" s="182"/>
-      <c r="BP28" s="187"/>
-      <c r="BQ28" s="188"/>
+      <c r="D28" s="149"/>
+      <c r="E28" s="150"/>
+      <c r="F28" s="151"/>
+      <c r="G28" s="152"/>
+      <c r="H28" s="153"/>
+      <c r="I28" s="154"/>
+      <c r="J28" s="155"/>
+      <c r="K28" s="156"/>
+      <c r="L28" s="156"/>
+      <c r="M28" s="156"/>
+      <c r="N28" s="157"/>
+      <c r="O28" s="157"/>
+      <c r="P28" s="157"/>
+      <c r="Q28" s="157"/>
+      <c r="R28" s="157"/>
+      <c r="S28" s="156"/>
+      <c r="T28" s="156"/>
+      <c r="U28" s="156"/>
+      <c r="V28" s="156"/>
+      <c r="W28" s="156"/>
+      <c r="X28" s="156"/>
+      <c r="Y28" s="156"/>
+      <c r="Z28" s="156"/>
+      <c r="AA28" s="156"/>
+      <c r="AB28" s="156"/>
+      <c r="AC28" s="158"/>
+      <c r="AD28" s="158"/>
+      <c r="AE28" s="158"/>
+      <c r="AF28" s="158"/>
+      <c r="AG28" s="158"/>
+      <c r="AH28" s="156"/>
+      <c r="AI28" s="156"/>
+      <c r="AJ28" s="156"/>
+      <c r="AK28" s="156"/>
+      <c r="AL28" s="156"/>
+      <c r="AM28" s="156"/>
+      <c r="AN28" s="156"/>
+      <c r="AO28" s="156"/>
+      <c r="AP28" s="156"/>
+      <c r="AQ28" s="156"/>
+      <c r="AR28" s="159"/>
+      <c r="AS28" s="159"/>
+      <c r="AT28" s="159"/>
+      <c r="AU28" s="159"/>
+      <c r="AV28" s="159"/>
+      <c r="AW28" s="156"/>
+      <c r="AX28" s="156"/>
+      <c r="AY28" s="156"/>
+      <c r="AZ28" s="156"/>
+      <c r="BA28" s="156"/>
+      <c r="BB28" s="156"/>
+      <c r="BC28" s="156"/>
+      <c r="BD28" s="156"/>
+      <c r="BE28" s="156"/>
+      <c r="BF28" s="156"/>
+      <c r="BG28" s="160"/>
+      <c r="BH28" s="160"/>
+      <c r="BI28" s="160"/>
+      <c r="BJ28" s="160"/>
+      <c r="BK28" s="160"/>
+      <c r="BL28" s="156"/>
+      <c r="BM28" s="156"/>
+      <c r="BN28" s="156"/>
+      <c r="BO28" s="156"/>
+      <c r="BP28" s="161"/>
+      <c r="BQ28" s="162"/>
     </row>
     <row r="29" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A29" s="36"/>
@@ -4802,7 +4812,7 @@
       <c r="AY32" s="118"/>
       <c r="AZ32" s="118"/>
       <c r="BA32" s="118"/>
-      <c r="BB32" s="199"/>
+      <c r="BB32" s="173"/>
       <c r="BC32" s="69"/>
       <c r="BD32" s="105"/>
       <c r="BE32" s="105"/>
@@ -4840,7 +4850,7 @@
         <v>3</v>
       </c>
       <c r="H33" s="88">
-        <v>0.85</v>
+        <v>0.75</v>
       </c>
       <c r="I33" s="67"/>
       <c r="J33" s="68"/>
@@ -4884,9 +4894,9 @@
       <c r="AV33" s="123"/>
       <c r="AW33" s="118"/>
       <c r="AX33" s="105"/>
-      <c r="AY33" s="198"/>
+      <c r="AY33" s="172"/>
       <c r="AZ33" s="118"/>
-      <c r="BA33" s="201"/>
+      <c r="BA33" s="175"/>
       <c r="BB33" s="74"/>
       <c r="BC33" s="74"/>
       <c r="BD33" s="105"/>
@@ -5064,13 +5074,13 @@
       <c r="BP35" s="35"/>
       <c r="BQ35" s="20"/>
     </row>
-    <row r="36" spans="1:69" s="197" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+    <row r="36" spans="1:69" s="171" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
       <c r="A36" s="36"/>
       <c r="B36" s="38">
         <v>3.1</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>69</v>
@@ -5085,7 +5095,7 @@
         <v>2</v>
       </c>
       <c r="H36" s="39">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="I36" s="40"/>
       <c r="J36" s="41"/>
@@ -5149,13 +5159,13 @@
       <c r="BP36" s="47"/>
       <c r="BQ36" s="36"/>
     </row>
-    <row r="37" spans="1:69" s="197" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+    <row r="37" spans="1:69" s="171" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
       <c r="A37" s="36"/>
       <c r="B37" s="38">
         <v>3.2</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D37" s="37" t="s">
         <v>69</v>
@@ -5170,7 +5180,7 @@
         <v>2</v>
       </c>
       <c r="H37" s="39">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="I37" s="48"/>
       <c r="J37" s="49"/>
@@ -5234,7 +5244,7 @@
       <c r="BP37" s="56"/>
       <c r="BQ37" s="36"/>
     </row>
-    <row r="38" spans="1:69" s="197" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+    <row r="38" spans="1:69" s="171" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
       <c r="A38" s="36"/>
       <c r="B38" s="38">
         <v>3.3</v>
@@ -5255,7 +5265,7 @@
         <v>3</v>
       </c>
       <c r="H38" s="39">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="I38" s="48"/>
       <c r="J38" s="49"/>
@@ -5340,7 +5350,7 @@
         <v>3</v>
       </c>
       <c r="H39" s="87">
-        <v>0.98</v>
+        <v>0.95</v>
       </c>
       <c r="I39" s="48"/>
       <c r="J39" s="49"/>
@@ -5564,90 +5574,90 @@
       <c r="BP41" s="125"/>
       <c r="BQ41" s="36"/>
     </row>
-    <row r="42" spans="1:69" s="196" customFormat="1" ht="21" customHeight="1">
-      <c r="A42" s="190"/>
-      <c r="B42" s="191">
+    <row r="42" spans="1:69" s="170" customFormat="1" ht="21" customHeight="1">
+      <c r="A42" s="164"/>
+      <c r="B42" s="165">
         <v>4.2</v>
       </c>
-      <c r="C42" s="190" t="s">
+      <c r="C42" s="164" t="s">
         <v>88</v>
       </c>
-      <c r="D42" s="192" t="s">
+      <c r="D42" s="166" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="193">
+      <c r="E42" s="167">
         <v>44260</v>
       </c>
-      <c r="F42" s="193">
+      <c r="F42" s="167">
         <v>44474</v>
       </c>
-      <c r="G42" s="191">
+      <c r="G42" s="165">
         <v>1</v>
       </c>
-      <c r="H42" s="194">
+      <c r="H42" s="168">
         <v>1</v>
       </c>
-      <c r="I42" s="190"/>
-      <c r="J42" s="190"/>
-      <c r="K42" s="190"/>
-      <c r="L42" s="190"/>
-      <c r="M42" s="190"/>
-      <c r="N42" s="190"/>
-      <c r="O42" s="190"/>
-      <c r="P42" s="190"/>
-      <c r="Q42" s="190"/>
-      <c r="R42" s="190"/>
-      <c r="S42" s="190"/>
-      <c r="T42" s="190"/>
-      <c r="U42" s="190"/>
-      <c r="V42" s="190"/>
-      <c r="W42" s="190"/>
-      <c r="X42" s="190"/>
-      <c r="Y42" s="190"/>
-      <c r="Z42" s="190"/>
-      <c r="AA42" s="190"/>
-      <c r="AB42" s="190"/>
-      <c r="AC42" s="190"/>
-      <c r="AD42" s="190"/>
-      <c r="AE42" s="190"/>
-      <c r="AF42" s="190"/>
-      <c r="AG42" s="190"/>
-      <c r="AH42" s="190"/>
-      <c r="AI42" s="190"/>
-      <c r="AJ42" s="190"/>
-      <c r="AK42" s="190"/>
-      <c r="AL42" s="190"/>
-      <c r="AM42" s="190"/>
-      <c r="AN42" s="190"/>
-      <c r="AO42" s="190"/>
-      <c r="AP42" s="190"/>
-      <c r="AQ42" s="190"/>
-      <c r="AR42" s="190"/>
-      <c r="AS42" s="190"/>
-      <c r="AT42" s="190"/>
-      <c r="AU42" s="190"/>
-      <c r="AV42" s="190"/>
-      <c r="AW42" s="190"/>
-      <c r="AX42" s="190"/>
-      <c r="AY42" s="190"/>
-      <c r="AZ42" s="190"/>
-      <c r="BA42" s="190"/>
-      <c r="BB42" s="190"/>
-      <c r="BC42" s="190"/>
-      <c r="BD42" s="190"/>
-      <c r="BE42" s="190"/>
-      <c r="BF42" s="190"/>
-      <c r="BG42" s="190"/>
-      <c r="BH42" s="190"/>
-      <c r="BI42" s="190"/>
-      <c r="BJ42" s="190"/>
-      <c r="BK42" s="190"/>
-      <c r="BL42" s="190"/>
-      <c r="BM42" s="195"/>
-      <c r="BN42" s="195"/>
-      <c r="BO42" s="195"/>
-      <c r="BP42" s="195"/>
-      <c r="BQ42" s="190"/>
+      <c r="I42" s="164"/>
+      <c r="J42" s="164"/>
+      <c r="K42" s="164"/>
+      <c r="L42" s="164"/>
+      <c r="M42" s="164"/>
+      <c r="N42" s="164"/>
+      <c r="O42" s="164"/>
+      <c r="P42" s="164"/>
+      <c r="Q42" s="164"/>
+      <c r="R42" s="164"/>
+      <c r="S42" s="164"/>
+      <c r="T42" s="164"/>
+      <c r="U42" s="164"/>
+      <c r="V42" s="164"/>
+      <c r="W42" s="164"/>
+      <c r="X42" s="164"/>
+      <c r="Y42" s="164"/>
+      <c r="Z42" s="164"/>
+      <c r="AA42" s="164"/>
+      <c r="AB42" s="164"/>
+      <c r="AC42" s="164"/>
+      <c r="AD42" s="164"/>
+      <c r="AE42" s="164"/>
+      <c r="AF42" s="164"/>
+      <c r="AG42" s="164"/>
+      <c r="AH42" s="164"/>
+      <c r="AI42" s="164"/>
+      <c r="AJ42" s="164"/>
+      <c r="AK42" s="164"/>
+      <c r="AL42" s="164"/>
+      <c r="AM42" s="164"/>
+      <c r="AN42" s="164"/>
+      <c r="AO42" s="164"/>
+      <c r="AP42" s="164"/>
+      <c r="AQ42" s="164"/>
+      <c r="AR42" s="164"/>
+      <c r="AS42" s="164"/>
+      <c r="AT42" s="164"/>
+      <c r="AU42" s="164"/>
+      <c r="AV42" s="164"/>
+      <c r="AW42" s="164"/>
+      <c r="AX42" s="164"/>
+      <c r="AY42" s="164"/>
+      <c r="AZ42" s="164"/>
+      <c r="BA42" s="164"/>
+      <c r="BB42" s="164"/>
+      <c r="BC42" s="164"/>
+      <c r="BD42" s="164"/>
+      <c r="BE42" s="164"/>
+      <c r="BF42" s="164"/>
+      <c r="BG42" s="164"/>
+      <c r="BH42" s="164"/>
+      <c r="BI42" s="164"/>
+      <c r="BJ42" s="164"/>
+      <c r="BK42" s="164"/>
+      <c r="BL42" s="164"/>
+      <c r="BM42" s="169"/>
+      <c r="BN42" s="169"/>
+      <c r="BO42" s="169"/>
+      <c r="BP42" s="169"/>
+      <c r="BQ42" s="164"/>
     </row>
     <row r="43" spans="1:69" ht="21" customHeight="1">
       <c r="A43" s="20"/>
@@ -5722,24 +5732,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="I9:M9"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="BB8:BP8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="AM9:AQ9"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="O2:AE2"/>
@@ -5756,6 +5748,24 @@
     <mergeCell ref="P4:AB4"/>
     <mergeCell ref="P5:AA5"/>
     <mergeCell ref="I5:O5"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="BB8:BP8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="AM9:AQ9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="I9:M9"/>
   </mergeCells>
   <conditionalFormatting sqref="H12:H23 H30:H41 H25:H28">
     <cfRule type="colorScale" priority="26">

</xml_diff>

<commit_message>
updated docs and files
</commit_message>
<xml_diff>
--- a/docs/Gantt chart.xlsx
+++ b/docs/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jagdishnarkar/Documents/GitHub/connecture/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{821D427E-2396-0145-8B52-890305ABDA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C3FFC-D142-C347-B14F-3E5584571FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="89">
   <si>
     <t>PROJECT TITLE</t>
   </si>
@@ -235,9 +235,6 @@
     <t>2.4.5</t>
   </si>
   <si>
-    <t>Devansh</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -256,15 +253,9 @@
     <t>15/4/21</t>
   </si>
   <si>
-    <t>20/3/2021</t>
-  </si>
-  <si>
     <t>20/4/2021</t>
   </si>
   <si>
-    <t>11/5.2021</t>
-  </si>
-  <si>
     <t>17/4/2021</t>
   </si>
   <si>
@@ -275,9 +266,6 @@
   </si>
   <si>
     <t>Module-4: Navbar</t>
-  </si>
-  <si>
-    <t>Module-5: Posts</t>
   </si>
   <si>
     <t>Module-1: Landing, Login, and Register</t>
@@ -1174,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1526,7 +1514,6 @@
     <xf numFmtId="0" fontId="29" fillId="47" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="36" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1671,51 +1658,10 @@
     </xf>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="53" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="54" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="54" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="54" fillId="44" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1728,9 +1674,14 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1748,6 +1699,36 @@
     </xf>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2074,20 +2055,20 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BQ43"/>
+  <dimension ref="A1:BQ42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="57" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="K52" sqref="K52"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D24" zoomScale="108" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="131" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="130" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="27.5" customWidth="1"/>
-    <col min="5" max="5" width="16.6640625" style="139" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" style="131" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" style="138" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" style="130" customWidth="1"/>
     <col min="7" max="7" width="8.5" customWidth="1"/>
     <col min="9" max="68" width="3.5" customWidth="1"/>
     <col min="69" max="69" width="3.83203125" customWidth="1"/>
@@ -2095,11 +2076,11 @@
   <sheetData>
     <row r="1" spans="1:69" ht="13" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="143"/>
+      <c r="B1" s="142"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="132"/>
-      <c r="F1" s="126"/>
+      <c r="E1" s="131"/>
+      <c r="F1" s="125"/>
       <c r="G1" s="3"/>
       <c r="H1" s="2"/>
       <c r="I1" s="4"/>
@@ -2166,38 +2147,38 @@
     </row>
     <row r="2" spans="1:69" ht="32" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="193" t="s">
+      <c r="B2" s="175" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="192"/>
-      <c r="D2" s="192"/>
-      <c r="E2" s="192"/>
-      <c r="F2" s="192"/>
-      <c r="G2" s="192"/>
+      <c r="C2" s="174"/>
+      <c r="D2" s="174"/>
+      <c r="E2" s="174"/>
+      <c r="F2" s="174"/>
+      <c r="G2" s="174"/>
       <c r="H2" s="86"/>
-      <c r="I2" s="191"/>
-      <c r="J2" s="192"/>
-      <c r="K2" s="192"/>
-      <c r="L2" s="192"/>
-      <c r="M2" s="192"/>
-      <c r="N2" s="192"/>
-      <c r="O2" s="194"/>
-      <c r="P2" s="192"/>
-      <c r="Q2" s="192"/>
-      <c r="R2" s="192"/>
-      <c r="S2" s="192"/>
-      <c r="T2" s="192"/>
-      <c r="U2" s="192"/>
-      <c r="V2" s="192"/>
-      <c r="W2" s="192"/>
-      <c r="X2" s="192"/>
-      <c r="Y2" s="192"/>
-      <c r="Z2" s="192"/>
-      <c r="AA2" s="192"/>
-      <c r="AB2" s="192"/>
-      <c r="AC2" s="192"/>
-      <c r="AD2" s="192"/>
-      <c r="AE2" s="192"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="174"/>
+      <c r="K2" s="174"/>
+      <c r="L2" s="174"/>
+      <c r="M2" s="174"/>
+      <c r="N2" s="174"/>
+      <c r="O2" s="176"/>
+      <c r="P2" s="174"/>
+      <c r="Q2" s="174"/>
+      <c r="R2" s="174"/>
+      <c r="S2" s="174"/>
+      <c r="T2" s="174"/>
+      <c r="U2" s="174"/>
+      <c r="V2" s="174"/>
+      <c r="W2" s="174"/>
+      <c r="X2" s="174"/>
+      <c r="Y2" s="174"/>
+      <c r="Z2" s="174"/>
+      <c r="AA2" s="174"/>
+      <c r="AB2" s="174"/>
+      <c r="AC2" s="174"/>
+      <c r="AD2" s="174"/>
+      <c r="AE2" s="174"/>
       <c r="AF2" s="10"/>
       <c r="AG2" s="10"/>
       <c r="AH2" s="10"/>
@@ -2239,11 +2220,11 @@
     </row>
     <row r="3" spans="1:69" ht="21" customHeight="1">
       <c r="A3" s="1"/>
-      <c r="B3" s="144"/>
+      <c r="B3" s="143"/>
       <c r="C3" s="11"/>
       <c r="D3" s="12"/>
-      <c r="E3" s="133"/>
-      <c r="F3" s="127"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="126"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
       <c r="I3" s="13"/>
@@ -2310,41 +2291,41 @@
     </row>
     <row r="4" spans="1:69" ht="21" customHeight="1">
       <c r="A4" s="1"/>
-      <c r="B4" s="176" t="s">
+      <c r="B4" s="177" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="177"/>
-      <c r="D4" s="196" t="s">
+      <c r="C4" s="178"/>
+      <c r="D4" s="181" t="s">
         <v>57</v>
       </c>
-      <c r="E4" s="177"/>
-      <c r="F4" s="177"/>
-      <c r="G4" s="177"/>
+      <c r="E4" s="178"/>
+      <c r="F4" s="178"/>
+      <c r="G4" s="178"/>
       <c r="H4" s="15"/>
-      <c r="I4" s="176" t="s">
+      <c r="I4" s="177" t="s">
+        <v>72</v>
+      </c>
+      <c r="J4" s="178"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="178"/>
+      <c r="N4" s="178"/>
+      <c r="O4" s="178"/>
+      <c r="P4" s="185" t="s">
         <v>73</v>
       </c>
-      <c r="J4" s="177"/>
-      <c r="K4" s="177"/>
-      <c r="L4" s="177"/>
-      <c r="M4" s="177"/>
-      <c r="N4" s="177"/>
-      <c r="O4" s="177"/>
-      <c r="P4" s="200" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="177"/>
-      <c r="S4" s="177"/>
-      <c r="T4" s="177"/>
-      <c r="U4" s="177"/>
-      <c r="V4" s="177"/>
-      <c r="W4" s="177"/>
-      <c r="X4" s="177"/>
-      <c r="Y4" s="177"/>
-      <c r="Z4" s="177"/>
-      <c r="AA4" s="177"/>
-      <c r="AB4" s="177"/>
+      <c r="Q4" s="178"/>
+      <c r="R4" s="178"/>
+      <c r="S4" s="178"/>
+      <c r="T4" s="178"/>
+      <c r="U4" s="178"/>
+      <c r="V4" s="178"/>
+      <c r="W4" s="178"/>
+      <c r="X4" s="178"/>
+      <c r="Y4" s="178"/>
+      <c r="Z4" s="178"/>
+      <c r="AA4" s="178"/>
+      <c r="AB4" s="178"/>
       <c r="AC4" s="16"/>
       <c r="AD4" s="9"/>
       <c r="AE4" s="9"/>
@@ -2389,40 +2370,40 @@
     </row>
     <row r="5" spans="1:69" ht="21" customHeight="1">
       <c r="A5" s="1"/>
-      <c r="B5" s="176" t="s">
+      <c r="B5" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="177"/>
-      <c r="D5" s="178" t="s">
+      <c r="C5" s="178"/>
+      <c r="D5" s="197" t="s">
         <v>58</v>
       </c>
-      <c r="E5" s="177"/>
-      <c r="F5" s="177"/>
-      <c r="G5" s="177"/>
+      <c r="E5" s="178"/>
+      <c r="F5" s="178"/>
+      <c r="G5" s="178"/>
       <c r="H5" s="17"/>
-      <c r="I5" s="176" t="s">
+      <c r="I5" s="177" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="177"/>
-      <c r="K5" s="177"/>
-      <c r="L5" s="177"/>
-      <c r="M5" s="177"/>
-      <c r="N5" s="177"/>
-      <c r="O5" s="177"/>
-      <c r="P5" s="201" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q5" s="177"/>
-      <c r="R5" s="177"/>
-      <c r="S5" s="177"/>
-      <c r="T5" s="177"/>
-      <c r="U5" s="177"/>
-      <c r="V5" s="177"/>
-      <c r="W5" s="177"/>
-      <c r="X5" s="177"/>
-      <c r="Y5" s="177"/>
-      <c r="Z5" s="177"/>
-      <c r="AA5" s="177"/>
+      <c r="J5" s="178"/>
+      <c r="K5" s="178"/>
+      <c r="L5" s="178"/>
+      <c r="M5" s="178"/>
+      <c r="N5" s="178"/>
+      <c r="O5" s="178"/>
+      <c r="P5" s="186" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="178"/>
+      <c r="S5" s="178"/>
+      <c r="T5" s="178"/>
+      <c r="U5" s="178"/>
+      <c r="V5" s="178"/>
+      <c r="W5" s="178"/>
+      <c r="X5" s="178"/>
+      <c r="Y5" s="178"/>
+      <c r="Z5" s="178"/>
+      <c r="AA5" s="178"/>
       <c r="AB5" s="18"/>
       <c r="AC5" s="16"/>
       <c r="AD5" s="1"/>
@@ -2471,7 +2452,7 @@
       <c r="B6" s="22"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="134"/>
+      <c r="E6" s="133"/>
       <c r="F6" s="22"/>
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
@@ -2542,7 +2523,7 @@
       <c r="B7" s="22"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="134"/>
+      <c r="E7" s="133"/>
       <c r="F7" s="22"/>
       <c r="G7" s="22"/>
       <c r="H7" s="22"/>
@@ -2610,201 +2591,201 @@
     </row>
     <row r="8" spans="1:69" ht="17.25" customHeight="1">
       <c r="A8" s="23"/>
-      <c r="B8" s="195" t="s">
+      <c r="B8" s="179" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="195" t="s">
+      <c r="C8" s="179" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="195" t="s">
+      <c r="D8" s="179" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="198" t="s">
+      <c r="E8" s="183" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="195" t="s">
+      <c r="F8" s="179" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="195" t="s">
+      <c r="G8" s="179" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="195" t="s">
+      <c r="H8" s="179" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="184" t="s">
+      <c r="I8" s="191" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="185"/>
-      <c r="K8" s="185"/>
-      <c r="L8" s="185"/>
-      <c r="M8" s="185"/>
-      <c r="N8" s="185"/>
-      <c r="O8" s="185"/>
-      <c r="P8" s="185"/>
-      <c r="Q8" s="185"/>
-      <c r="R8" s="185"/>
-      <c r="S8" s="185"/>
-      <c r="T8" s="185"/>
-      <c r="U8" s="185"/>
-      <c r="V8" s="185"/>
-      <c r="W8" s="185"/>
-      <c r="X8" s="186" t="s">
+      <c r="J8" s="180"/>
+      <c r="K8" s="180"/>
+      <c r="L8" s="180"/>
+      <c r="M8" s="180"/>
+      <c r="N8" s="180"/>
+      <c r="O8" s="180"/>
+      <c r="P8" s="180"/>
+      <c r="Q8" s="180"/>
+      <c r="R8" s="180"/>
+      <c r="S8" s="180"/>
+      <c r="T8" s="180"/>
+      <c r="U8" s="180"/>
+      <c r="V8" s="180"/>
+      <c r="W8" s="180"/>
+      <c r="X8" s="192" t="s">
         <v>11</v>
       </c>
-      <c r="Y8" s="185"/>
-      <c r="Z8" s="185"/>
-      <c r="AA8" s="185"/>
-      <c r="AB8" s="185"/>
-      <c r="AC8" s="185"/>
-      <c r="AD8" s="185"/>
-      <c r="AE8" s="185"/>
-      <c r="AF8" s="185"/>
-      <c r="AG8" s="185"/>
-      <c r="AH8" s="185"/>
-      <c r="AI8" s="185"/>
-      <c r="AJ8" s="185"/>
-      <c r="AK8" s="185"/>
-      <c r="AL8" s="185"/>
-      <c r="AM8" s="189" t="s">
+      <c r="Y8" s="180"/>
+      <c r="Z8" s="180"/>
+      <c r="AA8" s="180"/>
+      <c r="AB8" s="180"/>
+      <c r="AC8" s="180"/>
+      <c r="AD8" s="180"/>
+      <c r="AE8" s="180"/>
+      <c r="AF8" s="180"/>
+      <c r="AG8" s="180"/>
+      <c r="AH8" s="180"/>
+      <c r="AI8" s="180"/>
+      <c r="AJ8" s="180"/>
+      <c r="AK8" s="180"/>
+      <c r="AL8" s="180"/>
+      <c r="AM8" s="195" t="s">
         <v>12</v>
       </c>
-      <c r="AN8" s="185"/>
-      <c r="AO8" s="185"/>
-      <c r="AP8" s="185"/>
-      <c r="AQ8" s="185"/>
-      <c r="AR8" s="185"/>
-      <c r="AS8" s="185"/>
-      <c r="AT8" s="185"/>
-      <c r="AU8" s="185"/>
-      <c r="AV8" s="185"/>
-      <c r="AW8" s="185"/>
-      <c r="AX8" s="185"/>
-      <c r="AY8" s="185"/>
-      <c r="AZ8" s="185"/>
-      <c r="BA8" s="185"/>
-      <c r="BB8" s="187" t="s">
+      <c r="AN8" s="180"/>
+      <c r="AO8" s="180"/>
+      <c r="AP8" s="180"/>
+      <c r="AQ8" s="180"/>
+      <c r="AR8" s="180"/>
+      <c r="AS8" s="180"/>
+      <c r="AT8" s="180"/>
+      <c r="AU8" s="180"/>
+      <c r="AV8" s="180"/>
+      <c r="AW8" s="180"/>
+      <c r="AX8" s="180"/>
+      <c r="AY8" s="180"/>
+      <c r="AZ8" s="180"/>
+      <c r="BA8" s="180"/>
+      <c r="BB8" s="193" t="s">
         <v>13</v>
       </c>
-      <c r="BC8" s="185"/>
-      <c r="BD8" s="185"/>
-      <c r="BE8" s="185"/>
-      <c r="BF8" s="185"/>
-      <c r="BG8" s="185"/>
-      <c r="BH8" s="185"/>
-      <c r="BI8" s="185"/>
-      <c r="BJ8" s="185"/>
-      <c r="BK8" s="185"/>
-      <c r="BL8" s="185"/>
-      <c r="BM8" s="185"/>
-      <c r="BN8" s="185"/>
-      <c r="BO8" s="185"/>
-      <c r="BP8" s="188"/>
+      <c r="BC8" s="180"/>
+      <c r="BD8" s="180"/>
+      <c r="BE8" s="180"/>
+      <c r="BF8" s="180"/>
+      <c r="BG8" s="180"/>
+      <c r="BH8" s="180"/>
+      <c r="BI8" s="180"/>
+      <c r="BJ8" s="180"/>
+      <c r="BK8" s="180"/>
+      <c r="BL8" s="180"/>
+      <c r="BM8" s="180"/>
+      <c r="BN8" s="180"/>
+      <c r="BO8" s="180"/>
+      <c r="BP8" s="194"/>
       <c r="BQ8" s="20"/>
     </row>
     <row r="9" spans="1:69" ht="17.25" customHeight="1">
       <c r="A9" s="24"/>
-      <c r="B9" s="197"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="199"/>
-      <c r="F9" s="197"/>
-      <c r="G9" s="185"/>
-      <c r="H9" s="185"/>
-      <c r="I9" s="179" t="s">
+      <c r="B9" s="182"/>
+      <c r="C9" s="180"/>
+      <c r="D9" s="180"/>
+      <c r="E9" s="184"/>
+      <c r="F9" s="182"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="180"/>
+      <c r="I9" s="198" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="180"/>
-      <c r="K9" s="180"/>
-      <c r="L9" s="180"/>
-      <c r="M9" s="181"/>
-      <c r="N9" s="179" t="s">
+      <c r="J9" s="188"/>
+      <c r="K9" s="188"/>
+      <c r="L9" s="188"/>
+      <c r="M9" s="189"/>
+      <c r="N9" s="198" t="s">
         <v>15</v>
       </c>
-      <c r="O9" s="180"/>
-      <c r="P9" s="180"/>
-      <c r="Q9" s="180"/>
-      <c r="R9" s="181"/>
-      <c r="S9" s="179" t="s">
+      <c r="O9" s="188"/>
+      <c r="P9" s="188"/>
+      <c r="Q9" s="188"/>
+      <c r="R9" s="189"/>
+      <c r="S9" s="198" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="180"/>
-      <c r="U9" s="180"/>
-      <c r="V9" s="180"/>
-      <c r="W9" s="181"/>
-      <c r="X9" s="183" t="s">
+      <c r="T9" s="188"/>
+      <c r="U9" s="188"/>
+      <c r="V9" s="188"/>
+      <c r="W9" s="189"/>
+      <c r="X9" s="190" t="s">
         <v>17</v>
       </c>
-      <c r="Y9" s="180"/>
-      <c r="Z9" s="180"/>
-      <c r="AA9" s="180"/>
-      <c r="AB9" s="181"/>
-      <c r="AC9" s="183" t="s">
+      <c r="Y9" s="188"/>
+      <c r="Z9" s="188"/>
+      <c r="AA9" s="188"/>
+      <c r="AB9" s="189"/>
+      <c r="AC9" s="190" t="s">
         <v>18</v>
       </c>
-      <c r="AD9" s="180"/>
-      <c r="AE9" s="180"/>
-      <c r="AF9" s="180"/>
-      <c r="AG9" s="181"/>
-      <c r="AH9" s="183" t="s">
+      <c r="AD9" s="188"/>
+      <c r="AE9" s="188"/>
+      <c r="AF9" s="188"/>
+      <c r="AG9" s="189"/>
+      <c r="AH9" s="190" t="s">
         <v>19</v>
       </c>
-      <c r="AI9" s="180"/>
-      <c r="AJ9" s="180"/>
-      <c r="AK9" s="180"/>
-      <c r="AL9" s="181"/>
-      <c r="AM9" s="190" t="s">
+      <c r="AI9" s="188"/>
+      <c r="AJ9" s="188"/>
+      <c r="AK9" s="188"/>
+      <c r="AL9" s="189"/>
+      <c r="AM9" s="196" t="s">
         <v>20</v>
       </c>
-      <c r="AN9" s="180"/>
-      <c r="AO9" s="180"/>
-      <c r="AP9" s="180"/>
-      <c r="AQ9" s="181"/>
-      <c r="AR9" s="190" t="s">
+      <c r="AN9" s="188"/>
+      <c r="AO9" s="188"/>
+      <c r="AP9" s="188"/>
+      <c r="AQ9" s="189"/>
+      <c r="AR9" s="196" t="s">
         <v>21</v>
       </c>
-      <c r="AS9" s="180"/>
-      <c r="AT9" s="180"/>
-      <c r="AU9" s="180"/>
-      <c r="AV9" s="181"/>
-      <c r="AW9" s="190" t="s">
+      <c r="AS9" s="188"/>
+      <c r="AT9" s="188"/>
+      <c r="AU9" s="188"/>
+      <c r="AV9" s="189"/>
+      <c r="AW9" s="196" t="s">
         <v>22</v>
       </c>
-      <c r="AX9" s="180"/>
-      <c r="AY9" s="180"/>
-      <c r="AZ9" s="180"/>
-      <c r="BA9" s="181"/>
-      <c r="BB9" s="182" t="s">
+      <c r="AX9" s="188"/>
+      <c r="AY9" s="188"/>
+      <c r="AZ9" s="188"/>
+      <c r="BA9" s="189"/>
+      <c r="BB9" s="187" t="s">
         <v>23</v>
       </c>
-      <c r="BC9" s="180"/>
-      <c r="BD9" s="180"/>
-      <c r="BE9" s="180"/>
-      <c r="BF9" s="181"/>
-      <c r="BG9" s="182" t="s">
+      <c r="BC9" s="188"/>
+      <c r="BD9" s="188"/>
+      <c r="BE9" s="188"/>
+      <c r="BF9" s="189"/>
+      <c r="BG9" s="187" t="s">
         <v>24</v>
       </c>
-      <c r="BH9" s="180"/>
-      <c r="BI9" s="180"/>
-      <c r="BJ9" s="180"/>
-      <c r="BK9" s="181"/>
-      <c r="BL9" s="182" t="s">
+      <c r="BH9" s="188"/>
+      <c r="BI9" s="188"/>
+      <c r="BJ9" s="188"/>
+      <c r="BK9" s="189"/>
+      <c r="BL9" s="187" t="s">
         <v>25</v>
       </c>
-      <c r="BM9" s="180"/>
-      <c r="BN9" s="180"/>
-      <c r="BO9" s="180"/>
-      <c r="BP9" s="181"/>
+      <c r="BM9" s="188"/>
+      <c r="BN9" s="188"/>
+      <c r="BO9" s="188"/>
+      <c r="BP9" s="189"/>
       <c r="BQ9" s="24"/>
     </row>
     <row r="10" spans="1:69" ht="17.25" customHeight="1">
       <c r="A10" s="25"/>
-      <c r="B10" s="197"/>
-      <c r="C10" s="185"/>
-      <c r="D10" s="185"/>
-      <c r="E10" s="199"/>
-      <c r="F10" s="197"/>
-      <c r="G10" s="185"/>
-      <c r="H10" s="185"/>
+      <c r="B10" s="182"/>
+      <c r="C10" s="180"/>
+      <c r="D10" s="180"/>
+      <c r="E10" s="184"/>
+      <c r="F10" s="182"/>
+      <c r="G10" s="180"/>
+      <c r="H10" s="180"/>
       <c r="I10" s="26" t="s">
         <v>26</v>
       </c>
@@ -2989,15 +2970,15 @@
     </row>
     <row r="11" spans="1:69" ht="21" customHeight="1">
       <c r="A11" s="20"/>
-      <c r="B11" s="128">
+      <c r="B11" s="127">
         <v>1</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>31</v>
       </c>
       <c r="D11" s="31"/>
-      <c r="E11" s="135"/>
-      <c r="F11" s="128"/>
+      <c r="E11" s="134"/>
+      <c r="F11" s="127"/>
       <c r="G11" s="31"/>
       <c r="H11" s="31"/>
       <c r="I11" s="32"/>
@@ -3073,10 +3054,10 @@
       <c r="D12" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="136">
+      <c r="E12" s="135">
         <v>43961</v>
       </c>
-      <c r="F12" s="129">
+      <c r="F12" s="128">
         <v>44023</v>
       </c>
       <c r="G12" s="38">
@@ -3158,10 +3139,10 @@
       <c r="D13" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="136">
+      <c r="E13" s="135">
         <v>44023</v>
       </c>
-      <c r="F13" s="129">
+      <c r="F13" s="128">
         <v>44023</v>
       </c>
       <c r="G13" s="38">
@@ -3243,10 +3224,10 @@
       <c r="D14" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="136" t="s">
+      <c r="E14" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="F14" s="129" t="s">
+      <c r="F14" s="128" t="s">
         <v>66</v>
       </c>
       <c r="G14" s="38">
@@ -3328,10 +3309,10 @@
       <c r="D15" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="136" t="s">
+      <c r="E15" s="135" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="129" t="s">
+      <c r="F15" s="128" t="s">
         <v>66</v>
       </c>
       <c r="G15" s="38">
@@ -3413,10 +3394,10 @@
       <c r="D16" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="136">
+      <c r="E16" s="135">
         <v>44115</v>
       </c>
-      <c r="F16" s="129" t="s">
+      <c r="F16" s="128" t="s">
         <v>66</v>
       </c>
       <c r="G16" s="38">
@@ -3498,10 +3479,10 @@
       <c r="D17" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="136">
+      <c r="E17" s="135">
         <v>44115</v>
       </c>
-      <c r="F17" s="129" t="s">
+      <c r="F17" s="128" t="s">
         <v>66</v>
       </c>
       <c r="G17" s="38">
@@ -3583,10 +3564,10 @@
       <c r="D18" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="136">
+      <c r="E18" s="135">
         <v>44115</v>
       </c>
-      <c r="F18" s="129" t="s">
+      <c r="F18" s="128" t="s">
         <v>66</v>
       </c>
       <c r="G18" s="59">
@@ -3668,10 +3649,10 @@
       <c r="D19" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="137">
+      <c r="E19" s="136">
         <v>44115</v>
       </c>
-      <c r="F19" s="129" t="s">
+      <c r="F19" s="128" t="s">
         <v>66</v>
       </c>
       <c r="G19" s="59">
@@ -3753,10 +3734,10 @@
       <c r="D20" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="137">
+      <c r="E20" s="136">
         <v>44116</v>
       </c>
-      <c r="F20" s="130" t="s">
+      <c r="F20" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G20" s="59">
@@ -3838,10 +3819,10 @@
       <c r="D21" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E21" s="137">
+      <c r="E21" s="136">
         <v>44115</v>
       </c>
-      <c r="F21" s="130" t="s">
+      <c r="F21" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G21" s="59">
@@ -3923,10 +3904,10 @@
       <c r="D22" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="137">
+      <c r="E22" s="136">
         <v>44115</v>
       </c>
-      <c r="F22" s="130" t="s">
+      <c r="F22" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G22" s="59">
@@ -3999,7 +3980,7 @@
     </row>
     <row r="23" spans="1:69" ht="16.5" customHeight="1" outlineLevel="1">
       <c r="A23" s="36"/>
-      <c r="B23" s="145">
+      <c r="B23" s="144">
         <v>1.1100000000000001</v>
       </c>
       <c r="C23" s="58" t="s">
@@ -4008,10 +3989,10 @@
       <c r="D23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="137">
+      <c r="E23" s="136">
         <v>44115</v>
       </c>
-      <c r="F23" s="130" t="s">
+      <c r="F23" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G23" s="59">
@@ -4084,15 +4065,15 @@
     </row>
     <row r="24" spans="1:69" ht="21" customHeight="1">
       <c r="A24" s="20"/>
-      <c r="B24" s="128">
+      <c r="B24" s="127">
         <v>2</v>
       </c>
       <c r="C24" s="30" t="s">
         <v>42</v>
       </c>
       <c r="D24" s="31"/>
-      <c r="E24" s="135"/>
-      <c r="F24" s="128"/>
+      <c r="E24" s="134"/>
+      <c r="F24" s="127"/>
       <c r="G24" s="31"/>
       <c r="H24" s="31"/>
       <c r="I24" s="32"/>
@@ -4141,7 +4122,7 @@
       <c r="AZ24" s="35"/>
       <c r="BA24" s="35"/>
       <c r="BB24" s="35"/>
-      <c r="BC24" s="174"/>
+      <c r="BC24" s="172"/>
       <c r="BD24" s="35"/>
       <c r="BE24" s="35"/>
       <c r="BF24" s="35"/>
@@ -4168,10 +4149,10 @@
       <c r="D25" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E25" s="137">
+      <c r="E25" s="136">
         <v>44115</v>
       </c>
-      <c r="F25" s="130" t="s">
+      <c r="F25" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G25" s="38">
@@ -4253,10 +4234,10 @@
       <c r="D26" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E26" s="137">
+      <c r="E26" s="136">
         <v>44115</v>
       </c>
-      <c r="F26" s="130" t="s">
+      <c r="F26" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G26" s="38">
@@ -4338,10 +4319,10 @@
       <c r="D27" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="E27" s="137">
+      <c r="E27" s="136">
         <v>44115</v>
       </c>
-      <c r="F27" s="130" t="s">
+      <c r="F27" s="129" t="s">
         <v>67</v>
       </c>
       <c r="G27" s="38">
@@ -4412,80 +4393,80 @@
       <c r="BP27" s="56"/>
       <c r="BQ27" s="36"/>
     </row>
-    <row r="28" spans="1:69" s="163" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
-      <c r="A28" s="146"/>
-      <c r="B28" s="147">
+    <row r="28" spans="1:69" s="162" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+      <c r="A28" s="145"/>
+      <c r="B28" s="146">
         <v>2.4</v>
       </c>
-      <c r="C28" s="148" t="s">
+      <c r="C28" s="147" t="s">
         <v>45</v>
       </c>
-      <c r="D28" s="149"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="151"/>
-      <c r="G28" s="152"/>
-      <c r="H28" s="153"/>
-      <c r="I28" s="154"/>
-      <c r="J28" s="155"/>
-      <c r="K28" s="156"/>
-      <c r="L28" s="156"/>
-      <c r="M28" s="156"/>
-      <c r="N28" s="157"/>
-      <c r="O28" s="157"/>
-      <c r="P28" s="157"/>
-      <c r="Q28" s="157"/>
-      <c r="R28" s="157"/>
-      <c r="S28" s="156"/>
-      <c r="T28" s="156"/>
-      <c r="U28" s="156"/>
-      <c r="V28" s="156"/>
-      <c r="W28" s="156"/>
-      <c r="X28" s="156"/>
-      <c r="Y28" s="156"/>
-      <c r="Z28" s="156"/>
-      <c r="AA28" s="156"/>
-      <c r="AB28" s="156"/>
-      <c r="AC28" s="158"/>
-      <c r="AD28" s="158"/>
-      <c r="AE28" s="158"/>
-      <c r="AF28" s="158"/>
-      <c r="AG28" s="158"/>
-      <c r="AH28" s="156"/>
-      <c r="AI28" s="156"/>
-      <c r="AJ28" s="156"/>
-      <c r="AK28" s="156"/>
-      <c r="AL28" s="156"/>
-      <c r="AM28" s="156"/>
-      <c r="AN28" s="156"/>
-      <c r="AO28" s="156"/>
-      <c r="AP28" s="156"/>
-      <c r="AQ28" s="156"/>
-      <c r="AR28" s="159"/>
-      <c r="AS28" s="159"/>
-      <c r="AT28" s="159"/>
-      <c r="AU28" s="159"/>
-      <c r="AV28" s="159"/>
-      <c r="AW28" s="156"/>
-      <c r="AX28" s="156"/>
-      <c r="AY28" s="156"/>
-      <c r="AZ28" s="156"/>
-      <c r="BA28" s="156"/>
-      <c r="BB28" s="156"/>
-      <c r="BC28" s="156"/>
-      <c r="BD28" s="156"/>
-      <c r="BE28" s="156"/>
-      <c r="BF28" s="156"/>
-      <c r="BG28" s="160"/>
-      <c r="BH28" s="160"/>
-      <c r="BI28" s="160"/>
-      <c r="BJ28" s="160"/>
-      <c r="BK28" s="160"/>
-      <c r="BL28" s="156"/>
-      <c r="BM28" s="156"/>
-      <c r="BN28" s="156"/>
-      <c r="BO28" s="156"/>
-      <c r="BP28" s="161"/>
-      <c r="BQ28" s="162"/>
+      <c r="D28" s="148"/>
+      <c r="E28" s="149"/>
+      <c r="F28" s="150"/>
+      <c r="G28" s="151"/>
+      <c r="H28" s="152"/>
+      <c r="I28" s="153"/>
+      <c r="J28" s="154"/>
+      <c r="K28" s="155"/>
+      <c r="L28" s="155"/>
+      <c r="M28" s="155"/>
+      <c r="N28" s="156"/>
+      <c r="O28" s="156"/>
+      <c r="P28" s="156"/>
+      <c r="Q28" s="156"/>
+      <c r="R28" s="156"/>
+      <c r="S28" s="155"/>
+      <c r="T28" s="155"/>
+      <c r="U28" s="155"/>
+      <c r="V28" s="155"/>
+      <c r="W28" s="155"/>
+      <c r="X28" s="155"/>
+      <c r="Y28" s="155"/>
+      <c r="Z28" s="155"/>
+      <c r="AA28" s="155"/>
+      <c r="AB28" s="155"/>
+      <c r="AC28" s="157"/>
+      <c r="AD28" s="157"/>
+      <c r="AE28" s="157"/>
+      <c r="AF28" s="157"/>
+      <c r="AG28" s="157"/>
+      <c r="AH28" s="155"/>
+      <c r="AI28" s="155"/>
+      <c r="AJ28" s="155"/>
+      <c r="AK28" s="155"/>
+      <c r="AL28" s="155"/>
+      <c r="AM28" s="155"/>
+      <c r="AN28" s="155"/>
+      <c r="AO28" s="155"/>
+      <c r="AP28" s="155"/>
+      <c r="AQ28" s="155"/>
+      <c r="AR28" s="158"/>
+      <c r="AS28" s="158"/>
+      <c r="AT28" s="158"/>
+      <c r="AU28" s="158"/>
+      <c r="AV28" s="158"/>
+      <c r="AW28" s="155"/>
+      <c r="AX28" s="155"/>
+      <c r="AY28" s="155"/>
+      <c r="AZ28" s="155"/>
+      <c r="BA28" s="155"/>
+      <c r="BB28" s="155"/>
+      <c r="BC28" s="155"/>
+      <c r="BD28" s="155"/>
+      <c r="BE28" s="155"/>
+      <c r="BF28" s="155"/>
+      <c r="BG28" s="159"/>
+      <c r="BH28" s="159"/>
+      <c r="BI28" s="159"/>
+      <c r="BJ28" s="159"/>
+      <c r="BK28" s="159"/>
+      <c r="BL28" s="155"/>
+      <c r="BM28" s="155"/>
+      <c r="BN28" s="155"/>
+      <c r="BO28" s="155"/>
+      <c r="BP28" s="160"/>
+      <c r="BQ28" s="161"/>
     </row>
     <row r="29" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A29" s="36"/>
@@ -4493,15 +4474,15 @@
         <v>51</v>
       </c>
       <c r="C29" s="58" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D29" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E29" s="137" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="130">
+      <c r="E29" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="F29" s="129">
         <v>44319</v>
       </c>
       <c r="G29" s="59">
@@ -4540,7 +4521,7 @@
       <c r="AJ29" s="69"/>
       <c r="AK29" s="69"/>
       <c r="AL29" s="69"/>
-      <c r="AM29" s="122"/>
+      <c r="AM29" s="121"/>
       <c r="AN29" s="118"/>
       <c r="AO29" s="118"/>
       <c r="AP29" s="118"/>
@@ -4578,16 +4559,16 @@
         <v>52</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D30" s="117" t="s">
         <v>69</v>
       </c>
-      <c r="E30" s="137">
+      <c r="E30" s="136">
         <v>44533</v>
       </c>
-      <c r="F30" s="130" t="s">
-        <v>77</v>
+      <c r="F30" s="129" t="s">
+        <v>76</v>
       </c>
       <c r="G30" s="59">
         <v>5</v>
@@ -4633,7 +4614,7 @@
       <c r="AR30" s="71"/>
       <c r="AS30" s="71"/>
       <c r="AT30" s="119"/>
-      <c r="AU30" s="123"/>
+      <c r="AU30" s="122"/>
       <c r="AV30" s="119"/>
       <c r="AW30" s="118"/>
       <c r="AX30" s="118"/>
@@ -4644,7 +4625,7 @@
       <c r="BC30" s="69"/>
       <c r="BD30" s="69"/>
       <c r="BE30" s="105" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="BF30" s="105"/>
       <c r="BG30" s="72"/>
@@ -4665,15 +4646,15 @@
         <v>53</v>
       </c>
       <c r="C31" s="58" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D31" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="137" t="s">
-        <v>79</v>
-      </c>
-      <c r="F31" s="130">
+      <c r="E31" s="136" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="129">
         <v>44474</v>
       </c>
       <c r="G31" s="59">
@@ -4750,15 +4731,15 @@
         <v>54</v>
       </c>
       <c r="C32" s="58" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D32" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32" s="130">
+      <c r="E32" s="136" t="s">
+        <v>78</v>
+      </c>
+      <c r="F32" s="129">
         <v>44474</v>
       </c>
       <c r="G32" s="59">
@@ -4805,14 +4786,14 @@
       <c r="AR32" s="71"/>
       <c r="AS32" s="71"/>
       <c r="AT32" s="71"/>
-      <c r="AU32" s="123"/>
-      <c r="AV32" s="123"/>
+      <c r="AU32" s="122"/>
+      <c r="AV32" s="122"/>
       <c r="AW32" s="105"/>
       <c r="AX32" s="105"/>
       <c r="AY32" s="118"/>
       <c r="AZ32" s="118"/>
       <c r="BA32" s="118"/>
-      <c r="BB32" s="173"/>
+      <c r="BB32" s="171"/>
       <c r="BC32" s="69"/>
       <c r="BD32" s="105"/>
       <c r="BE32" s="105"/>
@@ -4829,358 +4810,358 @@
       <c r="BP32" s="105"/>
       <c r="BQ32" s="36"/>
     </row>
-    <row r="33" spans="1:69" s="121" customFormat="1" ht="20" customHeight="1" outlineLevel="1">
+    <row r="33" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A33" s="36"/>
       <c r="B33" s="59" t="s">
         <v>70</v>
       </c>
       <c r="C33" s="58" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D33" s="58" t="s">
-        <v>71</v>
-      </c>
-      <c r="E33" s="137" t="s">
-        <v>78</v>
-      </c>
-      <c r="F33" s="130" t="s">
-        <v>80</v>
+        <v>68</v>
+      </c>
+      <c r="E33" s="136">
+        <v>44116</v>
+      </c>
+      <c r="F33" s="129" t="s">
+        <v>67</v>
       </c>
       <c r="G33" s="59">
-        <v>3</v>
-      </c>
-      <c r="H33" s="88">
-        <v>0.75</v>
+        <v>2</v>
+      </c>
+      <c r="H33" s="73">
+        <v>1</v>
       </c>
       <c r="I33" s="67"/>
       <c r="J33" s="68"/>
       <c r="K33" s="74"/>
       <c r="L33" s="74"/>
-      <c r="M33" s="74"/>
+      <c r="M33" s="69"/>
       <c r="N33" s="70"/>
       <c r="O33" s="70"/>
       <c r="P33" s="70"/>
       <c r="Q33" s="70"/>
       <c r="R33" s="70"/>
-      <c r="S33" s="74"/>
-      <c r="T33" s="74"/>
-      <c r="U33" s="74"/>
-      <c r="V33" s="74"/>
-      <c r="W33" s="74"/>
-      <c r="X33" s="74"/>
-      <c r="Y33" s="74"/>
-      <c r="Z33" s="74"/>
-      <c r="AA33" s="74"/>
-      <c r="AB33" s="74"/>
+      <c r="S33" s="105"/>
+      <c r="T33" s="105"/>
+      <c r="U33" s="105"/>
+      <c r="V33" s="69"/>
+      <c r="W33" s="69"/>
+      <c r="X33" s="69"/>
+      <c r="Y33" s="69"/>
+      <c r="Z33" s="69"/>
+      <c r="AA33" s="69"/>
+      <c r="AB33" s="69"/>
       <c r="AC33" s="94"/>
       <c r="AD33" s="94"/>
       <c r="AE33" s="94"/>
       <c r="AF33" s="94"/>
-      <c r="AG33" s="94"/>
-      <c r="AH33" s="105"/>
-      <c r="AI33" s="105"/>
-      <c r="AJ33" s="105"/>
-      <c r="AK33" s="105"/>
-      <c r="AL33" s="105"/>
-      <c r="AM33" s="105"/>
-      <c r="AN33" s="105"/>
-      <c r="AO33" s="74"/>
-      <c r="AP33" s="74"/>
-      <c r="AQ33" s="74"/>
+      <c r="AG33" s="114"/>
+      <c r="AH33" s="109"/>
+      <c r="AI33" s="109"/>
+      <c r="AJ33" s="69"/>
+      <c r="AK33" s="69"/>
+      <c r="AL33" s="69"/>
+      <c r="AM33" s="69"/>
+      <c r="AN33" s="69"/>
+      <c r="AO33" s="69"/>
+      <c r="AP33" s="69"/>
+      <c r="AQ33" s="69"/>
       <c r="AR33" s="71"/>
       <c r="AS33" s="71"/>
       <c r="AT33" s="71"/>
-      <c r="AU33" s="123"/>
-      <c r="AV33" s="123"/>
-      <c r="AW33" s="118"/>
-      <c r="AX33" s="105"/>
-      <c r="AY33" s="172"/>
-      <c r="AZ33" s="118"/>
-      <c r="BA33" s="175"/>
-      <c r="BB33" s="74"/>
-      <c r="BC33" s="74"/>
-      <c r="BD33" s="105"/>
-      <c r="BE33" s="105"/>
-      <c r="BF33" s="105"/>
-      <c r="BG33" s="120"/>
+      <c r="AU33" s="71"/>
+      <c r="AV33" s="71"/>
+      <c r="AW33" s="69"/>
+      <c r="AX33" s="69"/>
+      <c r="AY33" s="69"/>
+      <c r="AZ33" s="105"/>
+      <c r="BA33" s="105"/>
+      <c r="BB33" s="69"/>
+      <c r="BC33" s="69"/>
+      <c r="BD33" s="69"/>
+      <c r="BE33" s="69"/>
+      <c r="BF33" s="69"/>
+      <c r="BG33" s="72"/>
       <c r="BH33" s="72"/>
       <c r="BI33" s="72"/>
-      <c r="BJ33" s="120"/>
-      <c r="BK33" s="120"/>
+      <c r="BJ33" s="72"/>
+      <c r="BK33" s="72"/>
       <c r="BL33" s="105"/>
-      <c r="BM33" s="105"/>
-      <c r="BN33" s="105"/>
+      <c r="BM33" s="69"/>
+      <c r="BN33" s="69"/>
       <c r="BO33" s="105"/>
       <c r="BP33" s="105"/>
       <c r="BQ33" s="36"/>
     </row>
-    <row r="34" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
-      <c r="A34" s="36"/>
-      <c r="B34" s="59" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="58" t="s">
+    <row r="34" spans="1:69" ht="21" customHeight="1">
+      <c r="A34" s="20"/>
+      <c r="B34" s="127">
+        <v>3</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="31"/>
+      <c r="E34" s="134"/>
+      <c r="F34" s="127"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="33"/>
+      <c r="K34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="35"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="35"/>
+      <c r="P34" s="32"/>
+      <c r="Q34" s="35"/>
+      <c r="R34" s="35"/>
+      <c r="S34" s="35"/>
+      <c r="T34" s="35"/>
+      <c r="U34" s="35"/>
+      <c r="V34" s="35"/>
+      <c r="W34" s="35"/>
+      <c r="X34" s="35"/>
+      <c r="Y34" s="35"/>
+      <c r="Z34" s="35"/>
+      <c r="AA34" s="35"/>
+      <c r="AB34" s="35"/>
+      <c r="AC34" s="96"/>
+      <c r="AD34" s="96"/>
+      <c r="AE34" s="96"/>
+      <c r="AF34" s="96"/>
+      <c r="AG34" s="96"/>
+      <c r="AH34" s="35"/>
+      <c r="AI34" s="35"/>
+      <c r="AJ34" s="35"/>
+      <c r="AK34" s="35"/>
+      <c r="AL34" s="35"/>
+      <c r="AM34" s="35"/>
+      <c r="AN34" s="35"/>
+      <c r="AO34" s="35"/>
+      <c r="AP34" s="35"/>
+      <c r="AQ34" s="35"/>
+      <c r="AR34" s="35"/>
+      <c r="AS34" s="35"/>
+      <c r="AT34" s="35"/>
+      <c r="AU34" s="35"/>
+      <c r="AV34" s="35"/>
+      <c r="AW34" s="35"/>
+      <c r="AX34" s="35"/>
+      <c r="AY34" s="35"/>
+      <c r="AZ34" s="35"/>
+      <c r="BA34" s="35"/>
+      <c r="BB34" s="35"/>
+      <c r="BC34" s="35"/>
+      <c r="BD34" s="35"/>
+      <c r="BE34" s="35"/>
+      <c r="BF34" s="35"/>
+      <c r="BG34" s="35"/>
+      <c r="BH34" s="35"/>
+      <c r="BI34" s="35"/>
+      <c r="BJ34" s="35"/>
+      <c r="BK34" s="35"/>
+      <c r="BL34" s="35"/>
+      <c r="BM34" s="35"/>
+      <c r="BN34" s="35"/>
+      <c r="BO34" s="35"/>
+      <c r="BP34" s="35"/>
+      <c r="BQ34" s="20"/>
+    </row>
+    <row r="35" spans="1:69" s="170" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+      <c r="A35" s="36"/>
+      <c r="B35" s="38">
+        <v>3.1</v>
+      </c>
+      <c r="C35" s="37" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="58" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="137">
-        <v>44116</v>
-      </c>
-      <c r="F34" s="130" t="s">
-        <v>67</v>
-      </c>
-      <c r="G34" s="59">
+      <c r="D35" s="37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E35" s="136" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="129">
+        <v>44319</v>
+      </c>
+      <c r="G35" s="38">
         <v>2</v>
       </c>
-      <c r="H34" s="73">
+      <c r="H35" s="39">
         <v>1</v>
       </c>
-      <c r="I34" s="67"/>
-      <c r="J34" s="68"/>
-      <c r="K34" s="74"/>
-      <c r="L34" s="74"/>
-      <c r="M34" s="69"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="70"/>
-      <c r="R34" s="70"/>
-      <c r="S34" s="105"/>
-      <c r="T34" s="105"/>
-      <c r="U34" s="105"/>
-      <c r="V34" s="69"/>
-      <c r="W34" s="69"/>
-      <c r="X34" s="69"/>
-      <c r="Y34" s="69"/>
-      <c r="Z34" s="69"/>
-      <c r="AA34" s="69"/>
-      <c r="AB34" s="69"/>
-      <c r="AC34" s="94"/>
-      <c r="AD34" s="94"/>
-      <c r="AE34" s="94"/>
-      <c r="AF34" s="94"/>
-      <c r="AG34" s="114"/>
-      <c r="AH34" s="109"/>
-      <c r="AI34" s="109"/>
-      <c r="AJ34" s="69"/>
-      <c r="AK34" s="69"/>
-      <c r="AL34" s="69"/>
-      <c r="AM34" s="69"/>
-      <c r="AN34" s="69"/>
-      <c r="AO34" s="69"/>
-      <c r="AP34" s="69"/>
-      <c r="AQ34" s="69"/>
-      <c r="AR34" s="71"/>
-      <c r="AS34" s="71"/>
-      <c r="AT34" s="71"/>
-      <c r="AU34" s="71"/>
-      <c r="AV34" s="71"/>
-      <c r="AW34" s="69"/>
-      <c r="AX34" s="69"/>
-      <c r="AY34" s="69"/>
-      <c r="AZ34" s="105"/>
-      <c r="BA34" s="105"/>
-      <c r="BB34" s="69"/>
-      <c r="BC34" s="69"/>
-      <c r="BD34" s="69"/>
-      <c r="BE34" s="69"/>
-      <c r="BF34" s="69"/>
-      <c r="BG34" s="72"/>
-      <c r="BH34" s="72"/>
-      <c r="BI34" s="72"/>
-      <c r="BJ34" s="72"/>
-      <c r="BK34" s="72"/>
-      <c r="BL34" s="105"/>
-      <c r="BM34" s="69"/>
-      <c r="BN34" s="69"/>
-      <c r="BO34" s="105"/>
-      <c r="BP34" s="105"/>
-      <c r="BQ34" s="36"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="41"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="53"/>
+      <c r="P35" s="53"/>
+      <c r="Q35" s="53"/>
+      <c r="R35" s="53"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="44"/>
+      <c r="X35" s="44"/>
+      <c r="Y35" s="44"/>
+      <c r="Z35" s="44"/>
+      <c r="AA35" s="44"/>
+      <c r="AB35" s="44"/>
+      <c r="AC35" s="94"/>
+      <c r="AD35" s="94"/>
+      <c r="AE35" s="94"/>
+      <c r="AF35" s="94"/>
+      <c r="AG35" s="94"/>
+      <c r="AH35" s="44"/>
+      <c r="AI35" s="44"/>
+      <c r="AJ35" s="44"/>
+      <c r="AK35" s="44"/>
+      <c r="AL35" s="44"/>
+      <c r="AM35" s="44"/>
+      <c r="AN35" s="44"/>
+      <c r="AO35" s="44"/>
+      <c r="AP35" s="44"/>
+      <c r="AQ35" s="44"/>
+      <c r="AR35" s="45"/>
+      <c r="AS35" s="45"/>
+      <c r="AT35" s="45"/>
+      <c r="AU35" s="45"/>
+      <c r="AV35" s="45"/>
+      <c r="AW35" s="44"/>
+      <c r="AX35" s="44"/>
+      <c r="AY35" s="44"/>
+      <c r="AZ35" s="44"/>
+      <c r="BA35" s="44"/>
+      <c r="BB35" s="123"/>
+      <c r="BC35" s="123"/>
+      <c r="BD35" s="44"/>
+      <c r="BE35" s="123"/>
+      <c r="BF35" s="123"/>
+      <c r="BG35" s="46"/>
+      <c r="BH35" s="46"/>
+      <c r="BI35" s="46"/>
+      <c r="BJ35" s="46"/>
+      <c r="BK35" s="46"/>
+      <c r="BL35" s="44"/>
+      <c r="BM35" s="44"/>
+      <c r="BN35" s="44"/>
+      <c r="BO35" s="44"/>
+      <c r="BP35" s="47"/>
+      <c r="BQ35" s="36"/>
     </row>
-    <row r="35" spans="1:69" ht="21" customHeight="1">
-      <c r="A35" s="20"/>
-      <c r="B35" s="128">
-        <v>3</v>
-      </c>
-      <c r="C35" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="D35" s="31"/>
-      <c r="E35" s="135"/>
-      <c r="F35" s="128"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="33"/>
-      <c r="K35" s="34"/>
-      <c r="L35" s="34"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="32"/>
-      <c r="O35" s="35"/>
-      <c r="P35" s="32"/>
-      <c r="Q35" s="35"/>
-      <c r="R35" s="35"/>
-      <c r="S35" s="35"/>
-      <c r="T35" s="35"/>
-      <c r="U35" s="35"/>
-      <c r="V35" s="35"/>
-      <c r="W35" s="35"/>
-      <c r="X35" s="35"/>
-      <c r="Y35" s="35"/>
-      <c r="Z35" s="35"/>
-      <c r="AA35" s="35"/>
-      <c r="AB35" s="35"/>
-      <c r="AC35" s="96"/>
-      <c r="AD35" s="96"/>
-      <c r="AE35" s="96"/>
-      <c r="AF35" s="96"/>
-      <c r="AG35" s="96"/>
-      <c r="AH35" s="35"/>
-      <c r="AI35" s="35"/>
-      <c r="AJ35" s="35"/>
-      <c r="AK35" s="35"/>
-      <c r="AL35" s="35"/>
-      <c r="AM35" s="35"/>
-      <c r="AN35" s="35"/>
-      <c r="AO35" s="35"/>
-      <c r="AP35" s="35"/>
-      <c r="AQ35" s="35"/>
-      <c r="AR35" s="35"/>
-      <c r="AS35" s="35"/>
-      <c r="AT35" s="35"/>
-      <c r="AU35" s="35"/>
-      <c r="AV35" s="35"/>
-      <c r="AW35" s="35"/>
-      <c r="AX35" s="35"/>
-      <c r="AY35" s="35"/>
-      <c r="AZ35" s="35"/>
-      <c r="BA35" s="35"/>
-      <c r="BB35" s="35"/>
-      <c r="BC35" s="35"/>
-      <c r="BD35" s="35"/>
-      <c r="BE35" s="35"/>
-      <c r="BF35" s="35"/>
-      <c r="BG35" s="35"/>
-      <c r="BH35" s="35"/>
-      <c r="BI35" s="35"/>
-      <c r="BJ35" s="35"/>
-      <c r="BK35" s="35"/>
-      <c r="BL35" s="35"/>
-      <c r="BM35" s="35"/>
-      <c r="BN35" s="35"/>
-      <c r="BO35" s="35"/>
-      <c r="BP35" s="35"/>
-      <c r="BQ35" s="20"/>
-    </row>
-    <row r="36" spans="1:69" s="171" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+    <row r="36" spans="1:69" s="170" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
       <c r="A36" s="36"/>
       <c r="B36" s="38">
-        <v>3.1</v>
+        <v>3.2</v>
       </c>
       <c r="C36" s="37" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D36" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="137" t="s">
-        <v>76</v>
-      </c>
-      <c r="F36" s="130">
-        <v>44319</v>
+      <c r="E36" s="136" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="129">
+        <v>44474</v>
       </c>
       <c r="G36" s="38">
         <v>2</v>
       </c>
       <c r="H36" s="39">
-        <v>0.95</v>
-      </c>
-      <c r="I36" s="40"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="44"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="44"/>
+        <v>1</v>
+      </c>
+      <c r="I36" s="48"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="51"/>
+      <c r="M36" s="51"/>
       <c r="N36" s="53"/>
       <c r="O36" s="53"/>
       <c r="P36" s="53"/>
       <c r="Q36" s="53"/>
       <c r="R36" s="53"/>
-      <c r="S36" s="44"/>
-      <c r="T36" s="44"/>
-      <c r="U36" s="44"/>
-      <c r="V36" s="44"/>
-      <c r="W36" s="44"/>
-      <c r="X36" s="44"/>
-      <c r="Y36" s="44"/>
-      <c r="Z36" s="44"/>
-      <c r="AA36" s="44"/>
-      <c r="AB36" s="44"/>
+      <c r="S36" s="51"/>
+      <c r="T36" s="51"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="51"/>
+      <c r="W36" s="51"/>
+      <c r="X36" s="51"/>
+      <c r="Y36" s="51"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="51"/>
+      <c r="AB36" s="51"/>
       <c r="AC36" s="94"/>
       <c r="AD36" s="94"/>
       <c r="AE36" s="94"/>
       <c r="AF36" s="94"/>
       <c r="AG36" s="94"/>
-      <c r="AH36" s="44"/>
-      <c r="AI36" s="44"/>
-      <c r="AJ36" s="44"/>
-      <c r="AK36" s="44"/>
-      <c r="AL36" s="44"/>
-      <c r="AM36" s="44"/>
-      <c r="AN36" s="44"/>
-      <c r="AO36" s="44"/>
-      <c r="AP36" s="44"/>
-      <c r="AQ36" s="44"/>
-      <c r="AR36" s="45"/>
-      <c r="AS36" s="45"/>
-      <c r="AT36" s="45"/>
-      <c r="AU36" s="45"/>
-      <c r="AV36" s="45"/>
-      <c r="AW36" s="44"/>
-      <c r="AX36" s="44"/>
-      <c r="AY36" s="44"/>
-      <c r="AZ36" s="44"/>
-      <c r="BA36" s="44"/>
-      <c r="BB36" s="124"/>
-      <c r="BC36" s="124"/>
-      <c r="BD36" s="44"/>
-      <c r="BE36" s="124"/>
-      <c r="BF36" s="124"/>
-      <c r="BG36" s="46"/>
-      <c r="BH36" s="46"/>
-      <c r="BI36" s="46"/>
-      <c r="BJ36" s="46"/>
-      <c r="BK36" s="46"/>
-      <c r="BL36" s="44"/>
-      <c r="BM36" s="44"/>
-      <c r="BN36" s="44"/>
-      <c r="BO36" s="44"/>
-      <c r="BP36" s="47"/>
+      <c r="AH36" s="51"/>
+      <c r="AI36" s="51"/>
+      <c r="AJ36" s="51"/>
+      <c r="AK36" s="51"/>
+      <c r="AL36" s="51"/>
+      <c r="AM36" s="51"/>
+      <c r="AN36" s="51"/>
+      <c r="AO36" s="51"/>
+      <c r="AP36" s="51"/>
+      <c r="AQ36" s="51"/>
+      <c r="AR36" s="54"/>
+      <c r="AS36" s="54"/>
+      <c r="AT36" s="54"/>
+      <c r="AU36" s="54"/>
+      <c r="AV36" s="54"/>
+      <c r="AW36" s="51"/>
+      <c r="AX36" s="51"/>
+      <c r="AY36" s="51"/>
+      <c r="AZ36" s="51"/>
+      <c r="BA36" s="51"/>
+      <c r="BB36" s="51"/>
+      <c r="BC36" s="51"/>
+      <c r="BD36" s="51"/>
+      <c r="BE36" s="51"/>
+      <c r="BF36" s="140"/>
+      <c r="BG36" s="141"/>
+      <c r="BH36" s="141"/>
+      <c r="BI36" s="55"/>
+      <c r="BJ36" s="141"/>
+      <c r="BK36" s="139"/>
+      <c r="BL36" s="140"/>
+      <c r="BM36" s="51"/>
+      <c r="BN36" s="51"/>
+      <c r="BO36" s="51"/>
+      <c r="BP36" s="56"/>
       <c r="BQ36" s="36"/>
     </row>
-    <row r="37" spans="1:69" s="171" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+    <row r="37" spans="1:69" s="170" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
       <c r="A37" s="36"/>
       <c r="B37" s="38">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="C37" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D37" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="137" t="s">
-        <v>79</v>
-      </c>
-      <c r="F37" s="130">
+      <c r="E37" s="136" t="s">
+        <v>78</v>
+      </c>
+      <c r="F37" s="129">
         <v>44474</v>
       </c>
       <c r="G37" s="38">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H37" s="39">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="I37" s="48"/>
       <c r="J37" s="49"/>
@@ -5192,10 +5173,10 @@
       <c r="P37" s="53"/>
       <c r="Q37" s="53"/>
       <c r="R37" s="53"/>
-      <c r="S37" s="51"/>
-      <c r="T37" s="51"/>
-      <c r="U37" s="51"/>
-      <c r="V37" s="51"/>
+      <c r="S37" s="44"/>
+      <c r="T37" s="44"/>
+      <c r="U37" s="44"/>
+      <c r="V37" s="44"/>
       <c r="W37" s="51"/>
       <c r="X37" s="51"/>
       <c r="Y37" s="51"/>
@@ -5231,56 +5212,56 @@
       <c r="BC37" s="51"/>
       <c r="BD37" s="51"/>
       <c r="BE37" s="51"/>
-      <c r="BF37" s="141"/>
-      <c r="BG37" s="142"/>
-      <c r="BH37" s="142"/>
+      <c r="BF37" s="51"/>
+      <c r="BG37" s="141"/>
+      <c r="BH37" s="55"/>
       <c r="BI37" s="55"/>
-      <c r="BJ37" s="142"/>
-      <c r="BK37" s="140"/>
-      <c r="BL37" s="141"/>
-      <c r="BM37" s="51"/>
+      <c r="BJ37" s="141"/>
+      <c r="BK37" s="55"/>
+      <c r="BL37" s="140"/>
+      <c r="BM37" s="140"/>
       <c r="BN37" s="51"/>
       <c r="BO37" s="51"/>
       <c r="BP37" s="56"/>
       <c r="BQ37" s="36"/>
     </row>
-    <row r="38" spans="1:69" s="171" customFormat="1" ht="21" customHeight="1" outlineLevel="1">
+    <row r="38" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
       <c r="A38" s="36"/>
       <c r="B38" s="38">
-        <v>3.3</v>
+        <v>3.4</v>
       </c>
       <c r="C38" s="37" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D38" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="F38" s="130">
+      <c r="E38" s="136" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="129">
         <v>44474</v>
       </c>
       <c r="G38" s="38">
         <v>3</v>
       </c>
-      <c r="H38" s="39">
-        <v>0.95</v>
+      <c r="H38" s="87">
+        <v>1</v>
       </c>
       <c r="I38" s="48"/>
       <c r="J38" s="49"/>
-      <c r="K38" s="51"/>
-      <c r="L38" s="51"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
       <c r="M38" s="51"/>
       <c r="N38" s="53"/>
       <c r="O38" s="53"/>
       <c r="P38" s="53"/>
       <c r="Q38" s="53"/>
       <c r="R38" s="53"/>
-      <c r="S38" s="44"/>
-      <c r="T38" s="44"/>
-      <c r="U38" s="44"/>
-      <c r="V38" s="44"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="42"/>
+      <c r="U38" s="42"/>
+      <c r="V38" s="42"/>
       <c r="W38" s="51"/>
       <c r="X38" s="51"/>
       <c r="Y38" s="51"/>
@@ -5317,421 +5298,354 @@
       <c r="BD38" s="51"/>
       <c r="BE38" s="51"/>
       <c r="BF38" s="51"/>
-      <c r="BG38" s="142"/>
+      <c r="BG38" s="55"/>
       <c r="BH38" s="55"/>
       <c r="BI38" s="55"/>
-      <c r="BJ38" s="142"/>
-      <c r="BK38" s="55"/>
-      <c r="BL38" s="141"/>
-      <c r="BM38" s="141"/>
-      <c r="BN38" s="51"/>
-      <c r="BO38" s="51"/>
+      <c r="BJ38" s="55"/>
+      <c r="BK38" s="141"/>
+      <c r="BL38" s="51"/>
+      <c r="BM38" s="140"/>
+      <c r="BN38" s="140"/>
+      <c r="BO38" s="140"/>
       <c r="BP38" s="56"/>
       <c r="BQ38" s="36"/>
     </row>
-    <row r="39" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
-      <c r="A39" s="36"/>
-      <c r="B39" s="38">
-        <v>3.4</v>
-      </c>
-      <c r="C39" s="37" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="37" t="s">
-        <v>69</v>
-      </c>
-      <c r="E39" s="137" t="s">
-        <v>81</v>
-      </c>
-      <c r="F39" s="130">
+    <row r="39" spans="1:69" ht="21" customHeight="1">
+      <c r="A39" s="20"/>
+      <c r="B39" s="127">
+        <v>4</v>
+      </c>
+      <c r="C39" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" s="31"/>
+      <c r="E39" s="134"/>
+      <c r="F39" s="127"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
+      <c r="I39" s="32"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="34"/>
+      <c r="L39" s="34"/>
+      <c r="M39" s="35"/>
+      <c r="N39" s="32"/>
+      <c r="O39" s="35"/>
+      <c r="P39" s="32"/>
+      <c r="Q39" s="35"/>
+      <c r="R39" s="35"/>
+      <c r="S39" s="35"/>
+      <c r="T39" s="35"/>
+      <c r="U39" s="35"/>
+      <c r="V39" s="35"/>
+      <c r="W39" s="35"/>
+      <c r="X39" s="35"/>
+      <c r="Y39" s="35"/>
+      <c r="Z39" s="35"/>
+      <c r="AA39" s="35"/>
+      <c r="AB39" s="35"/>
+      <c r="AC39" s="96"/>
+      <c r="AD39" s="96"/>
+      <c r="AE39" s="96"/>
+      <c r="AF39" s="96"/>
+      <c r="AG39" s="96"/>
+      <c r="AH39" s="35"/>
+      <c r="AI39" s="35"/>
+      <c r="AJ39" s="35"/>
+      <c r="AK39" s="35"/>
+      <c r="AL39" s="35"/>
+      <c r="AM39" s="35"/>
+      <c r="AN39" s="35"/>
+      <c r="AO39" s="35"/>
+      <c r="AP39" s="35"/>
+      <c r="AQ39" s="35"/>
+      <c r="AR39" s="35"/>
+      <c r="AS39" s="35"/>
+      <c r="AT39" s="35"/>
+      <c r="AU39" s="35"/>
+      <c r="AV39" s="35"/>
+      <c r="AW39" s="35"/>
+      <c r="AX39" s="35"/>
+      <c r="AY39" s="35"/>
+      <c r="AZ39" s="35"/>
+      <c r="BA39" s="35"/>
+      <c r="BB39" s="35"/>
+      <c r="BC39" s="35"/>
+      <c r="BD39" s="35"/>
+      <c r="BE39" s="35"/>
+      <c r="BF39" s="35"/>
+      <c r="BG39" s="35"/>
+      <c r="BH39" s="35"/>
+      <c r="BI39" s="35"/>
+      <c r="BJ39" s="35"/>
+      <c r="BK39" s="35"/>
+      <c r="BL39" s="35"/>
+      <c r="BM39" s="35"/>
+      <c r="BN39" s="35"/>
+      <c r="BO39" s="35"/>
+      <c r="BP39" s="35"/>
+      <c r="BQ39" s="20"/>
+    </row>
+    <row r="40" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
+      <c r="A40" s="36"/>
+      <c r="B40" s="38">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E40" s="135">
+        <v>44291</v>
+      </c>
+      <c r="F40" s="128">
+        <v>44291</v>
+      </c>
+      <c r="G40" s="38">
+        <v>1</v>
+      </c>
+      <c r="H40" s="39">
+        <v>1</v>
+      </c>
+      <c r="I40" s="40"/>
+      <c r="J40" s="41"/>
+      <c r="K40" s="42"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="43"/>
+      <c r="O40" s="43"/>
+      <c r="P40" s="43"/>
+      <c r="Q40" s="43"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="44"/>
+      <c r="T40" s="44"/>
+      <c r="U40" s="44"/>
+      <c r="V40" s="44"/>
+      <c r="W40" s="44"/>
+      <c r="X40" s="44"/>
+      <c r="Y40" s="44"/>
+      <c r="Z40" s="44"/>
+      <c r="AA40" s="44"/>
+      <c r="AB40" s="44"/>
+      <c r="AC40" s="94"/>
+      <c r="AD40" s="94"/>
+      <c r="AE40" s="94"/>
+      <c r="AF40" s="94"/>
+      <c r="AG40" s="94"/>
+      <c r="AH40" s="44"/>
+      <c r="AI40" s="44"/>
+      <c r="AJ40" s="44"/>
+      <c r="AK40" s="44"/>
+      <c r="AL40" s="44"/>
+      <c r="AM40" s="44"/>
+      <c r="AN40" s="44"/>
+      <c r="AO40" s="44"/>
+      <c r="AP40" s="44"/>
+      <c r="AQ40" s="44"/>
+      <c r="AR40" s="45"/>
+      <c r="AS40" s="45"/>
+      <c r="AT40" s="45"/>
+      <c r="AU40" s="45"/>
+      <c r="AV40" s="45"/>
+      <c r="AW40" s="44"/>
+      <c r="AX40" s="44"/>
+      <c r="AY40" s="44"/>
+      <c r="AZ40" s="44"/>
+      <c r="BA40" s="44"/>
+      <c r="BB40" s="44"/>
+      <c r="BC40" s="44"/>
+      <c r="BD40" s="44"/>
+      <c r="BE40" s="44"/>
+      <c r="BF40" s="44"/>
+      <c r="BG40" s="46"/>
+      <c r="BH40" s="46"/>
+      <c r="BI40" s="46"/>
+      <c r="BJ40" s="46"/>
+      <c r="BK40" s="46"/>
+      <c r="BL40" s="90"/>
+      <c r="BM40" s="90"/>
+      <c r="BN40" s="123"/>
+      <c r="BO40" s="90"/>
+      <c r="BP40" s="124"/>
+      <c r="BQ40" s="36"/>
+    </row>
+    <row r="41" spans="1:69" s="169" customFormat="1" ht="21" customHeight="1">
+      <c r="A41" s="163"/>
+      <c r="B41" s="164">
+        <v>4.2</v>
+      </c>
+      <c r="C41" s="163" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="165" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41" s="166">
+        <v>44260</v>
+      </c>
+      <c r="F41" s="166">
         <v>44474</v>
       </c>
-      <c r="G39" s="38">
-        <v>3</v>
-      </c>
-      <c r="H39" s="87">
-        <v>0.95</v>
-      </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="49"/>
-      <c r="K39" s="50"/>
-      <c r="L39" s="50"/>
-      <c r="M39" s="51"/>
-      <c r="N39" s="53"/>
-      <c r="O39" s="53"/>
-      <c r="P39" s="53"/>
-      <c r="Q39" s="53"/>
-      <c r="R39" s="53"/>
-      <c r="S39" s="42"/>
-      <c r="T39" s="42"/>
-      <c r="U39" s="42"/>
-      <c r="V39" s="42"/>
-      <c r="W39" s="51"/>
-      <c r="X39" s="51"/>
-      <c r="Y39" s="51"/>
-      <c r="Z39" s="51"/>
-      <c r="AA39" s="51"/>
-      <c r="AB39" s="51"/>
-      <c r="AC39" s="94"/>
-      <c r="AD39" s="94"/>
-      <c r="AE39" s="94"/>
-      <c r="AF39" s="94"/>
-      <c r="AG39" s="94"/>
-      <c r="AH39" s="51"/>
-      <c r="AI39" s="51"/>
-      <c r="AJ39" s="51"/>
-      <c r="AK39" s="51"/>
-      <c r="AL39" s="51"/>
-      <c r="AM39" s="51"/>
-      <c r="AN39" s="51"/>
-      <c r="AO39" s="51"/>
-      <c r="AP39" s="51"/>
-      <c r="AQ39" s="51"/>
-      <c r="AR39" s="54"/>
-      <c r="AS39" s="54"/>
-      <c r="AT39" s="54"/>
-      <c r="AU39" s="54"/>
-      <c r="AV39" s="54"/>
-      <c r="AW39" s="51"/>
-      <c r="AX39" s="51"/>
-      <c r="AY39" s="51"/>
-      <c r="AZ39" s="51"/>
-      <c r="BA39" s="51"/>
-      <c r="BB39" s="51"/>
-      <c r="BC39" s="51"/>
-      <c r="BD39" s="51"/>
-      <c r="BE39" s="51"/>
-      <c r="BF39" s="51"/>
-      <c r="BG39" s="55"/>
-      <c r="BH39" s="55"/>
-      <c r="BI39" s="55"/>
-      <c r="BJ39" s="55"/>
-      <c r="BK39" s="142"/>
-      <c r="BL39" s="51"/>
-      <c r="BM39" s="141"/>
-      <c r="BN39" s="141"/>
-      <c r="BO39" s="141"/>
-      <c r="BP39" s="56"/>
-      <c r="BQ39" s="36"/>
+      <c r="G41" s="164">
+        <v>1</v>
+      </c>
+      <c r="H41" s="167">
+        <v>1</v>
+      </c>
+      <c r="I41" s="163"/>
+      <c r="J41" s="163"/>
+      <c r="K41" s="163"/>
+      <c r="L41" s="163"/>
+      <c r="M41" s="163"/>
+      <c r="N41" s="163"/>
+      <c r="O41" s="163"/>
+      <c r="P41" s="163"/>
+      <c r="Q41" s="163"/>
+      <c r="R41" s="163"/>
+      <c r="S41" s="163"/>
+      <c r="T41" s="163"/>
+      <c r="U41" s="163"/>
+      <c r="V41" s="163"/>
+      <c r="W41" s="163"/>
+      <c r="X41" s="163"/>
+      <c r="Y41" s="163"/>
+      <c r="Z41" s="163"/>
+      <c r="AA41" s="163"/>
+      <c r="AB41" s="163"/>
+      <c r="AC41" s="163"/>
+      <c r="AD41" s="163"/>
+      <c r="AE41" s="163"/>
+      <c r="AF41" s="163"/>
+      <c r="AG41" s="163"/>
+      <c r="AH41" s="163"/>
+      <c r="AI41" s="163"/>
+      <c r="AJ41" s="163"/>
+      <c r="AK41" s="163"/>
+      <c r="AL41" s="163"/>
+      <c r="AM41" s="163"/>
+      <c r="AN41" s="163"/>
+      <c r="AO41" s="163"/>
+      <c r="AP41" s="163"/>
+      <c r="AQ41" s="163"/>
+      <c r="AR41" s="163"/>
+      <c r="AS41" s="163"/>
+      <c r="AT41" s="163"/>
+      <c r="AU41" s="163"/>
+      <c r="AV41" s="163"/>
+      <c r="AW41" s="163"/>
+      <c r="AX41" s="163"/>
+      <c r="AY41" s="163"/>
+      <c r="AZ41" s="163"/>
+      <c r="BA41" s="163"/>
+      <c r="BB41" s="163"/>
+      <c r="BC41" s="163"/>
+      <c r="BD41" s="163"/>
+      <c r="BE41" s="163"/>
+      <c r="BF41" s="163"/>
+      <c r="BG41" s="163"/>
+      <c r="BH41" s="163"/>
+      <c r="BI41" s="163"/>
+      <c r="BJ41" s="163"/>
+      <c r="BK41" s="163"/>
+      <c r="BL41" s="163"/>
+      <c r="BM41" s="168"/>
+      <c r="BN41" s="168"/>
+      <c r="BO41" s="168"/>
+      <c r="BP41" s="168"/>
+      <c r="BQ41" s="163"/>
     </row>
-    <row r="40" spans="1:69" ht="21" customHeight="1">
-      <c r="A40" s="20"/>
-      <c r="B40" s="128">
-        <v>4</v>
-      </c>
-      <c r="C40" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D40" s="31"/>
-      <c r="E40" s="135"/>
-      <c r="F40" s="128"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="32"/>
-      <c r="J40" s="33"/>
-      <c r="K40" s="34"/>
-      <c r="L40" s="34"/>
-      <c r="M40" s="35"/>
-      <c r="N40" s="32"/>
-      <c r="O40" s="35"/>
-      <c r="P40" s="32"/>
-      <c r="Q40" s="35"/>
-      <c r="R40" s="35"/>
-      <c r="S40" s="35"/>
-      <c r="T40" s="35"/>
-      <c r="U40" s="35"/>
-      <c r="V40" s="35"/>
-      <c r="W40" s="35"/>
-      <c r="X40" s="35"/>
-      <c r="Y40" s="35"/>
-      <c r="Z40" s="35"/>
-      <c r="AA40" s="35"/>
-      <c r="AB40" s="35"/>
-      <c r="AC40" s="96"/>
-      <c r="AD40" s="96"/>
-      <c r="AE40" s="96"/>
-      <c r="AF40" s="96"/>
-      <c r="AG40" s="96"/>
-      <c r="AH40" s="35"/>
-      <c r="AI40" s="35"/>
-      <c r="AJ40" s="35"/>
-      <c r="AK40" s="35"/>
-      <c r="AL40" s="35"/>
-      <c r="AM40" s="35"/>
-      <c r="AN40" s="35"/>
-      <c r="AO40" s="35"/>
-      <c r="AP40" s="35"/>
-      <c r="AQ40" s="35"/>
-      <c r="AR40" s="35"/>
-      <c r="AS40" s="35"/>
-      <c r="AT40" s="35"/>
-      <c r="AU40" s="35"/>
-      <c r="AV40" s="35"/>
-      <c r="AW40" s="35"/>
-      <c r="AX40" s="35"/>
-      <c r="AY40" s="35"/>
-      <c r="AZ40" s="35"/>
-      <c r="BA40" s="35"/>
-      <c r="BB40" s="35"/>
-      <c r="BC40" s="35"/>
-      <c r="BD40" s="35"/>
-      <c r="BE40" s="35"/>
-      <c r="BF40" s="35"/>
-      <c r="BG40" s="35"/>
-      <c r="BH40" s="35"/>
-      <c r="BI40" s="35"/>
-      <c r="BJ40" s="35"/>
-      <c r="BK40" s="35"/>
-      <c r="BL40" s="35"/>
-      <c r="BM40" s="35"/>
-      <c r="BN40" s="35"/>
-      <c r="BO40" s="35"/>
-      <c r="BP40" s="35"/>
-      <c r="BQ40" s="20"/>
-    </row>
-    <row r="41" spans="1:69" ht="21" customHeight="1" outlineLevel="1">
-      <c r="A41" s="36"/>
-      <c r="B41" s="38">
-        <v>4.0999999999999996</v>
-      </c>
-      <c r="C41" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="D41" s="37" t="s">
-        <v>61</v>
-      </c>
-      <c r="E41" s="136">
-        <v>44291</v>
-      </c>
-      <c r="F41" s="129">
-        <v>44291</v>
-      </c>
-      <c r="G41" s="38">
-        <v>1</v>
-      </c>
-      <c r="H41" s="39">
-        <v>1</v>
-      </c>
-      <c r="I41" s="40"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="42"/>
-      <c r="L41" s="42"/>
-      <c r="M41" s="42"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="43"/>
-      <c r="P41" s="43"/>
-      <c r="Q41" s="43"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="44"/>
-      <c r="T41" s="44"/>
-      <c r="U41" s="44"/>
-      <c r="V41" s="44"/>
-      <c r="W41" s="44"/>
-      <c r="X41" s="44"/>
-      <c r="Y41" s="44"/>
-      <c r="Z41" s="44"/>
-      <c r="AA41" s="44"/>
-      <c r="AB41" s="44"/>
-      <c r="AC41" s="94"/>
-      <c r="AD41" s="94"/>
-      <c r="AE41" s="94"/>
-      <c r="AF41" s="94"/>
-      <c r="AG41" s="94"/>
-      <c r="AH41" s="44"/>
-      <c r="AI41" s="44"/>
-      <c r="AJ41" s="44"/>
-      <c r="AK41" s="44"/>
-      <c r="AL41" s="44"/>
-      <c r="AM41" s="44"/>
-      <c r="AN41" s="44"/>
-      <c r="AO41" s="44"/>
-      <c r="AP41" s="44"/>
-      <c r="AQ41" s="44"/>
-      <c r="AR41" s="45"/>
-      <c r="AS41" s="45"/>
-      <c r="AT41" s="45"/>
-      <c r="AU41" s="45"/>
-      <c r="AV41" s="45"/>
-      <c r="AW41" s="44"/>
-      <c r="AX41" s="44"/>
-      <c r="AY41" s="44"/>
-      <c r="AZ41" s="44"/>
-      <c r="BA41" s="44"/>
-      <c r="BB41" s="44"/>
-      <c r="BC41" s="44"/>
-      <c r="BD41" s="44"/>
-      <c r="BE41" s="44"/>
-      <c r="BF41" s="44"/>
-      <c r="BG41" s="46"/>
-      <c r="BH41" s="46"/>
-      <c r="BI41" s="46"/>
-      <c r="BJ41" s="46"/>
-      <c r="BK41" s="46"/>
-      <c r="BL41" s="90"/>
-      <c r="BM41" s="90"/>
-      <c r="BN41" s="124"/>
-      <c r="BO41" s="90"/>
-      <c r="BP41" s="125"/>
-      <c r="BQ41" s="36"/>
-    </row>
-    <row r="42" spans="1:69" s="170" customFormat="1" ht="21" customHeight="1">
-      <c r="A42" s="164"/>
-      <c r="B42" s="165">
-        <v>4.2</v>
-      </c>
-      <c r="C42" s="164" t="s">
-        <v>88</v>
-      </c>
-      <c r="D42" s="166" t="s">
-        <v>61</v>
-      </c>
-      <c r="E42" s="167">
-        <v>44260</v>
-      </c>
-      <c r="F42" s="167">
-        <v>44474</v>
-      </c>
-      <c r="G42" s="165">
-        <v>1</v>
-      </c>
-      <c r="H42" s="168">
-        <v>1</v>
-      </c>
-      <c r="I42" s="164"/>
-      <c r="J42" s="164"/>
-      <c r="K42" s="164"/>
-      <c r="L42" s="164"/>
-      <c r="M42" s="164"/>
-      <c r="N42" s="164"/>
-      <c r="O42" s="164"/>
-      <c r="P42" s="164"/>
-      <c r="Q42" s="164"/>
-      <c r="R42" s="164"/>
-      <c r="S42" s="164"/>
-      <c r="T42" s="164"/>
-      <c r="U42" s="164"/>
-      <c r="V42" s="164"/>
-      <c r="W42" s="164"/>
-      <c r="X42" s="164"/>
-      <c r="Y42" s="164"/>
-      <c r="Z42" s="164"/>
-      <c r="AA42" s="164"/>
-      <c r="AB42" s="164"/>
-      <c r="AC42" s="164"/>
-      <c r="AD42" s="164"/>
-      <c r="AE42" s="164"/>
-      <c r="AF42" s="164"/>
-      <c r="AG42" s="164"/>
-      <c r="AH42" s="164"/>
-      <c r="AI42" s="164"/>
-      <c r="AJ42" s="164"/>
-      <c r="AK42" s="164"/>
-      <c r="AL42" s="164"/>
-      <c r="AM42" s="164"/>
-      <c r="AN42" s="164"/>
-      <c r="AO42" s="164"/>
-      <c r="AP42" s="164"/>
-      <c r="AQ42" s="164"/>
-      <c r="AR42" s="164"/>
-      <c r="AS42" s="164"/>
-      <c r="AT42" s="164"/>
-      <c r="AU42" s="164"/>
-      <c r="AV42" s="164"/>
-      <c r="AW42" s="164"/>
-      <c r="AX42" s="164"/>
-      <c r="AY42" s="164"/>
-      <c r="AZ42" s="164"/>
-      <c r="BA42" s="164"/>
-      <c r="BB42" s="164"/>
-      <c r="BC42" s="164"/>
-      <c r="BD42" s="164"/>
-      <c r="BE42" s="164"/>
-      <c r="BF42" s="164"/>
-      <c r="BG42" s="164"/>
-      <c r="BH42" s="164"/>
-      <c r="BI42" s="164"/>
-      <c r="BJ42" s="164"/>
-      <c r="BK42" s="164"/>
-      <c r="BL42" s="164"/>
-      <c r="BM42" s="169"/>
-      <c r="BN42" s="169"/>
-      <c r="BO42" s="169"/>
-      <c r="BP42" s="169"/>
-      <c r="BQ42" s="164"/>
-    </row>
-    <row r="43" spans="1:69" ht="21" customHeight="1">
-      <c r="A43" s="20"/>
-      <c r="B43" s="75"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="138"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
-      <c r="K43" s="20"/>
-      <c r="L43" s="20"/>
-      <c r="M43" s="20"/>
-      <c r="N43" s="20"/>
-      <c r="O43" s="20"/>
-      <c r="P43" s="20"/>
-      <c r="Q43" s="20"/>
-      <c r="R43" s="20"/>
-      <c r="S43" s="20"/>
-      <c r="T43" s="20"/>
-      <c r="U43" s="20"/>
-      <c r="V43" s="20"/>
-      <c r="W43" s="20"/>
-      <c r="X43" s="20"/>
-      <c r="Y43" s="20"/>
-      <c r="Z43" s="20"/>
-      <c r="AA43" s="20"/>
-      <c r="AB43" s="20"/>
-      <c r="AC43" s="20"/>
-      <c r="AD43" s="20"/>
-      <c r="AE43" s="20"/>
-      <c r="AF43" s="20"/>
-      <c r="AG43" s="20"/>
-      <c r="AH43" s="20"/>
-      <c r="AI43" s="20"/>
-      <c r="AJ43" s="20"/>
-      <c r="AK43" s="20"/>
-      <c r="AL43" s="20"/>
-      <c r="AM43" s="20"/>
-      <c r="AN43" s="20"/>
-      <c r="AO43" s="20"/>
-      <c r="AP43" s="20"/>
-      <c r="AQ43" s="20"/>
-      <c r="AR43" s="20"/>
-      <c r="AS43" s="20"/>
-      <c r="AT43" s="20"/>
-      <c r="AU43" s="20"/>
-      <c r="AV43" s="20"/>
-      <c r="AW43" s="20"/>
-      <c r="AX43" s="20"/>
-      <c r="AY43" s="20"/>
-      <c r="AZ43" s="20"/>
-      <c r="BA43" s="20"/>
-      <c r="BB43" s="20"/>
-      <c r="BC43" s="20"/>
-      <c r="BD43" s="20"/>
-      <c r="BE43" s="20"/>
-      <c r="BF43" s="20"/>
-      <c r="BG43" s="20"/>
-      <c r="BH43" s="20"/>
-      <c r="BI43" s="20"/>
-      <c r="BJ43" s="20"/>
-      <c r="BK43" s="20"/>
-      <c r="BL43" s="20"/>
-      <c r="BM43" s="20"/>
-      <c r="BN43" s="20"/>
-      <c r="BO43" s="20"/>
-      <c r="BP43" s="20"/>
-      <c r="BQ43" s="20"/>
+    <row r="42" spans="1:69" ht="21" customHeight="1">
+      <c r="A42" s="20"/>
+      <c r="B42" s="75"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="137"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+      <c r="N42" s="20"/>
+      <c r="O42" s="20"/>
+      <c r="P42" s="20"/>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="20"/>
+      <c r="S42" s="20"/>
+      <c r="T42" s="20"/>
+      <c r="U42" s="20"/>
+      <c r="V42" s="20"/>
+      <c r="W42" s="20"/>
+      <c r="X42" s="20"/>
+      <c r="Y42" s="20"/>
+      <c r="Z42" s="20"/>
+      <c r="AA42" s="20"/>
+      <c r="AB42" s="20"/>
+      <c r="AC42" s="20"/>
+      <c r="AD42" s="20"/>
+      <c r="AE42" s="20"/>
+      <c r="AF42" s="20"/>
+      <c r="AG42" s="20"/>
+      <c r="AH42" s="20"/>
+      <c r="AI42" s="20"/>
+      <c r="AJ42" s="20"/>
+      <c r="AK42" s="20"/>
+      <c r="AL42" s="20"/>
+      <c r="AM42" s="20"/>
+      <c r="AN42" s="20"/>
+      <c r="AO42" s="20"/>
+      <c r="AP42" s="20"/>
+      <c r="AQ42" s="20"/>
+      <c r="AR42" s="20"/>
+      <c r="AS42" s="20"/>
+      <c r="AT42" s="20"/>
+      <c r="AU42" s="20"/>
+      <c r="AV42" s="20"/>
+      <c r="AW42" s="20"/>
+      <c r="AX42" s="20"/>
+      <c r="AY42" s="20"/>
+      <c r="AZ42" s="20"/>
+      <c r="BA42" s="20"/>
+      <c r="BB42" s="20"/>
+      <c r="BC42" s="20"/>
+      <c r="BD42" s="20"/>
+      <c r="BE42" s="20"/>
+      <c r="BF42" s="20"/>
+      <c r="BG42" s="20"/>
+      <c r="BH42" s="20"/>
+      <c r="BI42" s="20"/>
+      <c r="BJ42" s="20"/>
+      <c r="BK42" s="20"/>
+      <c r="BL42" s="20"/>
+      <c r="BM42" s="20"/>
+      <c r="BN42" s="20"/>
+      <c r="BO42" s="20"/>
+      <c r="BP42" s="20"/>
+      <c r="BQ42" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:G5"/>
+    <mergeCell ref="N9:R9"/>
+    <mergeCell ref="S9:W9"/>
+    <mergeCell ref="I9:M9"/>
+    <mergeCell ref="BG9:BK9"/>
+    <mergeCell ref="BB9:BF9"/>
+    <mergeCell ref="X9:AB9"/>
+    <mergeCell ref="AC9:AG9"/>
+    <mergeCell ref="I8:W8"/>
+    <mergeCell ref="X8:AL8"/>
+    <mergeCell ref="AH9:AL9"/>
+    <mergeCell ref="BB8:BP8"/>
+    <mergeCell ref="AM8:BA8"/>
+    <mergeCell ref="AR9:AV9"/>
+    <mergeCell ref="AW9:BA9"/>
+    <mergeCell ref="BL9:BP9"/>
+    <mergeCell ref="AM9:AQ9"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="O2:AE2"/>
@@ -5748,27 +5662,9 @@
     <mergeCell ref="P4:AB4"/>
     <mergeCell ref="P5:AA5"/>
     <mergeCell ref="I5:O5"/>
-    <mergeCell ref="BG9:BK9"/>
-    <mergeCell ref="BB9:BF9"/>
-    <mergeCell ref="X9:AB9"/>
-    <mergeCell ref="AC9:AG9"/>
-    <mergeCell ref="I8:W8"/>
-    <mergeCell ref="X8:AL8"/>
-    <mergeCell ref="AH9:AL9"/>
-    <mergeCell ref="BB8:BP8"/>
-    <mergeCell ref="AM8:BA8"/>
-    <mergeCell ref="AR9:AV9"/>
-    <mergeCell ref="AW9:BA9"/>
-    <mergeCell ref="BL9:BP9"/>
-    <mergeCell ref="AM9:AQ9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:G5"/>
-    <mergeCell ref="N9:R9"/>
-    <mergeCell ref="S9:W9"/>
-    <mergeCell ref="I9:M9"/>
   </mergeCells>
-  <conditionalFormatting sqref="H12:H23 H30:H41 H25:H28">
-    <cfRule type="colorScale" priority="26">
+  <conditionalFormatting sqref="H12:H23 H30:H40 H25:H28">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -5777,8 +5673,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H12:H23 H30:H41 H25:H28">
-    <cfRule type="colorScale" priority="30">
+  <conditionalFormatting sqref="H12:H23 H30:H40 H25:H28">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>